<commit_message>
Test parameter setting with overrides
</commit_message>
<xml_diff>
--- a/Prototypes/ForageBrassica/Observed.xlsx
+++ b/Prototypes/ForageBrassica/Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\APSIMX\Prototypes\ForageBrassica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB01225-4C90-41FD-8ABC-30DF6A1E6C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC8A91C-9B03-4344-8458-F944039E02A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43185" yWindow="4620" windowWidth="21600" windowHeight="12405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="2355" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -955,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y2243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2270,7 +2270,7 @@
     <row r="26" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A26" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvGoliath</v>
+        <v>Tosari2018CvHTR24</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -2282,7 +2282,7 @@
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F26" s="1">
         <v>43202</v>
@@ -2304,7 +2304,7 @@
     <row r="27" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A27" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvGoliath</v>
+        <v>Tosari2018CvHTR24</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -2316,7 +2316,7 @@
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F27" s="1">
         <v>43202</v>
@@ -2338,7 +2338,7 @@
     <row r="28" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A28" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvGoliath</v>
+        <v>Tosari2018CvHTR24</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -2350,7 +2350,7 @@
         <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F28" s="1">
         <v>43202</v>
@@ -2372,7 +2372,7 @@
     <row r="29" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A29" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvGoliath</v>
+        <v>Tosari2018CvHTR24</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
@@ -2384,7 +2384,7 @@
         <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F29" s="1">
         <v>43202</v>
@@ -2406,7 +2406,7 @@
     <row r="30" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A30" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvGoliath</v>
+        <v>Tosari2018CvHTR24</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
@@ -2418,7 +2418,7 @@
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F30" s="1">
         <v>43202</v>
@@ -2440,7 +2440,7 @@
     <row r="31" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A31" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvGoliath</v>
+        <v>Tosari2018CvHTR24</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -2452,7 +2452,7 @@
         <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F31" s="1">
         <v>43202</v>
@@ -2542,7 +2542,7 @@
     <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvWinfred</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
@@ -2554,7 +2554,7 @@
         <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F34" s="1">
         <v>43202</v>
@@ -2576,7 +2576,7 @@
     <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvWinfred</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
@@ -2588,7 +2588,7 @@
         <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F35" s="1">
         <v>43202</v>
@@ -2610,7 +2610,7 @@
     <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvWinfred</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
@@ -2622,7 +2622,7 @@
         <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F36" s="1">
         <v>43202</v>
@@ -2644,7 +2644,7 @@
     <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvWinfred</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
@@ -2656,7 +2656,7 @@
         <v>9</v>
       </c>
       <c r="E37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F37" s="1">
         <v>43202</v>
@@ -2678,7 +2678,7 @@
     <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvWinfred</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
@@ -2690,7 +2690,7 @@
         <v>9</v>
       </c>
       <c r="E38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F38" s="1">
         <v>43202</v>
@@ -2712,7 +2712,7 @@
     <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvWinfred</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
@@ -2724,7 +2724,7 @@
         <v>9</v>
       </c>
       <c r="E39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F39" s="1">
         <v>43202</v>
@@ -2746,7 +2746,7 @@
     <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvWinfred</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
@@ -2758,7 +2758,7 @@
         <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F40" s="1">
         <v>43202</v>
@@ -2780,7 +2780,7 @@
     <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvWinfred</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
@@ -2792,7 +2792,7 @@
         <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F41" s="1">
         <v>43202</v>
@@ -2814,7 +2814,7 @@
     <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvPallaton</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
@@ -2826,7 +2826,7 @@
         <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F42" s="1">
         <v>43202</v>
@@ -2848,7 +2848,7 @@
     <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvPallaton</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
@@ -2860,7 +2860,7 @@
         <v>9</v>
       </c>
       <c r="E43" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F43" s="1">
         <v>43202</v>
@@ -2882,7 +2882,7 @@
     <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvPallaton</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
@@ -2894,7 +2894,7 @@
         <v>9</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F44" s="1">
         <v>43202</v>
@@ -2916,7 +2916,7 @@
     <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvPallaton</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
@@ -2928,7 +2928,7 @@
         <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F45" s="1">
         <v>43202</v>
@@ -2950,7 +2950,7 @@
     <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvWinfred</v>
+        <v>Tosari2018CvPallaton</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
@@ -2962,7 +2962,7 @@
         <v>9</v>
       </c>
       <c r="E46" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F46" s="1">
         <v>43202</v>
@@ -2984,7 +2984,7 @@
     <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvWinfred</v>
+        <v>Tosari2018CvPallaton</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
@@ -2996,7 +2996,7 @@
         <v>9</v>
       </c>
       <c r="E47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F47" s="1">
         <v>43202</v>
@@ -3018,7 +3018,7 @@
     <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvWinfred</v>
+        <v>Tosari2018CvPallaton</v>
       </c>
       <c r="B48" t="s">
         <v>8</v>
@@ -3030,7 +3030,7 @@
         <v>9</v>
       </c>
       <c r="E48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F48" s="1">
         <v>43202</v>
@@ -3052,7 +3052,7 @@
     <row r="49" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A49" t="str">
         <f t="shared" si="2"/>
-        <v>Tosari2018CvWinfred</v>
+        <v>Tosari2018CvPallaton</v>
       </c>
       <c r="B49" t="s">
         <v>8</v>
@@ -3064,7 +3064,7 @@
         <v>9</v>
       </c>
       <c r="E49" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F49" s="1">
         <v>43202</v>
@@ -3286,7 +3286,7 @@
     <row r="55" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A55" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvGoliath</v>
+        <v>Tosari2018CvHTR24</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
@@ -3298,7 +3298,7 @@
         <v>9</v>
       </c>
       <c r="E55" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F55" s="1">
         <v>43202</v>
@@ -3326,7 +3326,7 @@
     <row r="56" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A56" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvGoliath</v>
+        <v>Tosari2018CvHTR24</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
@@ -3338,7 +3338,7 @@
         <v>9</v>
       </c>
       <c r="E56" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F56" s="1">
         <v>43202</v>
@@ -3366,7 +3366,7 @@
     <row r="57" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A57" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvGoliath</v>
+        <v>Tosari2018CvHTR24</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
@@ -3378,7 +3378,7 @@
         <v>9</v>
       </c>
       <c r="E57" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F57" s="1">
         <v>43202</v>
@@ -3406,7 +3406,7 @@
     <row r="58" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A58" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvGoliath</v>
+        <v>Tosari2018CvHTR24</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
@@ -3418,7 +3418,7 @@
         <v>9</v>
       </c>
       <c r="E58" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F58" s="1">
         <v>43202</v>
@@ -3446,7 +3446,7 @@
     <row r="59" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A59" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvGoliath</v>
+        <v>Tosari2018CvHTR24</v>
       </c>
       <c r="B59" t="s">
         <v>8</v>
@@ -3458,7 +3458,7 @@
         <v>9</v>
       </c>
       <c r="E59" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F59" s="1">
         <v>43202</v>
@@ -3486,7 +3486,7 @@
     <row r="60" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A60" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvGoliath</v>
+        <v>Tosari2018CvWinfred</v>
       </c>
       <c r="B60" t="s">
         <v>8</v>
@@ -3498,7 +3498,7 @@
         <v>9</v>
       </c>
       <c r="E60" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F60" s="1">
         <v>43202</v>
@@ -3526,7 +3526,7 @@
     <row r="61" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A61" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvWinfred</v>
       </c>
       <c r="B61" t="s">
         <v>8</v>
@@ -3538,7 +3538,7 @@
         <v>9</v>
       </c>
       <c r="E61" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F61" s="1">
         <v>43202</v>
@@ -3566,7 +3566,7 @@
     <row r="62" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A62" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvWinfred</v>
       </c>
       <c r="B62" t="s">
         <v>8</v>
@@ -3578,7 +3578,7 @@
         <v>9</v>
       </c>
       <c r="E62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F62" s="1">
         <v>43202</v>
@@ -3606,7 +3606,7 @@
     <row r="63" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A63" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvWinfred</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
@@ -3618,7 +3618,7 @@
         <v>9</v>
       </c>
       <c r="E63" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F63" s="1">
         <v>43202</v>
@@ -3646,7 +3646,7 @@
     <row r="64" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A64" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvWinfred</v>
       </c>
       <c r="B64" t="s">
         <v>8</v>
@@ -3658,7 +3658,7 @@
         <v>9</v>
       </c>
       <c r="E64" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F64" s="1">
         <v>43202</v>
@@ -3686,7 +3686,7 @@
     <row r="65" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A65" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvPallaton</v>
       </c>
       <c r="B65" t="s">
         <v>8</v>
@@ -3698,7 +3698,7 @@
         <v>9</v>
       </c>
       <c r="E65" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F65" s="1">
         <v>43202</v>
@@ -3726,7 +3726,7 @@
     <row r="66" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A66" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvPallaton</v>
       </c>
       <c r="B66" t="s">
         <v>8</v>
@@ -3738,7 +3738,7 @@
         <v>9</v>
       </c>
       <c r="E66" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F66" s="1">
         <v>43202</v>
@@ -3766,7 +3766,7 @@
     <row r="67" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A67" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvPallaton</v>
       </c>
       <c r="B67" t="s">
         <v>8</v>
@@ -3778,7 +3778,7 @@
         <v>9</v>
       </c>
       <c r="E67" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F67" s="1">
         <v>43202</v>
@@ -3806,7 +3806,7 @@
     <row r="68" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A68" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvPallaton</v>
       </c>
       <c r="B68" t="s">
         <v>8</v>
@@ -3818,7 +3818,7 @@
         <v>9</v>
       </c>
       <c r="E68" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F68" s="1">
         <v>43202</v>
@@ -3846,7 +3846,7 @@
     <row r="69" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A69" t="str">
         <f t="shared" si="4"/>
-        <v>Tosari2018CvHTR24</v>
+        <v>Tosari2018CvPallaton</v>
       </c>
       <c r="B69" t="s">
         <v>8</v>
@@ -3858,7 +3858,7 @@
         <v>9</v>
       </c>
       <c r="E69" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F69" s="1">
         <v>43202</v>

</xml_diff>

<commit_message>
fixes to predicted vs observed
</commit_message>
<xml_diff>
--- a/Prototypes/ForageBrassica/Observed.xlsx
+++ b/Prototypes/ForageBrassica/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\APSIMX\Prototypes\ForageBrassica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC8A91C-9B03-4344-8458-F944039E02A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762D1426-D3A4-4E4B-AD9A-1A80424811D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40920" yWindow="2355" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -955,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y2243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65:E69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1085,11 +1085,11 @@
         <v>10</v>
       </c>
       <c r="F2" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G2" s="1">
         <f>F2+H2</f>
-        <v>43271</v>
+        <v>43333</v>
       </c>
       <c r="H2">
         <v>69</v>
@@ -1143,11 +1143,11 @@
         <v>10</v>
       </c>
       <c r="F3" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G17" si="1">F3+H3</f>
-        <v>43300</v>
+        <v>43362</v>
       </c>
       <c r="H3">
         <v>98</v>
@@ -1201,11 +1201,11 @@
         <v>10</v>
       </c>
       <c r="F4" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="1"/>
-        <v>43328</v>
+        <v>43390</v>
       </c>
       <c r="H4">
         <v>126</v>
@@ -1259,11 +1259,11 @@
         <v>10</v>
       </c>
       <c r="F5" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="1"/>
-        <v>43347</v>
+        <v>43409</v>
       </c>
       <c r="H5">
         <v>145</v>
@@ -1317,11 +1317,11 @@
         <v>11</v>
       </c>
       <c r="F6" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
-        <v>43271</v>
+        <v>43333</v>
       </c>
       <c r="H6">
         <v>69</v>
@@ -1375,11 +1375,11 @@
         <v>11</v>
       </c>
       <c r="F7" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="1"/>
-        <v>43300</v>
+        <v>43362</v>
       </c>
       <c r="H7">
         <v>98</v>
@@ -1433,11 +1433,11 @@
         <v>11</v>
       </c>
       <c r="F8" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="1"/>
-        <v>43320</v>
+        <v>43382</v>
       </c>
       <c r="H8">
         <v>118</v>
@@ -1491,11 +1491,11 @@
         <v>11</v>
       </c>
       <c r="F9" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="1"/>
-        <v>43347</v>
+        <v>43409</v>
       </c>
       <c r="H9">
         <v>145</v>
@@ -1549,11 +1549,11 @@
         <v>12</v>
       </c>
       <c r="F10" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="1"/>
-        <v>43271</v>
+        <v>43333</v>
       </c>
       <c r="H10">
         <v>69</v>
@@ -1607,11 +1607,11 @@
         <v>12</v>
       </c>
       <c r="F11" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="1"/>
-        <v>43300</v>
+        <v>43362</v>
       </c>
       <c r="H11">
         <v>98</v>
@@ -1665,11 +1665,11 @@
         <v>12</v>
       </c>
       <c r="F12" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>43328</v>
+        <v>43390</v>
       </c>
       <c r="H12">
         <v>126</v>
@@ -1723,11 +1723,11 @@
         <v>12</v>
       </c>
       <c r="F13" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="1"/>
-        <v>43347</v>
+        <v>43409</v>
       </c>
       <c r="H13">
         <v>145</v>
@@ -1781,11 +1781,11 @@
         <v>13</v>
       </c>
       <c r="F14" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="1"/>
-        <v>43271</v>
+        <v>43333</v>
       </c>
       <c r="H14">
         <v>69</v>
@@ -1839,11 +1839,11 @@
         <v>13</v>
       </c>
       <c r="F15" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="1"/>
-        <v>43300</v>
+        <v>43362</v>
       </c>
       <c r="H15">
         <v>98</v>
@@ -1897,11 +1897,11 @@
         <v>13</v>
       </c>
       <c r="F16" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="1"/>
-        <v>43328</v>
+        <v>43390</v>
       </c>
       <c r="H16">
         <v>126</v>
@@ -1955,11 +1955,11 @@
         <v>13</v>
       </c>
       <c r="F17" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="1"/>
-        <v>43347</v>
+        <v>43409</v>
       </c>
       <c r="H17">
         <v>145</v>
@@ -2013,11 +2013,11 @@
         <v>10</v>
       </c>
       <c r="F18" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" ref="G18:G49" si="3">F18+H18</f>
-        <v>43231</v>
+        <v>43293</v>
       </c>
       <c r="H18">
         <v>29</v>
@@ -2047,11 +2047,11 @@
         <v>10</v>
       </c>
       <c r="F19" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="3"/>
-        <v>43237</v>
+        <v>43299</v>
       </c>
       <c r="H19">
         <v>35</v>
@@ -2081,11 +2081,11 @@
         <v>10</v>
       </c>
       <c r="F20" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="3"/>
-        <v>43243</v>
+        <v>43305</v>
       </c>
       <c r="H20">
         <v>41</v>
@@ -2115,11 +2115,11 @@
         <v>10</v>
       </c>
       <c r="F21" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="3"/>
-        <v>43250</v>
+        <v>43312</v>
       </c>
       <c r="H21">
         <v>48</v>
@@ -2149,11 +2149,11 @@
         <v>10</v>
       </c>
       <c r="F22" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="3"/>
-        <v>43257</v>
+        <v>43319</v>
       </c>
       <c r="H22">
         <v>55</v>
@@ -2183,11 +2183,11 @@
         <v>10</v>
       </c>
       <c r="F23" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="3"/>
-        <v>43271</v>
+        <v>43333</v>
       </c>
       <c r="H23">
         <v>69</v>
@@ -2217,11 +2217,11 @@
         <v>10</v>
       </c>
       <c r="F24" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="3"/>
-        <v>43279</v>
+        <v>43341</v>
       </c>
       <c r="H24">
         <v>77</v>
@@ -2251,11 +2251,11 @@
         <v>10</v>
       </c>
       <c r="F25" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="3"/>
-        <v>43305</v>
+        <v>43367</v>
       </c>
       <c r="H25">
         <v>103</v>
@@ -2285,11 +2285,11 @@
         <v>11</v>
       </c>
       <c r="F26" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" si="3"/>
-        <v>43231</v>
+        <v>43293</v>
       </c>
       <c r="H26">
         <v>29</v>
@@ -2319,11 +2319,11 @@
         <v>11</v>
       </c>
       <c r="F27" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="3"/>
-        <v>43237</v>
+        <v>43299</v>
       </c>
       <c r="H27">
         <v>35</v>
@@ -2353,11 +2353,11 @@
         <v>11</v>
       </c>
       <c r="F28" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G28" s="1">
         <f t="shared" si="3"/>
-        <v>43243</v>
+        <v>43305</v>
       </c>
       <c r="H28">
         <v>41</v>
@@ -2387,11 +2387,11 @@
         <v>11</v>
       </c>
       <c r="F29" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G29" s="1">
         <f t="shared" si="3"/>
-        <v>43250</v>
+        <v>43312</v>
       </c>
       <c r="H29">
         <v>48</v>
@@ -2421,11 +2421,11 @@
         <v>11</v>
       </c>
       <c r="F30" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="3"/>
-        <v>43257</v>
+        <v>43319</v>
       </c>
       <c r="H30">
         <v>55</v>
@@ -2455,11 +2455,11 @@
         <v>11</v>
       </c>
       <c r="F31" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" si="3"/>
-        <v>43271</v>
+        <v>43333</v>
       </c>
       <c r="H31">
         <v>69</v>
@@ -2489,11 +2489,11 @@
         <v>11</v>
       </c>
       <c r="F32" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G32" s="1">
         <f t="shared" si="3"/>
-        <v>43279</v>
+        <v>43341</v>
       </c>
       <c r="H32">
         <v>77</v>
@@ -2523,11 +2523,11 @@
         <v>11</v>
       </c>
       <c r="F33" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G33" s="1">
         <f t="shared" si="3"/>
-        <v>43305</v>
+        <v>43367</v>
       </c>
       <c r="H33">
         <v>103</v>
@@ -2557,11 +2557,11 @@
         <v>12</v>
       </c>
       <c r="F34" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" si="3"/>
-        <v>43231</v>
+        <v>43293</v>
       </c>
       <c r="H34">
         <v>29</v>
@@ -2591,11 +2591,11 @@
         <v>12</v>
       </c>
       <c r="F35" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G35" s="1">
         <f t="shared" si="3"/>
-        <v>43237</v>
+        <v>43299</v>
       </c>
       <c r="H35">
         <v>35</v>
@@ -2625,11 +2625,11 @@
         <v>12</v>
       </c>
       <c r="F36" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G36" s="1">
         <f t="shared" si="3"/>
-        <v>43243</v>
+        <v>43305</v>
       </c>
       <c r="H36">
         <v>41</v>
@@ -2659,11 +2659,11 @@
         <v>12</v>
       </c>
       <c r="F37" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G37" s="1">
         <f t="shared" si="3"/>
-        <v>43250</v>
+        <v>43312</v>
       </c>
       <c r="H37">
         <v>48</v>
@@ -2693,11 +2693,11 @@
         <v>12</v>
       </c>
       <c r="F38" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G38" s="1">
         <f t="shared" si="3"/>
-        <v>43257</v>
+        <v>43319</v>
       </c>
       <c r="H38">
         <v>55</v>
@@ -2727,11 +2727,11 @@
         <v>12</v>
       </c>
       <c r="F39" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G39" s="1">
         <f t="shared" si="3"/>
-        <v>43271</v>
+        <v>43333</v>
       </c>
       <c r="H39">
         <v>69</v>
@@ -2761,11 +2761,11 @@
         <v>12</v>
       </c>
       <c r="F40" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G40" s="1">
         <f t="shared" si="3"/>
-        <v>43279</v>
+        <v>43341</v>
       </c>
       <c r="H40">
         <v>77</v>
@@ -2795,11 +2795,11 @@
         <v>12</v>
       </c>
       <c r="F41" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G41" s="1">
         <f t="shared" si="3"/>
-        <v>43305</v>
+        <v>43367</v>
       </c>
       <c r="H41">
         <v>103</v>
@@ -2829,11 +2829,11 @@
         <v>13</v>
       </c>
       <c r="F42" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G42" s="1">
         <f t="shared" si="3"/>
-        <v>43231</v>
+        <v>43293</v>
       </c>
       <c r="H42">
         <v>29</v>
@@ -2863,11 +2863,11 @@
         <v>13</v>
       </c>
       <c r="F43" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G43" s="1">
         <f t="shared" si="3"/>
-        <v>43237</v>
+        <v>43299</v>
       </c>
       <c r="H43">
         <v>35</v>
@@ -2897,11 +2897,11 @@
         <v>13</v>
       </c>
       <c r="F44" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G44" s="1">
         <f t="shared" si="3"/>
-        <v>43243</v>
+        <v>43305</v>
       </c>
       <c r="H44">
         <v>41</v>
@@ -2931,11 +2931,11 @@
         <v>13</v>
       </c>
       <c r="F45" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G45" s="1">
         <f t="shared" si="3"/>
-        <v>43250</v>
+        <v>43312</v>
       </c>
       <c r="H45">
         <v>48</v>
@@ -2965,11 +2965,11 @@
         <v>13</v>
       </c>
       <c r="F46" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G46" s="1">
         <f t="shared" si="3"/>
-        <v>43257</v>
+        <v>43319</v>
       </c>
       <c r="H46">
         <v>55</v>
@@ -2999,11 +2999,11 @@
         <v>13</v>
       </c>
       <c r="F47" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G47" s="1">
         <f t="shared" si="3"/>
-        <v>43271</v>
+        <v>43333</v>
       </c>
       <c r="H47">
         <v>69</v>
@@ -3033,11 +3033,11 @@
         <v>13</v>
       </c>
       <c r="F48" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G48" s="1">
         <f t="shared" si="3"/>
-        <v>43279</v>
+        <v>43341</v>
       </c>
       <c r="H48">
         <v>77</v>
@@ -3067,11 +3067,11 @@
         <v>13</v>
       </c>
       <c r="F49" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G49" s="1">
         <f t="shared" si="3"/>
-        <v>43305</v>
+        <v>43367</v>
       </c>
       <c r="H49">
         <v>103</v>
@@ -3101,11 +3101,11 @@
         <v>10</v>
       </c>
       <c r="F50" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G50" s="1">
         <f t="shared" ref="G50:G69" si="5">F50+H50</f>
-        <v>43271</v>
+        <v>43333</v>
       </c>
       <c r="H50">
         <v>69</v>
@@ -3141,11 +3141,11 @@
         <v>10</v>
       </c>
       <c r="F51" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G51" s="1">
         <f t="shared" si="5"/>
-        <v>43279</v>
+        <v>43341</v>
       </c>
       <c r="H51">
         <v>77</v>
@@ -3181,11 +3181,11 @@
         <v>10</v>
       </c>
       <c r="F52" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G52" s="1">
         <f t="shared" si="5"/>
-        <v>43300</v>
+        <v>43362</v>
       </c>
       <c r="H52">
         <v>98</v>
@@ -3221,11 +3221,11 @@
         <v>10</v>
       </c>
       <c r="F53" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G53" s="1">
         <f t="shared" si="5"/>
-        <v>43328</v>
+        <v>43390</v>
       </c>
       <c r="H53">
         <v>126</v>
@@ -3261,11 +3261,11 @@
         <v>10</v>
       </c>
       <c r="F54" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G54" s="1">
         <f t="shared" si="5"/>
-        <v>43347</v>
+        <v>43409</v>
       </c>
       <c r="H54">
         <v>145</v>
@@ -3301,11 +3301,11 @@
         <v>11</v>
       </c>
       <c r="F55" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G55" s="1">
         <f t="shared" si="5"/>
-        <v>43271</v>
+        <v>43333</v>
       </c>
       <c r="H55">
         <v>69</v>
@@ -3341,11 +3341,11 @@
         <v>11</v>
       </c>
       <c r="F56" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G56" s="1">
         <f t="shared" si="5"/>
-        <v>43279</v>
+        <v>43341</v>
       </c>
       <c r="H56">
         <v>77</v>
@@ -3381,11 +3381,11 @@
         <v>11</v>
       </c>
       <c r="F57" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G57" s="1">
         <f t="shared" si="5"/>
-        <v>43300</v>
+        <v>43362</v>
       </c>
       <c r="H57">
         <v>98</v>
@@ -3421,11 +3421,11 @@
         <v>11</v>
       </c>
       <c r="F58" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G58" s="1">
         <f t="shared" si="5"/>
-        <v>43328</v>
+        <v>43390</v>
       </c>
       <c r="H58">
         <v>126</v>
@@ -3461,11 +3461,11 @@
         <v>11</v>
       </c>
       <c r="F59" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G59" s="1">
         <f t="shared" si="5"/>
-        <v>43347</v>
+        <v>43409</v>
       </c>
       <c r="H59">
         <v>145</v>
@@ -3501,11 +3501,11 @@
         <v>12</v>
       </c>
       <c r="F60" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G60" s="1">
         <f t="shared" si="5"/>
-        <v>43271</v>
+        <v>43333</v>
       </c>
       <c r="H60">
         <v>69</v>
@@ -3541,11 +3541,11 @@
         <v>12</v>
       </c>
       <c r="F61" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G61" s="1">
         <f t="shared" si="5"/>
-        <v>43279</v>
+        <v>43341</v>
       </c>
       <c r="H61">
         <v>77</v>
@@ -3581,11 +3581,11 @@
         <v>12</v>
       </c>
       <c r="F62" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G62" s="1">
         <f t="shared" si="5"/>
-        <v>43300</v>
+        <v>43362</v>
       </c>
       <c r="H62">
         <v>98</v>
@@ -3621,11 +3621,11 @@
         <v>12</v>
       </c>
       <c r="F63" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G63" s="1">
         <f t="shared" si="5"/>
-        <v>43328</v>
+        <v>43390</v>
       </c>
       <c r="H63">
         <v>126</v>
@@ -3661,11 +3661,11 @@
         <v>12</v>
       </c>
       <c r="F64" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G64" s="1">
         <f t="shared" si="5"/>
-        <v>43347</v>
+        <v>43409</v>
       </c>
       <c r="H64">
         <v>145</v>
@@ -3701,11 +3701,11 @@
         <v>13</v>
       </c>
       <c r="F65" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G65" s="1">
         <f t="shared" si="5"/>
-        <v>43271</v>
+        <v>43333</v>
       </c>
       <c r="H65">
         <v>69</v>
@@ -3741,11 +3741,11 @@
         <v>13</v>
       </c>
       <c r="F66" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G66" s="1">
         <f t="shared" si="5"/>
-        <v>43279</v>
+        <v>43341</v>
       </c>
       <c r="H66">
         <v>77</v>
@@ -3781,11 +3781,11 @@
         <v>13</v>
       </c>
       <c r="F67" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G67" s="1">
         <f t="shared" si="5"/>
-        <v>43300</v>
+        <v>43362</v>
       </c>
       <c r="H67">
         <v>98</v>
@@ -3821,11 +3821,11 @@
         <v>13</v>
       </c>
       <c r="F68" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G68" s="1">
         <f t="shared" si="5"/>
-        <v>43328</v>
+        <v>43390</v>
       </c>
       <c r="H68">
         <v>126</v>
@@ -3861,11 +3861,11 @@
         <v>13</v>
       </c>
       <c r="F69" s="1">
-        <v>43202</v>
+        <v>43264</v>
       </c>
       <c r="G69" s="1">
         <f t="shared" si="5"/>
-        <v>43347</v>
+        <v>43409</v>
       </c>
       <c r="H69">
         <v>145</v>

</xml_diff>

<commit_message>
added hastings obs data
</commit_message>
<xml_diff>
--- a/Prototypes/ForageBrassica/Observed.xlsx
+++ b/Prototypes/ForageBrassica/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\APSIMX\Prototypes\ForageBrassica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05924DEF-FDC5-4E2E-839D-6FA9660403A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E2E150-5B91-4985-9720-4758F989F2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40920" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="35">
   <si>
     <t>SimulationName</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Treat</t>
+  </si>
+  <si>
+    <t>Hastings</t>
   </si>
 </sst>
 </file>
@@ -6605,10 +6608,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z2239"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="870" topLeftCell="A133" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="585" topLeftCell="A132" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="D163" sqref="D163"/>
+      <selection pane="bottomLeft" activeCell="K185" sqref="K185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12460,7 +12463,7 @@
     </row>
     <row r="140" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A140" t="str">
-        <f t="shared" ref="A140:A156" si="12">B140&amp;C140&amp;"Cv"&amp;E140&amp;"N"&amp;F140</f>
+        <f t="shared" ref="A140:A157" si="12">B140&amp;C140&amp;"Cv"&amp;E140&amp;"N"&amp;F140</f>
         <v>Lincoln2009CvTitanN1</v>
       </c>
       <c r="B140" t="s">
@@ -13129,125 +13132,1144 @@
         <v>326.62022175062702</v>
       </c>
     </row>
-    <row r="165" spans="9:9" x14ac:dyDescent="0.45">
-      <c r="I165" s="1"/>
-    </row>
-    <row r="166" spans="9:9" x14ac:dyDescent="0.45">
-      <c r="I166" s="1"/>
-    </row>
-    <row r="167" spans="9:9" x14ac:dyDescent="0.45">
-      <c r="I167" s="1"/>
-    </row>
-    <row r="168" spans="9:9" x14ac:dyDescent="0.45">
-      <c r="I168" s="1"/>
-    </row>
-    <row r="169" spans="9:9" x14ac:dyDescent="0.45">
-      <c r="I169" s="1"/>
-    </row>
-    <row r="170" spans="9:9" x14ac:dyDescent="0.45">
-      <c r="I170" s="1"/>
-    </row>
-    <row r="183" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G183" s="1"/>
-      <c r="H183" s="1"/>
-    </row>
-    <row r="184" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G184" s="1"/>
-      <c r="H184" s="1"/>
-    </row>
-    <row r="185" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A157" t="str">
+        <f t="shared" si="12"/>
+        <v>Hastings2011CvTitanN0</v>
+      </c>
+      <c r="B157" t="s">
+        <v>34</v>
+      </c>
+      <c r="C157">
+        <v>2011</v>
+      </c>
+      <c r="D157" t="s">
+        <v>9</v>
+      </c>
+      <c r="E157" t="s">
+        <v>32</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+      <c r="H157" s="1">
+        <v>40940</v>
+      </c>
+      <c r="I157">
+        <v>91</v>
+      </c>
+      <c r="M157">
+        <v>8.1645905694107608</v>
+      </c>
+      <c r="O157">
+        <v>0.998676919785911</v>
+      </c>
+      <c r="Q157">
+        <v>9762.9904923440899</v>
+      </c>
+      <c r="W157">
+        <v>542.35263824976505</v>
+      </c>
+      <c r="Y157">
+        <v>433.94641098464399</v>
+      </c>
+    </row>
+    <row r="158" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A158" t="str">
+        <f t="shared" ref="A158:A161" si="13">B158&amp;C158&amp;"Cv"&amp;E158&amp;"N"&amp;F158</f>
+        <v>Hastings2011CvTitanN0</v>
+      </c>
+      <c r="B158" t="s">
+        <v>34</v>
+      </c>
+      <c r="C158">
+        <v>2011</v>
+      </c>
+      <c r="D158" t="s">
+        <v>9</v>
+      </c>
+      <c r="E158" t="s">
+        <v>32</v>
+      </c>
+      <c r="F158">
+        <v>0</v>
+      </c>
+      <c r="H158" s="1">
+        <v>40912</v>
+      </c>
+      <c r="I158">
+        <v>63</v>
+      </c>
+      <c r="M158">
+        <v>7.0655156887573503</v>
+      </c>
+      <c r="O158">
+        <v>0.99640813147117302</v>
+      </c>
+      <c r="Q158">
+        <v>7951.5884628649201</v>
+      </c>
+      <c r="W158">
+        <v>594.62333005370999</v>
+      </c>
+      <c r="Y158">
+        <v>200.53551623278199</v>
+      </c>
+    </row>
+    <row r="159" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A159" t="str">
+        <f t="shared" si="13"/>
+        <v>Hastings2011CvTitanN0</v>
+      </c>
+      <c r="B159" t="s">
+        <v>34</v>
+      </c>
+      <c r="C159">
+        <v>2011</v>
+      </c>
+      <c r="D159" t="s">
+        <v>9</v>
+      </c>
+      <c r="E159" t="s">
+        <v>32</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+      <c r="H159" s="1">
+        <v>40890</v>
+      </c>
+      <c r="I159">
+        <v>41</v>
+      </c>
+      <c r="M159">
+        <v>3.7301918073282101</v>
+      </c>
+      <c r="O159">
+        <v>0.948382583815777</v>
+      </c>
+      <c r="Q159">
+        <v>3312.9813225682301</v>
+      </c>
+      <c r="W159">
+        <v>301.11871435414099</v>
+      </c>
+      <c r="Y159">
+        <v>30.179417902682601</v>
+      </c>
+    </row>
+    <row r="160" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A160" t="str">
+        <f t="shared" si="13"/>
+        <v>Hastings2011CvTitanN0</v>
+      </c>
+      <c r="B160" t="s">
+        <v>34</v>
+      </c>
+      <c r="C160">
+        <v>2011</v>
+      </c>
+      <c r="D160" t="s">
+        <v>9</v>
+      </c>
+      <c r="E160" t="s">
+        <v>32</v>
+      </c>
+      <c r="F160">
+        <v>0</v>
+      </c>
+      <c r="H160" s="1">
+        <v>40926</v>
+      </c>
+      <c r="I160">
+        <v>77</v>
+      </c>
+      <c r="M160">
+        <v>4.5986571790632702</v>
+      </c>
+      <c r="O160">
+        <v>0.97632837783242599</v>
+      </c>
+      <c r="Q160">
+        <v>9448.6475449364298</v>
+      </c>
+      <c r="W160">
+        <v>547.13557461379798</v>
+      </c>
+      <c r="Y160">
+        <v>397.72917987984601</v>
+      </c>
+    </row>
+    <row r="161" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A161" t="str">
+        <f t="shared" si="13"/>
+        <v>Hastings2011CvTitanN0</v>
+      </c>
+      <c r="B161" t="s">
+        <v>34</v>
+      </c>
+      <c r="C161">
+        <v>2011</v>
+      </c>
+      <c r="D161" t="s">
+        <v>9</v>
+      </c>
+      <c r="E161" t="s">
+        <v>32</v>
+      </c>
+      <c r="F161">
+        <v>0</v>
+      </c>
+      <c r="H161" s="1">
+        <v>40898</v>
+      </c>
+      <c r="I161">
+        <v>49</v>
+      </c>
+      <c r="M161">
+        <v>5.5882933584288796</v>
+      </c>
+      <c r="O161">
+        <v>0.98948355895990103</v>
+      </c>
+      <c r="Q161">
+        <v>4926.49292863344</v>
+      </c>
+      <c r="W161">
+        <v>414.942746637629</v>
+      </c>
+      <c r="Y161">
+        <v>77.706546225714803</v>
+      </c>
+    </row>
+    <row r="162" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A162" t="str">
+        <f t="shared" ref="A162" si="14">B162&amp;C162&amp;"Cv"&amp;E162&amp;"N"&amp;F162</f>
+        <v>Hastings2011CvTitanN25</v>
+      </c>
+      <c r="B162" t="s">
+        <v>34</v>
+      </c>
+      <c r="C162">
+        <v>2011</v>
+      </c>
+      <c r="D162" t="s">
+        <v>9</v>
+      </c>
+      <c r="E162" t="s">
+        <v>32</v>
+      </c>
+      <c r="F162">
+        <v>25</v>
+      </c>
+      <c r="H162" s="1">
+        <v>40940</v>
+      </c>
+      <c r="I162">
+        <v>91</v>
+      </c>
+      <c r="M162">
+        <v>10.7786098294357</v>
+      </c>
+      <c r="O162">
+        <v>0.99964587216560097</v>
+      </c>
+      <c r="Q162">
+        <v>10973.6367949293</v>
+      </c>
+      <c r="W162">
+        <v>667.24898664496197</v>
+      </c>
+      <c r="Y162">
+        <v>430.11469284797198</v>
+      </c>
+    </row>
+    <row r="163" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A163" t="str">
+        <f t="shared" ref="A163:A166" si="15">B163&amp;C163&amp;"Cv"&amp;E163&amp;"N"&amp;F163</f>
+        <v>Hastings2011CvTitanN25</v>
+      </c>
+      <c r="B163" t="s">
+        <v>34</v>
+      </c>
+      <c r="C163">
+        <v>2011</v>
+      </c>
+      <c r="D163" t="s">
+        <v>9</v>
+      </c>
+      <c r="E163" t="s">
+        <v>32</v>
+      </c>
+      <c r="F163">
+        <v>25</v>
+      </c>
+      <c r="H163" s="1">
+        <v>40912</v>
+      </c>
+      <c r="I163">
+        <v>63</v>
+      </c>
+      <c r="M163">
+        <v>7.6040515264749597</v>
+      </c>
+      <c r="O163">
+        <v>0.99593683096649499</v>
+      </c>
+      <c r="Q163">
+        <v>8741.2869633606297</v>
+      </c>
+      <c r="W163">
+        <v>686.30898240402098</v>
+      </c>
+      <c r="Y163">
+        <v>187.81971393204199</v>
+      </c>
+    </row>
+    <row r="164" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A164" t="str">
+        <f t="shared" si="15"/>
+        <v>Hastings2011CvTitanN25</v>
+      </c>
+      <c r="B164" t="s">
+        <v>34</v>
+      </c>
+      <c r="C164">
+        <v>2011</v>
+      </c>
+      <c r="D164" t="s">
+        <v>9</v>
+      </c>
+      <c r="E164" t="s">
+        <v>32</v>
+      </c>
+      <c r="F164">
+        <v>25</v>
+      </c>
+      <c r="H164" s="1">
+        <v>40890</v>
+      </c>
+      <c r="I164">
+        <v>41</v>
+      </c>
+      <c r="M164">
+        <v>3.87838285025913</v>
+      </c>
+      <c r="O164">
+        <v>0.93942268559731501</v>
+      </c>
+      <c r="Q164">
+        <v>3602.0018772098001</v>
+      </c>
+      <c r="W164">
+        <v>327.20131091511701</v>
+      </c>
+      <c r="Y164">
+        <v>32.998876805862501</v>
+      </c>
+    </row>
+    <row r="165" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A165" t="str">
+        <f t="shared" si="15"/>
+        <v>Hastings2011CvTitanN25</v>
+      </c>
+      <c r="B165" t="s">
+        <v>34</v>
+      </c>
+      <c r="C165">
+        <v>2011</v>
+      </c>
+      <c r="D165" t="s">
+        <v>9</v>
+      </c>
+      <c r="E165" t="s">
+        <v>32</v>
+      </c>
+      <c r="F165">
+        <v>25</v>
+      </c>
+      <c r="H165" s="1">
+        <v>40926</v>
+      </c>
+      <c r="I165">
+        <v>77</v>
+      </c>
+      <c r="M165">
+        <v>6.3985198614214003</v>
+      </c>
+      <c r="O165">
+        <v>0.99246142865783105</v>
+      </c>
+      <c r="Q165">
+        <v>10293.856954487301</v>
+      </c>
+      <c r="W165">
+        <v>670.91238619369301</v>
+      </c>
+      <c r="Y165">
+        <v>358.47330925504201</v>
+      </c>
+    </row>
+    <row r="166" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A166" t="str">
+        <f t="shared" si="15"/>
+        <v>Hastings2011CvTitanN25</v>
+      </c>
+      <c r="B166" t="s">
+        <v>34</v>
+      </c>
+      <c r="C166">
+        <v>2011</v>
+      </c>
+      <c r="D166" t="s">
+        <v>9</v>
+      </c>
+      <c r="E166" t="s">
+        <v>32</v>
+      </c>
+      <c r="F166">
+        <v>25</v>
+      </c>
+      <c r="H166" s="1">
+        <v>40898</v>
+      </c>
+      <c r="I166">
+        <v>49</v>
+      </c>
+      <c r="M166">
+        <v>5.0841657364863204</v>
+      </c>
+      <c r="O166">
+        <v>0.98235493341950297</v>
+      </c>
+      <c r="Q166">
+        <v>4479.3273904906</v>
+      </c>
+      <c r="W166">
+        <v>376.24548377927999</v>
+      </c>
+      <c r="Y166">
+        <v>71.687255269780707</v>
+      </c>
+    </row>
+    <row r="167" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A167" t="str">
+        <f t="shared" ref="A167" si="16">B167&amp;C167&amp;"Cv"&amp;E167&amp;"N"&amp;F167</f>
+        <v>Hastings2011CvTitanN50</v>
+      </c>
+      <c r="B167" t="s">
+        <v>34</v>
+      </c>
+      <c r="C167">
+        <v>2011</v>
+      </c>
+      <c r="D167" t="s">
+        <v>9</v>
+      </c>
+      <c r="E167" t="s">
+        <v>32</v>
+      </c>
+      <c r="F167">
+        <v>50</v>
+      </c>
+      <c r="H167" s="1">
+        <v>40940</v>
+      </c>
+      <c r="I167">
+        <v>91</v>
+      </c>
+      <c r="M167">
+        <v>10.2328039729657</v>
+      </c>
+      <c r="O167">
+        <v>0.99964421924505398</v>
+      </c>
+      <c r="Q167">
+        <v>10135.9557791151</v>
+      </c>
+      <c r="W167">
+        <v>618.22768753192804</v>
+      </c>
+      <c r="Y167">
+        <v>395.36789037958602</v>
+      </c>
+    </row>
+    <row r="168" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A168" t="str">
+        <f t="shared" ref="A168:A171" si="17">B168&amp;C168&amp;"Cv"&amp;E168&amp;"N"&amp;F168</f>
+        <v>Hastings2011CvTitanN50</v>
+      </c>
+      <c r="B168" t="s">
+        <v>34</v>
+      </c>
+      <c r="C168">
+        <v>2011</v>
+      </c>
+      <c r="D168" t="s">
+        <v>9</v>
+      </c>
+      <c r="E168" t="s">
+        <v>32</v>
+      </c>
+      <c r="F168">
+        <v>50</v>
+      </c>
+      <c r="H168" s="1">
+        <v>40912</v>
+      </c>
+      <c r="I168">
+        <v>63</v>
+      </c>
+      <c r="M168">
+        <v>7.44165157531648</v>
+      </c>
+      <c r="O168">
+        <v>0.99746104046542305</v>
+      </c>
+      <c r="Q168">
+        <v>7834.5644140710801</v>
+      </c>
+      <c r="W168">
+        <v>603.97863155138498</v>
+      </c>
+      <c r="Y168">
+        <v>179.477809855723</v>
+      </c>
+    </row>
+    <row r="169" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A169" t="str">
+        <f t="shared" si="17"/>
+        <v>Hastings2011CvTitanN50</v>
+      </c>
+      <c r="B169" t="s">
+        <v>34</v>
+      </c>
+      <c r="C169">
+        <v>2011</v>
+      </c>
+      <c r="D169" t="s">
+        <v>9</v>
+      </c>
+      <c r="E169" t="s">
+        <v>32</v>
+      </c>
+      <c r="F169">
+        <v>50</v>
+      </c>
+      <c r="H169" s="1">
+        <v>40890</v>
+      </c>
+      <c r="I169">
+        <v>41</v>
+      </c>
+      <c r="M169">
+        <v>4.2889581482423198</v>
+      </c>
+      <c r="O169">
+        <v>0.96649161667198802</v>
+      </c>
+      <c r="Q169">
+        <v>3961.7369853126802</v>
+      </c>
+      <c r="W169">
+        <v>355.19334505096703</v>
+      </c>
+      <c r="Y169">
+        <v>40.980353480300998</v>
+      </c>
+    </row>
+    <row r="170" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A170" t="str">
+        <f t="shared" si="17"/>
+        <v>Hastings2011CvTitanN50</v>
+      </c>
+      <c r="B170" t="s">
+        <v>34</v>
+      </c>
+      <c r="C170">
+        <v>2011</v>
+      </c>
+      <c r="D170" t="s">
+        <v>9</v>
+      </c>
+      <c r="E170" t="s">
+        <v>32</v>
+      </c>
+      <c r="F170">
+        <v>50</v>
+      </c>
+      <c r="H170" s="1">
+        <v>40926</v>
+      </c>
+      <c r="I170">
+        <v>77</v>
+      </c>
+      <c r="M170">
+        <v>6.1086857158512</v>
+      </c>
+      <c r="O170">
+        <v>0.99204073520302305</v>
+      </c>
+      <c r="Q170">
+        <v>9572.4095323670208</v>
+      </c>
+      <c r="W170">
+        <v>618.64072973923896</v>
+      </c>
+      <c r="Y170">
+        <v>338.60022349746299</v>
+      </c>
+    </row>
+    <row r="171" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A171" t="str">
+        <f t="shared" si="17"/>
+        <v>Hastings2011CvTitanN50</v>
+      </c>
+      <c r="B171" t="s">
+        <v>34</v>
+      </c>
+      <c r="C171">
+        <v>2011</v>
+      </c>
+      <c r="D171" t="s">
+        <v>9</v>
+      </c>
+      <c r="E171" t="s">
+        <v>32</v>
+      </c>
+      <c r="F171">
+        <v>50</v>
+      </c>
+      <c r="H171" s="1">
+        <v>40898</v>
+      </c>
+      <c r="I171">
+        <v>49</v>
+      </c>
+      <c r="M171">
+        <v>6.5332892314333497</v>
+      </c>
+      <c r="O171">
+        <v>0.99439289520270202</v>
+      </c>
+      <c r="Q171">
+        <v>5221.7158633650597</v>
+      </c>
+      <c r="W171">
+        <v>443.54304041113397</v>
+      </c>
+      <c r="Y171">
+        <v>78.628545925372194</v>
+      </c>
+    </row>
+    <row r="172" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A172" t="str">
+        <f t="shared" ref="A172" si="18">B172&amp;C172&amp;"Cv"&amp;E172&amp;"N"&amp;F172</f>
+        <v>Hastings2011CvTitanN100</v>
+      </c>
+      <c r="B172" t="s">
+        <v>34</v>
+      </c>
+      <c r="C172">
+        <v>2011</v>
+      </c>
+      <c r="D172" t="s">
+        <v>9</v>
+      </c>
+      <c r="E172" t="s">
+        <v>32</v>
+      </c>
+      <c r="F172">
+        <v>100</v>
+      </c>
+      <c r="H172" s="1">
+        <v>40940</v>
+      </c>
+      <c r="I172">
+        <v>91</v>
+      </c>
+      <c r="M172">
+        <v>11.410471358379599</v>
+      </c>
+      <c r="O172">
+        <v>0.99983776118276302</v>
+      </c>
+      <c r="Q172">
+        <v>10661.3502581296</v>
+      </c>
+      <c r="W172">
+        <v>663.56840684830104</v>
+      </c>
+      <c r="Y172">
+        <v>402.56661896465903</v>
+      </c>
+    </row>
+    <row r="173" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A173" t="str">
+        <f t="shared" ref="A173:A176" si="19">B173&amp;C173&amp;"Cv"&amp;E173&amp;"N"&amp;F173</f>
+        <v>Hastings2011CvTitanN100</v>
+      </c>
+      <c r="B173" t="s">
+        <v>34</v>
+      </c>
+      <c r="C173">
+        <v>2011</v>
+      </c>
+      <c r="D173" t="s">
+        <v>9</v>
+      </c>
+      <c r="E173" t="s">
+        <v>32</v>
+      </c>
+      <c r="F173">
+        <v>100</v>
+      </c>
+      <c r="H173" s="1">
+        <v>40912</v>
+      </c>
+      <c r="I173">
+        <v>63</v>
+      </c>
+      <c r="M173">
+        <v>7.7910150450980904</v>
+      </c>
+      <c r="O173">
+        <v>0.99745476885937701</v>
+      </c>
+      <c r="Q173">
+        <v>9194.4515914772492</v>
+      </c>
+      <c r="W173">
+        <v>677.68770407906698</v>
+      </c>
+      <c r="Y173">
+        <v>241.757455068658</v>
+      </c>
+    </row>
+    <row r="174" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A174" t="str">
+        <f t="shared" si="19"/>
+        <v>Hastings2011CvTitanN100</v>
+      </c>
+      <c r="B174" t="s">
+        <v>34</v>
+      </c>
+      <c r="C174">
+        <v>2011</v>
+      </c>
+      <c r="D174" t="s">
+        <v>9</v>
+      </c>
+      <c r="E174" t="s">
+        <v>32</v>
+      </c>
+      <c r="F174">
+        <v>100</v>
+      </c>
+      <c r="H174" s="1">
+        <v>40890</v>
+      </c>
+      <c r="I174">
+        <v>41</v>
+      </c>
+      <c r="M174">
+        <v>3.6301283723671198</v>
+      </c>
+      <c r="O174">
+        <v>0.93317213558617196</v>
+      </c>
+      <c r="Q174">
+        <v>3575.7028388522199</v>
+      </c>
+      <c r="W174">
+        <v>316.41763865877402</v>
+      </c>
+      <c r="Y174">
+        <v>41.152645226447397</v>
+      </c>
+    </row>
+    <row r="175" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A175" t="str">
+        <f t="shared" si="19"/>
+        <v>Hastings2011CvTitanN100</v>
+      </c>
+      <c r="B175" t="s">
+        <v>34</v>
+      </c>
+      <c r="C175">
+        <v>2011</v>
+      </c>
+      <c r="D175" t="s">
+        <v>9</v>
+      </c>
+      <c r="E175" t="s">
+        <v>32</v>
+      </c>
+      <c r="F175">
+        <v>100</v>
+      </c>
+      <c r="H175" s="1">
+        <v>40926</v>
+      </c>
+      <c r="I175">
+        <v>77</v>
+      </c>
+      <c r="M175">
+        <v>5.4603953848704903</v>
+      </c>
+      <c r="O175">
+        <v>0.98602505439316901</v>
+      </c>
+      <c r="Q175">
+        <v>9187.3766154087898</v>
+      </c>
+      <c r="W175">
+        <v>575.96608209016097</v>
+      </c>
+      <c r="Y175">
+        <v>342.77157945071798</v>
+      </c>
+    </row>
+    <row r="176" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A176" t="str">
+        <f t="shared" si="19"/>
+        <v>Hastings2011CvTitanN100</v>
+      </c>
+      <c r="B176" t="s">
+        <v>34</v>
+      </c>
+      <c r="C176">
+        <v>2011</v>
+      </c>
+      <c r="D176" t="s">
+        <v>9</v>
+      </c>
+      <c r="E176" t="s">
+        <v>32</v>
+      </c>
+      <c r="F176">
+        <v>100</v>
+      </c>
+      <c r="H176" s="1">
+        <v>40898</v>
+      </c>
+      <c r="I176">
+        <v>49</v>
+      </c>
+      <c r="M176">
+        <v>6.1329578285221604</v>
+      </c>
+      <c r="O176">
+        <v>0.99003700217363599</v>
+      </c>
+      <c r="Q176">
+        <v>5753.5511134419303</v>
+      </c>
+      <c r="W176">
+        <v>485.94440612528899</v>
+      </c>
+      <c r="Y176">
+        <v>89.410705218903601</v>
+      </c>
+    </row>
+    <row r="177" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A177" t="str">
+        <f t="shared" ref="A177" si="20">B177&amp;C177&amp;"Cv"&amp;E177&amp;"N"&amp;F177</f>
+        <v>Hastings2011CvTitanN200</v>
+      </c>
+      <c r="B177" t="s">
+        <v>34</v>
+      </c>
+      <c r="C177">
+        <v>2011</v>
+      </c>
+      <c r="D177" t="s">
+        <v>9</v>
+      </c>
+      <c r="E177" t="s">
+        <v>32</v>
+      </c>
+      <c r="F177">
+        <v>200</v>
+      </c>
+      <c r="H177" s="1">
+        <v>40940</v>
+      </c>
+      <c r="I177">
+        <v>91</v>
+      </c>
+      <c r="M177">
+        <v>12.035353604108399</v>
+      </c>
+      <c r="O177">
+        <v>0.99977870015273196</v>
+      </c>
+      <c r="Q177">
+        <v>11525.3900132663</v>
+      </c>
+      <c r="W177">
+        <v>694.20234648603605</v>
+      </c>
+      <c r="Y177">
+        <v>458.336654840596</v>
+      </c>
+    </row>
+    <row r="178" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A178" t="str">
+        <f t="shared" ref="A178:A181" si="21">B178&amp;C178&amp;"Cv"&amp;E178&amp;"N"&amp;F178</f>
+        <v>Hastings2011CvTitanN200</v>
+      </c>
+      <c r="B178" t="s">
+        <v>34</v>
+      </c>
+      <c r="C178">
+        <v>2011</v>
+      </c>
+      <c r="D178" t="s">
+        <v>9</v>
+      </c>
+      <c r="E178" t="s">
+        <v>32</v>
+      </c>
+      <c r="F178">
+        <v>200</v>
+      </c>
+      <c r="H178" s="1">
+        <v>40912</v>
+      </c>
+      <c r="I178">
+        <v>63</v>
+      </c>
+      <c r="M178">
+        <v>6.6521133690446499</v>
+      </c>
+      <c r="O178">
+        <v>0.99040155103923599</v>
+      </c>
+      <c r="Q178">
+        <v>9273.3935458875603</v>
+      </c>
+      <c r="W178">
+        <v>675.81100296593297</v>
+      </c>
+      <c r="Y178">
+        <v>251.52835162282301</v>
+      </c>
+    </row>
+    <row r="179" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A179" t="str">
+        <f t="shared" si="21"/>
+        <v>Hastings2011CvTitanN200</v>
+      </c>
+      <c r="B179" t="s">
+        <v>34</v>
+      </c>
+      <c r="C179">
+        <v>2011</v>
+      </c>
+      <c r="D179" t="s">
+        <v>9</v>
+      </c>
+      <c r="E179" t="s">
+        <v>32</v>
+      </c>
+      <c r="F179">
+        <v>200</v>
+      </c>
+      <c r="H179" s="1">
+        <v>40890</v>
+      </c>
+      <c r="I179">
+        <v>41</v>
+      </c>
+      <c r="M179">
+        <v>4.2183130272042701</v>
+      </c>
+      <c r="O179">
+        <v>0.96173343690170099</v>
+      </c>
+      <c r="Q179">
+        <v>3745.9739082838</v>
+      </c>
+      <c r="W179">
+        <v>335.13764334311202</v>
+      </c>
+      <c r="Y179">
+        <v>39.459747485267599</v>
+      </c>
+    </row>
+    <row r="180" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A180" t="str">
+        <f t="shared" si="21"/>
+        <v>Hastings2011CvTitanN200</v>
+      </c>
+      <c r="B180" t="s">
+        <v>34</v>
+      </c>
+      <c r="C180">
+        <v>2011</v>
+      </c>
+      <c r="D180" t="s">
+        <v>9</v>
+      </c>
+      <c r="E180" t="s">
+        <v>32</v>
+      </c>
+      <c r="F180">
+        <v>200</v>
+      </c>
+      <c r="H180" s="1">
+        <v>40926</v>
+      </c>
+      <c r="I180">
+        <v>77</v>
+      </c>
+      <c r="M180">
+        <v>6.7147977953260902</v>
+      </c>
+      <c r="O180">
+        <v>0.99234972995231197</v>
+      </c>
+      <c r="Q180">
+        <v>9988.7930057539106</v>
+      </c>
+      <c r="W180">
+        <v>612.79245342483603</v>
+      </c>
+      <c r="Y180">
+        <v>386.086847150555</v>
+      </c>
+    </row>
+    <row r="181" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A181" t="str">
+        <f t="shared" si="21"/>
+        <v>Hastings2011CvTitanN200</v>
+      </c>
+      <c r="B181" t="s">
+        <v>34</v>
+      </c>
+      <c r="C181">
+        <v>2011</v>
+      </c>
+      <c r="D181" t="s">
+        <v>9</v>
+      </c>
+      <c r="E181" t="s">
+        <v>32</v>
+      </c>
+      <c r="F181">
+        <v>200</v>
+      </c>
+      <c r="H181" s="1">
+        <v>40898</v>
+      </c>
+      <c r="I181">
+        <v>49</v>
+      </c>
+      <c r="M181">
+        <v>6.1139445182990704</v>
+      </c>
+      <c r="O181">
+        <v>0.99257280072212395</v>
+      </c>
+      <c r="Q181">
+        <v>5553.2735676788698</v>
+      </c>
+      <c r="W181">
+        <v>468.95391224573001</v>
+      </c>
+      <c r="Y181">
+        <v>86.373444522156802</v>
+      </c>
+    </row>
+    <row r="185" spans="1:25" x14ac:dyDescent="0.45">
       <c r="G185" s="1"/>
-      <c r="H185" s="1"/>
-    </row>
-    <row r="186" spans="7:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="186" spans="1:25" x14ac:dyDescent="0.45">
       <c r="G186" s="1"/>
-      <c r="H186" s="1"/>
-    </row>
-    <row r="187" spans="7:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="187" spans="1:25" x14ac:dyDescent="0.45">
       <c r="G187" s="1"/>
-      <c r="H187" s="1"/>
-    </row>
-    <row r="188" spans="7:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="188" spans="1:25" x14ac:dyDescent="0.45">
       <c r="G188" s="1"/>
-      <c r="H188" s="1"/>
-    </row>
-    <row r="189" spans="7:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="189" spans="1:25" x14ac:dyDescent="0.45">
       <c r="G189" s="1"/>
-      <c r="H189" s="1"/>
-    </row>
-    <row r="190" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="K189" s="1"/>
+    </row>
+    <row r="190" spans="1:25" x14ac:dyDescent="0.45">
       <c r="G190" s="1"/>
-      <c r="H190" s="1"/>
-    </row>
-    <row r="191" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="K190" s="1"/>
+    </row>
+    <row r="191" spans="1:25" x14ac:dyDescent="0.45">
       <c r="G191" s="1"/>
-      <c r="H191" s="1"/>
-    </row>
-    <row r="192" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="K191" s="1"/>
+    </row>
+    <row r="192" spans="1:25" x14ac:dyDescent="0.45">
       <c r="G192" s="1"/>
-      <c r="H192" s="1"/>
-    </row>
-    <row r="193" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="K192" s="1"/>
+    </row>
+    <row r="193" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G193" s="1"/>
-      <c r="H193" s="1"/>
-    </row>
-    <row r="194" spans="7:8" x14ac:dyDescent="0.45">
+      <c r="K193" s="1"/>
+    </row>
+    <row r="194" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G194" s="1"/>
-      <c r="H194" s="1"/>
-    </row>
-    <row r="195" spans="7:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="195" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G195" s="1"/>
       <c r="H195" s="1"/>
     </row>
-    <row r="196" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="196" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G196" s="1"/>
       <c r="H196" s="1"/>
     </row>
-    <row r="197" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="197" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G197" s="1"/>
       <c r="H197" s="1"/>
     </row>
-    <row r="198" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="198" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G198" s="1"/>
       <c r="H198" s="1"/>
     </row>
-    <row r="199" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="199" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G199" s="1"/>
       <c r="H199" s="1"/>
     </row>
-    <row r="200" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="200" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G200" s="1"/>
       <c r="H200" s="1"/>
     </row>
-    <row r="201" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="201" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G201" s="1"/>
       <c r="H201" s="1"/>
     </row>
-    <row r="202" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="202" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G202" s="1"/>
       <c r="H202" s="1"/>
     </row>
-    <row r="203" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="203" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G203" s="1"/>
       <c r="H203" s="1"/>
     </row>
-    <row r="204" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="204" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G204" s="1"/>
       <c r="H204" s="1"/>
     </row>
-    <row r="205" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="205" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G205" s="1"/>
       <c r="H205" s="1"/>
     </row>
-    <row r="206" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="206" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G206" s="1"/>
       <c r="H206" s="1"/>
     </row>
-    <row r="207" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="207" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G207" s="1"/>
       <c r="H207" s="1"/>
     </row>
-    <row r="208" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="208" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G208" s="1"/>
       <c r="H208" s="1"/>
     </row>

</xml_diff>

<commit_message>
Fixed unites in obs data
</commit_message>
<xml_diff>
--- a/Prototypes/ForageBrassica/Observed.xlsx
+++ b/Prototypes/ForageBrassica/Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\APSIMX\Prototypes\ForageBrassica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E2E150-5B91-4985-9720-4758F989F2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4A69E0-D370-4133-8A0E-52F4DF4261F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="35">
   <si>
     <t>SimulationName</t>
   </si>
@@ -737,36 +737,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -921,6 +891,314 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F67B-4442-AC5B-AD316F741579}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$34:$J$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>4.2734128856839702</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.38593511386666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2074015713720101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.91095004022019</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.20162893622065</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.44915963655935</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.7784439334703199</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0097414712836899</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.8940096372478501</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.7004576582050701</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.60301068571549</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.8318485419168304</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.6459567578710699</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.1809689235905498</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.9900769428124101</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.7936517312670399</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.39104473691087</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.1898377099208197</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.1645905694107608</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.0655156887573503</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.7301918073282101</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.5986571790632702</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.5882933584288796</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10.7786098294357</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.6040515264749597</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.87838285025913</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.3985198614214003</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.0841657364863204</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.2328039729657</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.44165157531648</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.2889581482423198</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.1086857158512</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.5332892314333497</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>11.410471358379599</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7.7910150450980904</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.6301283723671198</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.4603953848704903</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.1329578285221604</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12.035353604108399</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.6521133690446499</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.2183130272042701</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6.7147977953260902</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6.1139445182990704</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$34:$L$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>0.12495256192634233</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12003137138056319</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16537393739537953</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14589343039559829</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.20558007598951858</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17560800452325512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.13511590300706813</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1448053472718607</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16839421484165754</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.13613992781782014</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.18590770224766739</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.15905654538386446</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.13052114777242335</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.13849632446770541</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.16030221302109182</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.14656854575584108</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.17324862370081551</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.15813111998903817</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.15054025727170503</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.11882338501785912</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.12387778073936614</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.4049683340537418E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.13467625121084853</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.16153804719333228</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.11079632820539941</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.11853200830436969</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.5370423815281019E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.13512895053031085</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.16551837097132974</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.12321051087853534</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.12074995795956969</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.8743671766100008E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.14729775097761513</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.17195621793652024</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.1149646806073539</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.11472585370886558</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.4804113552223498E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.12620698481589118</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.17336953216925624</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.8431563556238486E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.12586807572927833</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.10957703146959062</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.13037410198841431</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6C4D-4D0A-B515-2D5A7B794208}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1111,7 +1389,901 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Observed!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ForageBrassica.Leaf.CoverTotal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Observed!$M$2:$M$181</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="180"/>
+                <c:pt idx="48">
+                  <c:v>0.74750000000000005</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.0649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.0225</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.3233333333333333</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.3225</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.79500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.0449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.6400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.6333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.4675000000000002</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.085</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.9325000000000001</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.9675000000000002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.6400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.5524999999999998</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.27750000000000002</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.0524999999999998</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.5425</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2.9175000000000004</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>5.1549999999999994</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>4.76</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3.7725</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2.99</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>3.22</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2.9649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>5.2625000000000002</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>4.5724999999999998</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>3.07</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>4.0925000000000002</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>3.5550000000000002</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>5.4850000000000003</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>4.4275000000000002</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>3.68</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>2.7449999999999997</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>3.1025</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1.9875</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>3.9725000000000001</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>4.6375000000000002</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>3.88</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>3.335</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>2.7324999999999999</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>3.6950000000000003</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>4.2734128856839702</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>2.38593511386666</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>4.2074015713720101</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>3.91095004022019</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>1.20162893622065</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>4.44915963655935</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>4.7784439334703199</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>3.0097414712836899</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>3.8940096372478501</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>3.7004576582050701</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>1.60301068571549</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>4.8318485419168304</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>4.6459567578710699</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>3.1809689235905498</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>3.9900769428124101</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>3.7936517312670399</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>1.39104473691087</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>4.1898377099208197</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>8.1645905694107608</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>7.0655156887573503</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>3.7301918073282101</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>4.5986571790632702</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>5.5882933584288796</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>10.7786098294357</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>7.6040515264749597</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>3.87838285025913</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>6.3985198614214003</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>5.0841657364863204</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>10.2328039729657</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>7.44165157531648</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>4.2889581482423198</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>6.1086857158512</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>6.5332892314333497</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>11.410471358379599</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>7.7910150450980904</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>3.6301283723671198</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>5.4603953848704903</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>6.1329578285221604</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>12.035353604108399</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>6.6521133690446499</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>4.2183130272042701</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>6.7147977953260902</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>6.1139445182990704</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Observed!$O$2:$O$181</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="180"/>
+                <c:pt idx="48">
+                  <c:v>0.27500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.47499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.67499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.82500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.32499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.57499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.52500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.37500000000000006</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.77500000000000013</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.8175</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.96000000000000008</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.92749999999999999</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.80249999999999999</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.82250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.82499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.96500000000000008</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.93500000000000005</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.86249999999999993</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.80749999999999988</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.88749999999999996</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.96250000000000002</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.81750000000000012</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.65249999999999997</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.91250000000000009</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.94750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.84499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.71500000000000008</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.83499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>0.998676919785911</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.99640813147117302</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.948382583815777</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.97632837783242599</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.98948355895990103</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0.99964587216560097</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.99593683096649499</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.93942268559731501</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0.99246142865783105</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.98235493341950297</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.99964421924505398</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.99746104046542305</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.96649161667198802</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.99204073520302305</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.99439289520270202</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.99983776118276302</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.99745476885937701</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.93317213558617196</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.98602505439316901</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.99003700217363599</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.99977870015273196</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.99040155103923599</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.96173343690170099</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.99234972995231197</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.99257280072212395</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3800-4E9E-BCA5-3FB06F346EA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AA$25:$AA$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AB$25:$AB$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4.8770575499285984E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22119921692859512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.39346934028736658</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63212055882855767</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.77686983985157021</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8646647167633873</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91791500137610116</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.95021293163213605</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96980261657768152</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98168436111126578</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3800-4E9E-BCA5-3FB06F346EA6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="857944064"/>
+        <c:axId val="857943648"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="857944064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="857943648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="857943648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="857944064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1667,6 +2839,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1700,6 +3388,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>42862</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E749CD4-74A9-49D2-9C4A-F26CB7F776AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6034,10 +7760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF77B2C-709F-457D-BEEB-E013464C345A}">
-  <dimension ref="A2:O34"/>
+  <dimension ref="A2:AB76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AG25" sqref="AG25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6352,7 +8078,7 @@
         <v>6.1956087824351296E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C17">
         <v>145</v>
       </c>
@@ -6378,7 +8104,7 @@
         <v>7.1720430107526878E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>2019</v>
       </c>
@@ -6407,7 +8133,7 @@
         <v>0.14189602446483182</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C19">
         <v>34</v>
       </c>
@@ -6429,7 +8155,7 @@
         <v>7.6383763837638369E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C20">
         <v>40</v>
       </c>
@@ -6453,7 +8179,7 @@
         <v>0.13539755351681956</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C21">
         <v>41</v>
       </c>
@@ -6477,14 +8203,14 @@
         <v>0.1810578105781058</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C22">
         <v>48</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C23">
         <v>61</v>
       </c>
@@ -6493,7 +8219,7 @@
       </c>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C24">
         <v>69</v>
       </c>
@@ -6504,8 +8230,11 @@
       <c r="J24" s="5"/>
       <c r="K24" s="4"/>
       <c r="M24" s="3"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="AB24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C25">
         <v>82</v>
       </c>
@@ -6516,8 +8245,15 @@
       <c r="L25" s="6"/>
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="AA25">
+        <v>0.1</v>
+      </c>
+      <c r="AB25">
+        <f>1-EXP(-AB$24*AA25)</f>
+        <v>4.8770575499285984E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C26">
         <v>98</v>
       </c>
@@ -6525,15 +8261,29 @@
       <c r="E26" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="AA26">
+        <v>0.5</v>
+      </c>
+      <c r="AB26">
+        <f t="shared" ref="AB26:AB34" si="1">1-EXP(-AB$24*AA26)</f>
+        <v>0.22119921692859512</v>
+      </c>
+    </row>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C27">
         <v>110</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="AA27">
+        <v>1</v>
+      </c>
+      <c r="AB27">
+        <f t="shared" si="1"/>
+        <v>0.39346934028736658</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C28">
         <v>118</v>
       </c>
@@ -6541,8 +8291,15 @@
       <c r="E28" s="3">
         <v>47.2</v>
       </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="AA28">
+        <v>2</v>
+      </c>
+      <c r="AB28">
+        <f t="shared" si="1"/>
+        <v>0.63212055882855767</v>
+      </c>
+    </row>
+    <row r="29" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C29">
         <v>132</v>
       </c>
@@ -6550,8 +8307,15 @@
         <v>4.5724999999999998</v>
       </c>
       <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="AA29">
+        <v>3</v>
+      </c>
+      <c r="AB29">
+        <f t="shared" si="1"/>
+        <v>0.77686983985157021</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C30">
         <v>144</v>
       </c>
@@ -6559,8 +8323,15 @@
         <v>3.9</v>
       </c>
       <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="AA30">
+        <v>4</v>
+      </c>
+      <c r="AB30">
+        <f t="shared" si="1"/>
+        <v>0.8646647167633873</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C31">
         <v>145</v>
       </c>
@@ -6568,8 +8339,15 @@
       <c r="E31" s="3">
         <v>28.2</v>
       </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="AA31">
+        <v>5</v>
+      </c>
+      <c r="AB31">
+        <f t="shared" si="1"/>
+        <v>0.91791500137610116</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C32">
         <v>151</v>
       </c>
@@ -6577,8 +8355,18 @@
         <v>3.07</v>
       </c>
       <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="J32" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA32">
+        <v>6</v>
+      </c>
+      <c r="AB32">
+        <f t="shared" si="1"/>
+        <v>0.95021293163213605</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.45">
       <c r="C33">
         <v>165</v>
       </c>
@@ -6586,8 +8374,24 @@
         <v>4.0925000000000002</v>
       </c>
       <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="J33" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" t="s">
+        <v>29</v>
+      </c>
+      <c r="L33" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA33">
+        <v>7</v>
+      </c>
+      <c r="AB33">
+        <f t="shared" si="1"/>
+        <v>0.96980261657768152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -6596,6 +8400,527 @@
       </c>
       <c r="E34" s="3">
         <v>18.850000000000001</v>
+      </c>
+      <c r="J34">
+        <v>4.2734128856839702</v>
+      </c>
+      <c r="K34">
+        <v>34.200282249539498</v>
+      </c>
+      <c r="L34">
+        <f>J34/K34</f>
+        <v>0.12495256192634233</v>
+      </c>
+      <c r="AA34">
+        <v>8</v>
+      </c>
+      <c r="AB34">
+        <f t="shared" si="1"/>
+        <v>0.98168436111126578</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="J35">
+        <v>2.38593511386666</v>
+      </c>
+      <c r="K35">
+        <v>19.877596051968602</v>
+      </c>
+      <c r="L35">
+        <f t="shared" ref="L35:L76" si="2">J35/K35</f>
+        <v>0.12003137138056319</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="J36">
+        <v>4.2074015713720101</v>
+      </c>
+      <c r="K36">
+        <v>25.441745160320302</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="2"/>
+        <v>0.16537393739537953</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="J37">
+        <v>3.91095004022019</v>
+      </c>
+      <c r="K37">
+        <v>26.806896168082602</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="2"/>
+        <v>0.14589343039559829</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="J38">
+        <v>1.20162893622065</v>
+      </c>
+      <c r="K38">
+        <v>5.8450651428006797</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="2"/>
+        <v>0.20558007598951858</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="J39">
+        <v>4.44915963655935</v>
+      </c>
+      <c r="K39">
+        <v>25.3357450797191</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="2"/>
+        <v>0.17560800452325512</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="J40">
+        <v>4.7784439334703199</v>
+      </c>
+      <c r="K40">
+        <v>35.365518248583598</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="2"/>
+        <v>0.13511590300706813</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="J41">
+        <v>3.0097414712836899</v>
+      </c>
+      <c r="K41">
+        <v>20.784739845505399</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="2"/>
+        <v>0.1448053472718607</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="J42">
+        <v>3.8940096372478501</v>
+      </c>
+      <c r="K42">
+        <v>23.124367074661201</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="2"/>
+        <v>0.16839421484165754</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="J43">
+        <v>3.7004576582050701</v>
+      </c>
+      <c r="K43">
+        <v>27.1812811826737</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="2"/>
+        <v>0.13613992781782014</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="J44">
+        <v>1.60301068571549</v>
+      </c>
+      <c r="K44">
+        <v>8.6226157729600104</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="2"/>
+        <v>0.18590770224766739</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="J45">
+        <v>4.8318485419168304</v>
+      </c>
+      <c r="K45">
+        <v>30.378181106949899</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="2"/>
+        <v>0.15905654538386446</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="J46">
+        <v>4.6459567578710699</v>
+      </c>
+      <c r="K46">
+        <v>35.595432902350503</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="2"/>
+        <v>0.13052114777242335</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="J47">
+        <v>3.1809689235905498</v>
+      </c>
+      <c r="K47">
+        <v>22.967894172038399</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="2"/>
+        <v>0.13849632446770541</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="J48">
+        <v>3.9900769428124101</v>
+      </c>
+      <c r="K48">
+        <v>24.8909660547694</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="2"/>
+        <v>0.16030221302109182</v>
+      </c>
+    </row>
+    <row r="49" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J49">
+        <v>3.7936517312670399</v>
+      </c>
+      <c r="K49">
+        <v>25.883123228817698</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="2"/>
+        <v>0.14656854575584108</v>
+      </c>
+    </row>
+    <row r="50" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J50">
+        <v>1.39104473691087</v>
+      </c>
+      <c r="K50">
+        <v>8.0291820344447693</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="2"/>
+        <v>0.17324862370081551</v>
+      </c>
+    </row>
+    <row r="51" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J51">
+        <v>4.1898377099208197</v>
+      </c>
+      <c r="K51">
+        <v>26.4959718884636</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="2"/>
+        <v>0.15813111998903817</v>
+      </c>
+    </row>
+    <row r="52" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J52">
+        <v>8.1645905694107608</v>
+      </c>
+      <c r="K52">
+        <v>54.235263824976506</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="2"/>
+        <v>0.15054025727170503</v>
+      </c>
+    </row>
+    <row r="53" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J53">
+        <v>7.0655156887573503</v>
+      </c>
+      <c r="K53">
+        <v>59.462333005371001</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="2"/>
+        <v>0.11882338501785912</v>
+      </c>
+    </row>
+    <row r="54" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J54">
+        <v>3.7301918073282101</v>
+      </c>
+      <c r="K54">
+        <v>30.111871435414098</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="2"/>
+        <v>0.12387778073936614</v>
+      </c>
+    </row>
+    <row r="55" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J55">
+        <v>4.5986571790632702</v>
+      </c>
+      <c r="K55">
+        <v>54.7135574613798</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="2"/>
+        <v>8.4049683340537418E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J56">
+        <v>5.5882933584288796</v>
+      </c>
+      <c r="K56">
+        <v>41.494274663762901</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="2"/>
+        <v>0.13467625121084853</v>
+      </c>
+    </row>
+    <row r="57" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J57">
+        <v>10.7786098294357</v>
+      </c>
+      <c r="K57">
+        <v>66.724898664496195</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="2"/>
+        <v>0.16153804719333228</v>
+      </c>
+    </row>
+    <row r="58" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J58">
+        <v>7.6040515264749597</v>
+      </c>
+      <c r="K58">
+        <v>68.630898240402104</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="2"/>
+        <v>0.11079632820539941</v>
+      </c>
+    </row>
+    <row r="59" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J59">
+        <v>3.87838285025913</v>
+      </c>
+      <c r="K59">
+        <v>32.720131091511703</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="2"/>
+        <v>0.11853200830436969</v>
+      </c>
+    </row>
+    <row r="60" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J60">
+        <v>6.3985198614214003</v>
+      </c>
+      <c r="K60">
+        <v>67.091238619369307</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="2"/>
+        <v>9.5370423815281019E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J61">
+        <v>5.0841657364863204</v>
+      </c>
+      <c r="K61">
+        <v>37.624548377928001</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="2"/>
+        <v>0.13512895053031085</v>
+      </c>
+    </row>
+    <row r="62" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J62">
+        <v>10.2328039729657</v>
+      </c>
+      <c r="K62">
+        <v>61.822768753192804</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="2"/>
+        <v>0.16551837097132974</v>
+      </c>
+    </row>
+    <row r="63" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J63">
+        <v>7.44165157531648</v>
+      </c>
+      <c r="K63">
+        <v>60.397863155138495</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="2"/>
+        <v>0.12321051087853534</v>
+      </c>
+    </row>
+    <row r="64" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J64">
+        <v>4.2889581482423198</v>
+      </c>
+      <c r="K64">
+        <v>35.519334505096701</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="2"/>
+        <v>0.12074995795956969</v>
+      </c>
+    </row>
+    <row r="65" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J65">
+        <v>6.1086857158512</v>
+      </c>
+      <c r="K65">
+        <v>61.864072973923896</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="2"/>
+        <v>9.8743671766100008E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J66">
+        <v>6.5332892314333497</v>
+      </c>
+      <c r="K66">
+        <v>44.354304041113394</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="2"/>
+        <v>0.14729775097761513</v>
+      </c>
+    </row>
+    <row r="67" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J67">
+        <v>11.410471358379599</v>
+      </c>
+      <c r="K67">
+        <v>66.356840684830104</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="2"/>
+        <v>0.17195621793652024</v>
+      </c>
+    </row>
+    <row r="68" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J68">
+        <v>7.7910150450980904</v>
+      </c>
+      <c r="K68">
+        <v>67.7687704079067</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="2"/>
+        <v>0.1149646806073539</v>
+      </c>
+    </row>
+    <row r="69" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J69">
+        <v>3.6301283723671198</v>
+      </c>
+      <c r="K69">
+        <v>31.641763865877401</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="2"/>
+        <v>0.11472585370886558</v>
+      </c>
+    </row>
+    <row r="70" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J70">
+        <v>5.4603953848704903</v>
+      </c>
+      <c r="K70">
+        <v>57.596608209016097</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="2"/>
+        <v>9.4804113552223498E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J71">
+        <v>6.1329578285221604</v>
+      </c>
+      <c r="K71">
+        <v>48.594440612528899</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="2"/>
+        <v>0.12620698481589118</v>
+      </c>
+    </row>
+    <row r="72" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J72">
+        <v>12.035353604108399</v>
+      </c>
+      <c r="K72">
+        <v>69.420234648603611</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="2"/>
+        <v>0.17336953216925624</v>
+      </c>
+    </row>
+    <row r="73" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J73">
+        <v>6.6521133690446499</v>
+      </c>
+      <c r="K73">
+        <v>67.581100296593291</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="2"/>
+        <v>9.8431563556238486E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J74">
+        <v>4.2183130272042701</v>
+      </c>
+      <c r="K74">
+        <v>33.513764334311205</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="2"/>
+        <v>0.12586807572927833</v>
+      </c>
+    </row>
+    <row r="75" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J75">
+        <v>6.7147977953260902</v>
+      </c>
+      <c r="K75">
+        <v>61.279245342483605</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="2"/>
+        <v>0.10957703146959062</v>
+      </c>
+    </row>
+    <row r="76" spans="10:12" x14ac:dyDescent="0.45">
+      <c r="J76">
+        <v>6.1139445182990704</v>
+      </c>
+      <c r="K76">
+        <v>46.895391224573004</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="2"/>
+        <v>0.13037410198841431</v>
       </c>
     </row>
   </sheetData>
@@ -6608,10 +8933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z2239"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="585" topLeftCell="A132" activePane="bottomLeft"/>
-      <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="K185" sqref="K185"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O181" activeCellId="1" sqref="M1:M181 O1:O181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11495,7 +13818,7 @@
     </row>
     <row r="123" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A123" t="str">
-        <f t="shared" ref="A123:A139" si="10">B123&amp;C123&amp;"Cv"&amp;E123</f>
+        <f t="shared" ref="A123:A138" si="10">B123&amp;C123&amp;"Cv"&amp;E123</f>
         <v>Tosari2019CvGoliath</v>
       </c>
       <c r="B123" t="s">
@@ -12452,13 +14775,13 @@
         <v>4.2734128856839702</v>
       </c>
       <c r="Q139">
-        <v>8409.4345548029505</v>
+        <v>840.94345548029503</v>
       </c>
       <c r="W139">
-        <v>342.00282249539498</v>
+        <v>34.200282249539498</v>
       </c>
       <c r="Y139">
-        <v>498.94063298489903</v>
+        <v>49.894063298489904</v>
       </c>
     </row>
     <row r="140" spans="1:26" x14ac:dyDescent="0.45">
@@ -12492,13 +14815,13 @@
         <v>2.38593511386666</v>
       </c>
       <c r="Q140">
-        <v>3790.7291271215599</v>
+        <v>379.07291271215598</v>
       </c>
       <c r="W140">
-        <v>198.77596051968601</v>
+        <v>19.877596051968602</v>
       </c>
       <c r="Y140">
-        <v>180.296952192471</v>
+        <v>18.029695219247099</v>
       </c>
     </row>
     <row r="141" spans="1:26" x14ac:dyDescent="0.45">
@@ -12532,13 +14855,13 @@
         <v>4.2074015713720101</v>
       </c>
       <c r="Q141">
-        <v>5003.7858111965097</v>
+        <v>500.37858111965096</v>
       </c>
       <c r="W141">
-        <v>254.41745160320301</v>
+        <v>25.441745160320302</v>
       </c>
       <c r="Y141">
-        <v>245.96112951644801</v>
+        <v>24.596112951644802</v>
       </c>
     </row>
     <row r="142" spans="1:26" x14ac:dyDescent="0.45">
@@ -12572,13 +14895,13 @@
         <v>3.91095004022019</v>
       </c>
       <c r="Q142">
-        <v>8271.2209745050604</v>
+        <v>827.12209745050609</v>
       </c>
       <c r="W142">
-        <v>268.06896168082602</v>
+        <v>26.806896168082602</v>
       </c>
       <c r="Y142">
-        <v>559.05313576968001</v>
+        <v>55.905313576967998</v>
       </c>
     </row>
     <row r="143" spans="1:26" x14ac:dyDescent="0.45">
@@ -12612,13 +14935,13 @@
         <v>1.20162893622065</v>
       </c>
       <c r="Q143">
-        <v>958.31223335796597</v>
+        <v>95.831223335796594</v>
       </c>
       <c r="W143">
-        <v>58.4506514280068</v>
+        <v>5.8450651428006797</v>
       </c>
       <c r="Y143">
-        <v>37.3805719077898</v>
+        <v>3.7380571907789801</v>
       </c>
     </row>
     <row r="144" spans="1:26" x14ac:dyDescent="0.45">
@@ -12652,13 +14975,13 @@
         <v>4.44915963655935</v>
       </c>
       <c r="Q144">
-        <v>5906.2235950673303</v>
+        <v>590.62235950673301</v>
       </c>
       <c r="W144">
-        <v>253.35745079719101</v>
+        <v>25.3357450797191</v>
       </c>
       <c r="Y144">
-        <v>337.264908709542</v>
+        <v>33.726490870954201</v>
       </c>
     </row>
     <row r="145" spans="1:25" x14ac:dyDescent="0.45">
@@ -12692,13 +15015,13 @@
         <v>4.7784439334703199</v>
       </c>
       <c r="Q145">
-        <v>9081.3247776613007</v>
+        <v>908.13247776613002</v>
       </c>
       <c r="W145">
-        <v>353.65518248583601</v>
+        <v>35.365518248583598</v>
       </c>
       <c r="Y145">
-        <v>554.47729528029402</v>
+        <v>55.447729528029399</v>
       </c>
     </row>
     <row r="146" spans="1:25" x14ac:dyDescent="0.45">
@@ -12732,13 +15055,13 @@
         <v>3.0097414712836899</v>
       </c>
       <c r="Q146">
-        <v>4267.8622576223897</v>
+        <v>426.78622576223898</v>
       </c>
       <c r="W146">
-        <v>207.84739845505399</v>
+        <v>20.784739845505399</v>
       </c>
       <c r="Y146">
-        <v>218.93882730718499</v>
+        <v>21.893882730718499</v>
       </c>
     </row>
     <row r="147" spans="1:25" x14ac:dyDescent="0.45">
@@ -12772,13 +15095,13 @@
         <v>3.8940096372478501</v>
       </c>
       <c r="Q147">
-        <v>4685.2981772967696</v>
+        <v>468.52981772967695</v>
       </c>
       <c r="W147">
-        <v>231.243670746612</v>
+        <v>23.124367074661201</v>
       </c>
       <c r="Y147">
-        <v>237.28614698306399</v>
+        <v>23.728614698306398</v>
       </c>
     </row>
     <row r="148" spans="1:25" x14ac:dyDescent="0.45">
@@ -12811,13 +15134,13 @@
         <v>3.7004576582050701</v>
       </c>
       <c r="Q148">
-        <v>9133.8811105518107</v>
+        <v>913.38811105518107</v>
       </c>
       <c r="W148">
-        <v>271.812811826737</v>
+        <v>27.1812811826737</v>
       </c>
       <c r="Y148">
-        <v>641.57529922844401</v>
+        <v>64.157529922844404</v>
       </c>
     </row>
     <row r="149" spans="1:25" x14ac:dyDescent="0.45">
@@ -12850,13 +15173,13 @@
         <v>1.60301068571549</v>
       </c>
       <c r="Q149">
-        <v>1193.34667608724</v>
+        <v>119.334667608724</v>
       </c>
       <c r="W149">
-        <v>86.226157729600104</v>
+        <v>8.6226157729600104</v>
       </c>
       <c r="Y149">
-        <v>33.108509879124</v>
+        <v>3.3108509879124002</v>
       </c>
     </row>
     <row r="150" spans="1:25" x14ac:dyDescent="0.45">
@@ -12889,13 +15212,13 @@
         <v>4.8318485419168304</v>
       </c>
       <c r="Q150">
-        <v>6790.5599068424899</v>
+        <v>679.05599068424897</v>
       </c>
       <c r="W150">
-        <v>303.78181106949899</v>
+        <v>30.378181106949899</v>
       </c>
       <c r="Y150">
-        <v>375.27417961474998</v>
+        <v>37.527417961474995</v>
       </c>
     </row>
     <row r="151" spans="1:25" x14ac:dyDescent="0.45">
@@ -12928,13 +15251,13 @@
         <v>4.6459567578710699</v>
       </c>
       <c r="Q151">
-        <v>8706.9473661811699</v>
+        <v>870.69473661811696</v>
       </c>
       <c r="W151">
-        <v>355.95432902350501</v>
+        <v>35.595432902350503</v>
       </c>
       <c r="Y151">
-        <v>514.74040759461104</v>
+        <v>51.474040759461104</v>
       </c>
     </row>
     <row r="152" spans="1:25" x14ac:dyDescent="0.45">
@@ -12967,13 +15290,13 @@
         <v>3.1809689235905498</v>
       </c>
       <c r="Q152">
-        <v>4339.8961949680897</v>
+        <v>433.98961949680898</v>
       </c>
       <c r="W152">
-        <v>229.67894172038399</v>
+        <v>22.967894172038399</v>
       </c>
       <c r="Y152">
-        <v>204.310677776425</v>
+        <v>20.4310677776425</v>
       </c>
     </row>
     <row r="153" spans="1:25" x14ac:dyDescent="0.45">
@@ -13006,13 +15329,13 @@
         <v>3.9900769428124101</v>
       </c>
       <c r="Q153">
-        <v>4965.0415522431304</v>
+        <v>496.50415522431302</v>
       </c>
       <c r="W153">
-        <v>248.90966054769399</v>
+        <v>24.8909660547694</v>
       </c>
       <c r="Y153">
-        <v>247.59449467661901</v>
+        <v>24.759449467661902</v>
       </c>
     </row>
     <row r="154" spans="1:25" x14ac:dyDescent="0.45">
@@ -13045,13 +15368,13 @@
         <v>3.7936517312670399</v>
       </c>
       <c r="Q154">
-        <v>8965.1452421549893</v>
+        <v>896.51452421549891</v>
       </c>
       <c r="W154">
-        <v>258.83123228817698</v>
+        <v>25.883123228817698</v>
       </c>
       <c r="Y154">
-        <v>637.68329192732199</v>
+        <v>63.768329192732196</v>
       </c>
     </row>
     <row r="155" spans="1:25" x14ac:dyDescent="0.45">
@@ -13084,13 +15407,13 @@
         <v>1.39104473691087</v>
       </c>
       <c r="Q155">
-        <v>1075.2894469022799</v>
+        <v>107.52894469022799</v>
       </c>
       <c r="W155">
-        <v>80.2918203444477</v>
+        <v>8.0291820344447693</v>
       </c>
       <c r="Y155">
-        <v>27.237124345780501</v>
+        <v>2.7237124345780499</v>
       </c>
     </row>
     <row r="156" spans="1:25" x14ac:dyDescent="0.45">
@@ -13123,13 +15446,13 @@
         <v>4.1898377099208197</v>
       </c>
       <c r="Q156">
-        <v>5915.7994063526403</v>
+        <v>591.57994063526405</v>
       </c>
       <c r="W156">
-        <v>264.959718884636</v>
+        <v>26.4959718884636</v>
       </c>
       <c r="Y156">
-        <v>326.62022175062702</v>
+        <v>32.662022175062702</v>
       </c>
     </row>
     <row r="157" spans="1:25" x14ac:dyDescent="0.45">
@@ -13165,13 +15488,13 @@
         <v>0.998676919785911</v>
       </c>
       <c r="Q157">
-        <v>9762.9904923440899</v>
+        <v>976.29904923440904</v>
       </c>
       <c r="W157">
-        <v>542.35263824976505</v>
+        <v>54.235263824976506</v>
       </c>
       <c r="Y157">
-        <v>433.94641098464399</v>
+        <v>43.394641098464398</v>
       </c>
     </row>
     <row r="158" spans="1:25" x14ac:dyDescent="0.45">
@@ -13207,13 +15530,13 @@
         <v>0.99640813147117302</v>
       </c>
       <c r="Q158">
-        <v>7951.5884628649201</v>
+        <v>795.15884628649201</v>
       </c>
       <c r="W158">
-        <v>594.62333005370999</v>
+        <v>59.462333005371001</v>
       </c>
       <c r="Y158">
-        <v>200.53551623278199</v>
+        <v>20.053551623278199</v>
       </c>
     </row>
     <row r="159" spans="1:25" x14ac:dyDescent="0.45">
@@ -13249,13 +15572,13 @@
         <v>0.948382583815777</v>
       </c>
       <c r="Q159">
-        <v>3312.9813225682301</v>
+        <v>331.29813225682301</v>
       </c>
       <c r="W159">
-        <v>301.11871435414099</v>
+        <v>30.111871435414098</v>
       </c>
       <c r="Y159">
-        <v>30.179417902682601</v>
+        <v>3.0179417902682601</v>
       </c>
     </row>
     <row r="160" spans="1:25" x14ac:dyDescent="0.45">
@@ -13291,13 +15614,13 @@
         <v>0.97632837783242599</v>
       </c>
       <c r="Q160">
-        <v>9448.6475449364298</v>
+        <v>944.86475449364298</v>
       </c>
       <c r="W160">
-        <v>547.13557461379798</v>
+        <v>54.7135574613798</v>
       </c>
       <c r="Y160">
-        <v>397.72917987984601</v>
+        <v>39.772917987984599</v>
       </c>
     </row>
     <row r="161" spans="1:25" x14ac:dyDescent="0.45">
@@ -13333,13 +15656,13 @@
         <v>0.98948355895990103</v>
       </c>
       <c r="Q161">
-        <v>4926.49292863344</v>
+        <v>492.64929286334399</v>
       </c>
       <c r="W161">
-        <v>414.942746637629</v>
+        <v>41.494274663762901</v>
       </c>
       <c r="Y161">
-        <v>77.706546225714803</v>
+        <v>7.7706546225714801</v>
       </c>
     </row>
     <row r="162" spans="1:25" x14ac:dyDescent="0.45">
@@ -13375,13 +15698,13 @@
         <v>0.99964587216560097</v>
       </c>
       <c r="Q162">
-        <v>10973.6367949293</v>
+        <v>1097.36367949293</v>
       </c>
       <c r="W162">
-        <v>667.24898664496197</v>
+        <v>66.724898664496195</v>
       </c>
       <c r="Y162">
-        <v>430.11469284797198</v>
+        <v>43.011469284797201</v>
       </c>
     </row>
     <row r="163" spans="1:25" x14ac:dyDescent="0.45">
@@ -13417,13 +15740,13 @@
         <v>0.99593683096649499</v>
       </c>
       <c r="Q163">
-        <v>8741.2869633606297</v>
+        <v>874.12869633606294</v>
       </c>
       <c r="W163">
-        <v>686.30898240402098</v>
+        <v>68.630898240402104</v>
       </c>
       <c r="Y163">
-        <v>187.81971393204199</v>
+        <v>18.781971393204199</v>
       </c>
     </row>
     <row r="164" spans="1:25" x14ac:dyDescent="0.45">
@@ -13459,13 +15782,13 @@
         <v>0.93942268559731501</v>
       </c>
       <c r="Q164">
-        <v>3602.0018772098001</v>
+        <v>360.20018772098001</v>
       </c>
       <c r="W164">
-        <v>327.20131091511701</v>
+        <v>32.720131091511703</v>
       </c>
       <c r="Y164">
-        <v>32.998876805862501</v>
+        <v>3.29988768058625</v>
       </c>
     </row>
     <row r="165" spans="1:25" x14ac:dyDescent="0.45">
@@ -13501,13 +15824,13 @@
         <v>0.99246142865783105</v>
       </c>
       <c r="Q165">
-        <v>10293.856954487301</v>
+        <v>1029.3856954487301</v>
       </c>
       <c r="W165">
-        <v>670.91238619369301</v>
+        <v>67.091238619369307</v>
       </c>
       <c r="Y165">
-        <v>358.47330925504201</v>
+        <v>35.847330925504203</v>
       </c>
     </row>
     <row r="166" spans="1:25" x14ac:dyDescent="0.45">
@@ -13543,13 +15866,13 @@
         <v>0.98235493341950297</v>
       </c>
       <c r="Q166">
-        <v>4479.3273904906</v>
+        <v>447.93273904905999</v>
       </c>
       <c r="W166">
-        <v>376.24548377927999</v>
+        <v>37.624548377928001</v>
       </c>
       <c r="Y166">
-        <v>71.687255269780707</v>
+        <v>7.1687255269780703</v>
       </c>
     </row>
     <row r="167" spans="1:25" x14ac:dyDescent="0.45">
@@ -13585,13 +15908,13 @@
         <v>0.99964421924505398</v>
       </c>
       <c r="Q167">
-        <v>10135.9557791151</v>
+        <v>1013.59557791151</v>
       </c>
       <c r="W167">
-        <v>618.22768753192804</v>
+        <v>61.822768753192804</v>
       </c>
       <c r="Y167">
-        <v>395.36789037958602</v>
+        <v>39.536789037958599</v>
       </c>
     </row>
     <row r="168" spans="1:25" x14ac:dyDescent="0.45">
@@ -13627,13 +15950,13 @@
         <v>0.99746104046542305</v>
       </c>
       <c r="Q168">
-        <v>7834.5644140710801</v>
+        <v>783.45644140710806</v>
       </c>
       <c r="W168">
-        <v>603.97863155138498</v>
+        <v>60.397863155138495</v>
       </c>
       <c r="Y168">
-        <v>179.477809855723</v>
+        <v>17.947780985572301</v>
       </c>
     </row>
     <row r="169" spans="1:25" x14ac:dyDescent="0.45">
@@ -13669,13 +15992,13 @@
         <v>0.96649161667198802</v>
       </c>
       <c r="Q169">
-        <v>3961.7369853126802</v>
+        <v>396.17369853126803</v>
       </c>
       <c r="W169">
-        <v>355.19334505096703</v>
+        <v>35.519334505096701</v>
       </c>
       <c r="Y169">
-        <v>40.980353480300998</v>
+        <v>4.0980353480301002</v>
       </c>
     </row>
     <row r="170" spans="1:25" x14ac:dyDescent="0.45">
@@ -13711,13 +16034,13 @@
         <v>0.99204073520302305</v>
       </c>
       <c r="Q170">
-        <v>9572.4095323670208</v>
+        <v>957.24095323670213</v>
       </c>
       <c r="W170">
-        <v>618.64072973923896</v>
+        <v>61.864072973923896</v>
       </c>
       <c r="Y170">
-        <v>338.60022349746299</v>
+        <v>33.860022349746302</v>
       </c>
     </row>
     <row r="171" spans="1:25" x14ac:dyDescent="0.45">
@@ -13753,13 +16076,13 @@
         <v>0.99439289520270202</v>
       </c>
       <c r="Q171">
-        <v>5221.7158633650597</v>
+        <v>522.17158633650592</v>
       </c>
       <c r="W171">
-        <v>443.54304041113397</v>
+        <v>44.354304041113394</v>
       </c>
       <c r="Y171">
-        <v>78.628545925372194</v>
+        <v>7.8628545925372197</v>
       </c>
     </row>
     <row r="172" spans="1:25" x14ac:dyDescent="0.45">
@@ -13795,13 +16118,13 @@
         <v>0.99983776118276302</v>
       </c>
       <c r="Q172">
-        <v>10661.3502581296</v>
+        <v>1066.1350258129601</v>
       </c>
       <c r="W172">
-        <v>663.56840684830104</v>
+        <v>66.356840684830104</v>
       </c>
       <c r="Y172">
-        <v>402.56661896465903</v>
+        <v>40.2566618964659</v>
       </c>
     </row>
     <row r="173" spans="1:25" x14ac:dyDescent="0.45">
@@ -13837,13 +16160,13 @@
         <v>0.99745476885937701</v>
       </c>
       <c r="Q173">
-        <v>9194.4515914772492</v>
+        <v>919.44515914772489</v>
       </c>
       <c r="W173">
-        <v>677.68770407906698</v>
+        <v>67.7687704079067</v>
       </c>
       <c r="Y173">
-        <v>241.757455068658</v>
+        <v>24.175745506865802</v>
       </c>
     </row>
     <row r="174" spans="1:25" x14ac:dyDescent="0.45">
@@ -13879,13 +16202,13 @@
         <v>0.93317213558617196</v>
       </c>
       <c r="Q174">
-        <v>3575.7028388522199</v>
+        <v>357.57028388522201</v>
       </c>
       <c r="W174">
-        <v>316.41763865877402</v>
+        <v>31.641763865877401</v>
       </c>
       <c r="Y174">
-        <v>41.152645226447397</v>
+        <v>4.1152645226447397</v>
       </c>
     </row>
     <row r="175" spans="1:25" x14ac:dyDescent="0.45">
@@ -13921,13 +16244,13 @@
         <v>0.98602505439316901</v>
       </c>
       <c r="Q175">
-        <v>9187.3766154087898</v>
+        <v>918.737661540879</v>
       </c>
       <c r="W175">
-        <v>575.96608209016097</v>
+        <v>57.596608209016097</v>
       </c>
       <c r="Y175">
-        <v>342.77157945071798</v>
+        <v>34.277157945071799</v>
       </c>
     </row>
     <row r="176" spans="1:25" x14ac:dyDescent="0.45">
@@ -13963,13 +16286,13 @@
         <v>0.99003700217363599</v>
       </c>
       <c r="Q176">
-        <v>5753.5511134419303</v>
+        <v>575.35511134419301</v>
       </c>
       <c r="W176">
-        <v>485.94440612528899</v>
+        <v>48.594440612528899</v>
       </c>
       <c r="Y176">
-        <v>89.410705218903601</v>
+        <v>8.9410705218903601</v>
       </c>
     </row>
     <row r="177" spans="1:25" x14ac:dyDescent="0.45">
@@ -14005,13 +16328,13 @@
         <v>0.99977870015273196</v>
       </c>
       <c r="Q177">
-        <v>11525.3900132663</v>
+        <v>1152.5390013266301</v>
       </c>
       <c r="W177">
-        <v>694.20234648603605</v>
+        <v>69.420234648603611</v>
       </c>
       <c r="Y177">
-        <v>458.336654840596</v>
+        <v>45.833665484059601</v>
       </c>
     </row>
     <row r="178" spans="1:25" x14ac:dyDescent="0.45">
@@ -14047,13 +16370,13 @@
         <v>0.99040155103923599</v>
       </c>
       <c r="Q178">
-        <v>9273.3935458875603</v>
+        <v>927.33935458875601</v>
       </c>
       <c r="W178">
-        <v>675.81100296593297</v>
+        <v>67.581100296593291</v>
       </c>
       <c r="Y178">
-        <v>251.52835162282301</v>
+        <v>25.152835162282301</v>
       </c>
     </row>
     <row r="179" spans="1:25" x14ac:dyDescent="0.45">
@@ -14089,13 +16412,13 @@
         <v>0.96173343690170099</v>
       </c>
       <c r="Q179">
-        <v>3745.9739082838</v>
+        <v>374.59739082838001</v>
       </c>
       <c r="W179">
-        <v>335.13764334311202</v>
+        <v>33.513764334311205</v>
       </c>
       <c r="Y179">
-        <v>39.459747485267599</v>
+        <v>3.9459747485267598</v>
       </c>
     </row>
     <row r="180" spans="1:25" x14ac:dyDescent="0.45">
@@ -14131,13 +16454,13 @@
         <v>0.99234972995231197</v>
       </c>
       <c r="Q180">
-        <v>9988.7930057539106</v>
+        <v>998.87930057539108</v>
       </c>
       <c r="W180">
-        <v>612.79245342483603</v>
+        <v>61.279245342483605</v>
       </c>
       <c r="Y180">
-        <v>386.086847150555</v>
+        <v>38.608684715055503</v>
       </c>
     </row>
     <row r="181" spans="1:25" x14ac:dyDescent="0.45">
@@ -14173,13 +16496,13 @@
         <v>0.99257280072212395</v>
       </c>
       <c r="Q181">
-        <v>5553.2735676788698</v>
+        <v>555.32735676788695</v>
       </c>
       <c r="W181">
-        <v>468.95391224573001</v>
+        <v>46.895391224573004</v>
       </c>
       <c r="Y181">
-        <v>86.373444522156802</v>
+        <v>8.6373444522156806</v>
       </c>
     </row>
     <row r="185" spans="1:25" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Add Hastings Experiment Simulations
</commit_message>
<xml_diff>
--- a/Prototypes/ForageBrassica/Observed.xlsx
+++ b/Prototypes/ForageBrassica/Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\APSIMX\Prototypes\ForageBrassica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4A69E0-D370-4133-8A0E-52F4DF4261F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5120331-17F4-49D6-80E6-DB4E9FFF6973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -7762,7 +7762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF77B2C-709F-457D-BEEB-E013464C345A}">
   <dimension ref="A2:AB76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AG25" sqref="AG25"/>
     </sheetView>
   </sheetViews>
@@ -8933,8 +8933,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z2239"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O181" activeCellId="1" sqref="M1:M181 O1:O181"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="25035" ySplit="975" topLeftCell="Q129" activePane="bottomRight"/>
+      <selection activeCell="G8" sqref="G8"/>
+      <selection pane="topRight" activeCell="Q1" sqref="Q1"/>
+      <selection pane="bottomLeft" activeCell="I61" sqref="I61"/>
+      <selection pane="bottomRight" activeCell="Z139" sqref="Z139:Z181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14778,10 +14782,10 @@
         <v>840.94345548029503</v>
       </c>
       <c r="W139">
-        <v>34.200282249539498</v>
+        <v>342.00282249539498</v>
       </c>
       <c r="Y139">
-        <v>49.894063298489904</v>
+        <v>498.94063298489903</v>
       </c>
     </row>
     <row r="140" spans="1:26" x14ac:dyDescent="0.45">
@@ -14818,10 +14822,10 @@
         <v>379.07291271215598</v>
       </c>
       <c r="W140">
-        <v>19.877596051968602</v>
+        <v>198.77596051968601</v>
       </c>
       <c r="Y140">
-        <v>18.029695219247099</v>
+        <v>180.296952192471</v>
       </c>
     </row>
     <row r="141" spans="1:26" x14ac:dyDescent="0.45">
@@ -14858,10 +14862,10 @@
         <v>500.37858111965096</v>
       </c>
       <c r="W141">
-        <v>25.441745160320302</v>
+        <v>254.41745160320301</v>
       </c>
       <c r="Y141">
-        <v>24.596112951644802</v>
+        <v>245.96112951644801</v>
       </c>
     </row>
     <row r="142" spans="1:26" x14ac:dyDescent="0.45">
@@ -14898,10 +14902,10 @@
         <v>827.12209745050609</v>
       </c>
       <c r="W142">
-        <v>26.806896168082602</v>
+        <v>268.06896168082602</v>
       </c>
       <c r="Y142">
-        <v>55.905313576967998</v>
+        <v>559.05313576968001</v>
       </c>
     </row>
     <row r="143" spans="1:26" x14ac:dyDescent="0.45">
@@ -14938,10 +14942,10 @@
         <v>95.831223335796594</v>
       </c>
       <c r="W143">
-        <v>5.8450651428006797</v>
+        <v>58.450651428006793</v>
       </c>
       <c r="Y143">
-        <v>3.7380571907789801</v>
+        <v>37.3805719077898</v>
       </c>
     </row>
     <row r="144" spans="1:26" x14ac:dyDescent="0.45">
@@ -14978,10 +14982,10 @@
         <v>590.62235950673301</v>
       </c>
       <c r="W144">
-        <v>25.3357450797191</v>
+        <v>253.35745079719101</v>
       </c>
       <c r="Y144">
-        <v>33.726490870954201</v>
+        <v>337.264908709542</v>
       </c>
     </row>
     <row r="145" spans="1:25" x14ac:dyDescent="0.45">
@@ -15018,10 +15022,10 @@
         <v>908.13247776613002</v>
       </c>
       <c r="W145">
-        <v>35.365518248583598</v>
+        <v>353.65518248583601</v>
       </c>
       <c r="Y145">
-        <v>55.447729528029399</v>
+        <v>554.47729528029402</v>
       </c>
     </row>
     <row r="146" spans="1:25" x14ac:dyDescent="0.45">
@@ -15058,10 +15062,10 @@
         <v>426.78622576223898</v>
       </c>
       <c r="W146">
-        <v>20.784739845505399</v>
+        <v>207.84739845505399</v>
       </c>
       <c r="Y146">
-        <v>21.893882730718499</v>
+        <v>218.93882730718499</v>
       </c>
     </row>
     <row r="147" spans="1:25" x14ac:dyDescent="0.45">
@@ -15098,10 +15102,10 @@
         <v>468.52981772967695</v>
       </c>
       <c r="W147">
-        <v>23.124367074661201</v>
+        <v>231.243670746612</v>
       </c>
       <c r="Y147">
-        <v>23.728614698306398</v>
+        <v>237.28614698306399</v>
       </c>
     </row>
     <row r="148" spans="1:25" x14ac:dyDescent="0.45">
@@ -15137,10 +15141,10 @@
         <v>913.38811105518107</v>
       </c>
       <c r="W148">
-        <v>27.1812811826737</v>
+        <v>271.812811826737</v>
       </c>
       <c r="Y148">
-        <v>64.157529922844404</v>
+        <v>641.57529922844401</v>
       </c>
     </row>
     <row r="149" spans="1:25" x14ac:dyDescent="0.45">
@@ -15176,10 +15180,10 @@
         <v>119.334667608724</v>
       </c>
       <c r="W149">
-        <v>8.6226157729600104</v>
+        <v>86.226157729600104</v>
       </c>
       <c r="Y149">
-        <v>3.3108509879124002</v>
+        <v>33.108509879124</v>
       </c>
     </row>
     <row r="150" spans="1:25" x14ac:dyDescent="0.45">
@@ -15215,10 +15219,10 @@
         <v>679.05599068424897</v>
       </c>
       <c r="W150">
-        <v>30.378181106949899</v>
+        <v>303.78181106949899</v>
       </c>
       <c r="Y150">
-        <v>37.527417961474995</v>
+        <v>375.27417961474998</v>
       </c>
     </row>
     <row r="151" spans="1:25" x14ac:dyDescent="0.45">
@@ -15254,10 +15258,10 @@
         <v>870.69473661811696</v>
       </c>
       <c r="W151">
-        <v>35.595432902350503</v>
+        <v>355.95432902350501</v>
       </c>
       <c r="Y151">
-        <v>51.474040759461104</v>
+        <v>514.74040759461104</v>
       </c>
     </row>
     <row r="152" spans="1:25" x14ac:dyDescent="0.45">
@@ -15293,10 +15297,10 @@
         <v>433.98961949680898</v>
       </c>
       <c r="W152">
-        <v>22.967894172038399</v>
+        <v>229.67894172038399</v>
       </c>
       <c r="Y152">
-        <v>20.4310677776425</v>
+        <v>204.310677776425</v>
       </c>
     </row>
     <row r="153" spans="1:25" x14ac:dyDescent="0.45">
@@ -15332,10 +15336,10 @@
         <v>496.50415522431302</v>
       </c>
       <c r="W153">
-        <v>24.8909660547694</v>
+        <v>248.90966054769399</v>
       </c>
       <c r="Y153">
-        <v>24.759449467661902</v>
+        <v>247.59449467661904</v>
       </c>
     </row>
     <row r="154" spans="1:25" x14ac:dyDescent="0.45">
@@ -15371,10 +15375,10 @@
         <v>896.51452421549891</v>
       </c>
       <c r="W154">
-        <v>25.883123228817698</v>
+        <v>258.83123228817698</v>
       </c>
       <c r="Y154">
-        <v>63.768329192732196</v>
+        <v>637.68329192732199</v>
       </c>
     </row>
     <row r="155" spans="1:25" x14ac:dyDescent="0.45">
@@ -15410,10 +15414,10 @@
         <v>107.52894469022799</v>
       </c>
       <c r="W155">
-        <v>8.0291820344447693</v>
+        <v>80.2918203444477</v>
       </c>
       <c r="Y155">
-        <v>2.7237124345780499</v>
+        <v>27.237124345780501</v>
       </c>
     </row>
     <row r="156" spans="1:25" x14ac:dyDescent="0.45">
@@ -15449,10 +15453,10 @@
         <v>591.57994063526405</v>
       </c>
       <c r="W156">
-        <v>26.4959718884636</v>
+        <v>264.959718884636</v>
       </c>
       <c r="Y156">
-        <v>32.662022175062702</v>
+        <v>326.62022175062702</v>
       </c>
     </row>
     <row r="157" spans="1:25" x14ac:dyDescent="0.45">
@@ -15491,10 +15495,10 @@
         <v>976.29904923440904</v>
       </c>
       <c r="W157">
-        <v>54.235263824976506</v>
+        <v>542.35263824976505</v>
       </c>
       <c r="Y157">
-        <v>43.394641098464398</v>
+        <v>433.94641098464399</v>
       </c>
     </row>
     <row r="158" spans="1:25" x14ac:dyDescent="0.45">
@@ -15533,10 +15537,10 @@
         <v>795.15884628649201</v>
       </c>
       <c r="W158">
-        <v>59.462333005371001</v>
+        <v>594.62333005370999</v>
       </c>
       <c r="Y158">
-        <v>20.053551623278199</v>
+        <v>200.53551623278199</v>
       </c>
     </row>
     <row r="159" spans="1:25" x14ac:dyDescent="0.45">
@@ -15575,10 +15579,10 @@
         <v>331.29813225682301</v>
       </c>
       <c r="W159">
-        <v>30.111871435414098</v>
+        <v>301.11871435414099</v>
       </c>
       <c r="Y159">
-        <v>3.0179417902682601</v>
+        <v>30.179417902682601</v>
       </c>
     </row>
     <row r="160" spans="1:25" x14ac:dyDescent="0.45">
@@ -15617,10 +15621,10 @@
         <v>944.86475449364298</v>
       </c>
       <c r="W160">
-        <v>54.7135574613798</v>
+        <v>547.13557461379798</v>
       </c>
       <c r="Y160">
-        <v>39.772917987984599</v>
+        <v>397.72917987984601</v>
       </c>
     </row>
     <row r="161" spans="1:25" x14ac:dyDescent="0.45">
@@ -15659,10 +15663,10 @@
         <v>492.64929286334399</v>
       </c>
       <c r="W161">
-        <v>41.494274663762901</v>
+        <v>414.942746637629</v>
       </c>
       <c r="Y161">
-        <v>7.7706546225714801</v>
+        <v>77.706546225714803</v>
       </c>
     </row>
     <row r="162" spans="1:25" x14ac:dyDescent="0.45">
@@ -15701,10 +15705,10 @@
         <v>1097.36367949293</v>
       </c>
       <c r="W162">
-        <v>66.724898664496195</v>
+        <v>667.24898664496197</v>
       </c>
       <c r="Y162">
-        <v>43.011469284797201</v>
+        <v>430.11469284797204</v>
       </c>
     </row>
     <row r="163" spans="1:25" x14ac:dyDescent="0.45">
@@ -15743,10 +15747,10 @@
         <v>874.12869633606294</v>
       </c>
       <c r="W163">
-        <v>68.630898240402104</v>
+        <v>686.30898240402098</v>
       </c>
       <c r="Y163">
-        <v>18.781971393204199</v>
+        <v>187.81971393204199</v>
       </c>
     </row>
     <row r="164" spans="1:25" x14ac:dyDescent="0.45">
@@ -15785,10 +15789,10 @@
         <v>360.20018772098001</v>
       </c>
       <c r="W164">
-        <v>32.720131091511703</v>
+        <v>327.20131091511701</v>
       </c>
       <c r="Y164">
-        <v>3.29988768058625</v>
+        <v>32.998876805862501</v>
       </c>
     </row>
     <row r="165" spans="1:25" x14ac:dyDescent="0.45">
@@ -15827,10 +15831,10 @@
         <v>1029.3856954487301</v>
       </c>
       <c r="W165">
-        <v>67.091238619369307</v>
+        <v>670.91238619369301</v>
       </c>
       <c r="Y165">
-        <v>35.847330925504203</v>
+        <v>358.47330925504201</v>
       </c>
     </row>
     <row r="166" spans="1:25" x14ac:dyDescent="0.45">
@@ -15869,10 +15873,10 @@
         <v>447.93273904905999</v>
       </c>
       <c r="W166">
-        <v>37.624548377928001</v>
+        <v>376.24548377927999</v>
       </c>
       <c r="Y166">
-        <v>7.1687255269780703</v>
+        <v>71.687255269780707</v>
       </c>
     </row>
     <row r="167" spans="1:25" x14ac:dyDescent="0.45">
@@ -15911,10 +15915,10 @@
         <v>1013.59557791151</v>
       </c>
       <c r="W167">
-        <v>61.822768753192804</v>
+        <v>618.22768753192804</v>
       </c>
       <c r="Y167">
-        <v>39.536789037958599</v>
+        <v>395.36789037958602</v>
       </c>
     </row>
     <row r="168" spans="1:25" x14ac:dyDescent="0.45">
@@ -15953,10 +15957,10 @@
         <v>783.45644140710806</v>
       </c>
       <c r="W168">
-        <v>60.397863155138495</v>
+        <v>603.97863155138498</v>
       </c>
       <c r="Y168">
-        <v>17.947780985572301</v>
+        <v>179.47780985572302</v>
       </c>
     </row>
     <row r="169" spans="1:25" x14ac:dyDescent="0.45">
@@ -15995,10 +15999,10 @@
         <v>396.17369853126803</v>
       </c>
       <c r="W169">
-        <v>35.519334505096701</v>
+        <v>355.19334505096703</v>
       </c>
       <c r="Y169">
-        <v>4.0980353480301002</v>
+        <v>40.980353480301005</v>
       </c>
     </row>
     <row r="170" spans="1:25" x14ac:dyDescent="0.45">
@@ -16037,10 +16041,10 @@
         <v>957.24095323670213</v>
       </c>
       <c r="W170">
-        <v>61.864072973923896</v>
+        <v>618.64072973923896</v>
       </c>
       <c r="Y170">
-        <v>33.860022349746302</v>
+        <v>338.60022349746305</v>
       </c>
     </row>
     <row r="171" spans="1:25" x14ac:dyDescent="0.45">
@@ -16079,10 +16083,10 @@
         <v>522.17158633650592</v>
       </c>
       <c r="W171">
-        <v>44.354304041113394</v>
+        <v>443.54304041113392</v>
       </c>
       <c r="Y171">
-        <v>7.8628545925372197</v>
+        <v>78.628545925372194</v>
       </c>
     </row>
     <row r="172" spans="1:25" x14ac:dyDescent="0.45">
@@ -16121,10 +16125,10 @@
         <v>1066.1350258129601</v>
       </c>
       <c r="W172">
-        <v>66.356840684830104</v>
+        <v>663.56840684830104</v>
       </c>
       <c r="Y172">
-        <v>40.2566618964659</v>
+        <v>402.56661896465903</v>
       </c>
     </row>
     <row r="173" spans="1:25" x14ac:dyDescent="0.45">
@@ -16163,10 +16167,10 @@
         <v>919.44515914772489</v>
       </c>
       <c r="W173">
-        <v>67.7687704079067</v>
+        <v>677.68770407906698</v>
       </c>
       <c r="Y173">
-        <v>24.175745506865802</v>
+        <v>241.75745506865803</v>
       </c>
     </row>
     <row r="174" spans="1:25" x14ac:dyDescent="0.45">
@@ -16205,10 +16209,10 @@
         <v>357.57028388522201</v>
       </c>
       <c r="W174">
-        <v>31.641763865877401</v>
+        <v>316.41763865877402</v>
       </c>
       <c r="Y174">
-        <v>4.1152645226447397</v>
+        <v>41.152645226447397</v>
       </c>
     </row>
     <row r="175" spans="1:25" x14ac:dyDescent="0.45">
@@ -16247,10 +16251,10 @@
         <v>918.737661540879</v>
       </c>
       <c r="W175">
-        <v>57.596608209016097</v>
+        <v>575.96608209016097</v>
       </c>
       <c r="Y175">
-        <v>34.277157945071799</v>
+        <v>342.77157945071798</v>
       </c>
     </row>
     <row r="176" spans="1:25" x14ac:dyDescent="0.45">
@@ -16289,10 +16293,10 @@
         <v>575.35511134419301</v>
       </c>
       <c r="W176">
-        <v>48.594440612528899</v>
+        <v>485.94440612528899</v>
       </c>
       <c r="Y176">
-        <v>8.9410705218903601</v>
+        <v>89.410705218903601</v>
       </c>
     </row>
     <row r="177" spans="1:25" x14ac:dyDescent="0.45">
@@ -16331,10 +16335,10 @@
         <v>1152.5390013266301</v>
       </c>
       <c r="W177">
-        <v>69.420234648603611</v>
+        <v>694.20234648603605</v>
       </c>
       <c r="Y177">
-        <v>45.833665484059601</v>
+        <v>458.336654840596</v>
       </c>
     </row>
     <row r="178" spans="1:25" x14ac:dyDescent="0.45">
@@ -16373,10 +16377,10 @@
         <v>927.33935458875601</v>
       </c>
       <c r="W178">
-        <v>67.581100296593291</v>
+        <v>675.81100296593286</v>
       </c>
       <c r="Y178">
-        <v>25.152835162282301</v>
+        <v>251.52835162282301</v>
       </c>
     </row>
     <row r="179" spans="1:25" x14ac:dyDescent="0.45">
@@ -16415,10 +16419,10 @@
         <v>374.59739082838001</v>
       </c>
       <c r="W179">
-        <v>33.513764334311205</v>
+        <v>335.13764334311202</v>
       </c>
       <c r="Y179">
-        <v>3.9459747485267598</v>
+        <v>39.459747485267599</v>
       </c>
     </row>
     <row r="180" spans="1:25" x14ac:dyDescent="0.45">
@@ -16457,10 +16461,10 @@
         <v>998.87930057539108</v>
       </c>
       <c r="W180">
-        <v>61.279245342483605</v>
+        <v>612.79245342483603</v>
       </c>
       <c r="Y180">
-        <v>38.608684715055503</v>
+        <v>386.08684715055506</v>
       </c>
     </row>
     <row r="181" spans="1:25" x14ac:dyDescent="0.45">
@@ -16499,10 +16503,10 @@
         <v>555.32735676788695</v>
       </c>
       <c r="W181">
-        <v>46.895391224573004</v>
+        <v>468.95391224573007</v>
       </c>
       <c r="Y181">
-        <v>8.6373444522156806</v>
+        <v>86.373444522156802</v>
       </c>
     </row>
     <row r="185" spans="1:25" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
fixed DAS in OBS
</commit_message>
<xml_diff>
--- a/Prototypes/ForageBrassica/Observed.xlsx
+++ b/Prototypes/ForageBrassica/Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\APSIMX\Prototypes\ForageBrassica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEFB3A3-9B90-4A80-A5D1-D404ABAFFA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06B3040-6924-48FC-ADA3-1B91CF190736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="870" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19215" yWindow="1035" windowWidth="19065" windowHeight="20700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -689,7 +689,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -699,6 +699,8 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7297,7 +7299,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E37CBB69-8253-4EBA-9B3E-56DDB7A5EE18}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E37CBB69-8253-4EBA-9B3E-56DDB7A5EE18}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A4:E34" firstHeaderRow="1" firstDataRow="2" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="25">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -7796,8 +7798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF77B2C-709F-457D-BEEB-E013464C345A}">
   <dimension ref="A2:AB76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AG25" sqref="AG25"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8967,11 +8969,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB2235"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="46305" ySplit="1875" topLeftCell="Y241" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="46305" ySplit="1875" topLeftCell="Y238" activePane="bottomLeft"/>
       <selection activeCell="G8" sqref="G8"/>
       <selection pane="topRight" activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="C270" sqref="C270:C274"/>
+      <selection pane="bottomLeft" activeCell="I139" sqref="I139:I274"/>
       <selection pane="bottomRight" activeCell="Z139" sqref="Z139:Z181"/>
     </sheetView>
   </sheetViews>
@@ -12145,7 +12147,7 @@
         <v>17.916666666666668</v>
       </c>
       <c r="L76">
-        <v>3.5021638332824323</v>
+        <v>3.5021638332824301</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.45">
@@ -14810,11 +14812,14 @@
       <c r="F139">
         <v>1</v>
       </c>
-      <c r="G139" s="1"/>
+      <c r="G139" s="1">
+        <v>40135</v>
+      </c>
       <c r="H139" s="1">
         <v>40212</v>
       </c>
       <c r="I139">
+        <f>H139-G139</f>
         <v>77</v>
       </c>
       <c r="M139">
@@ -14850,11 +14855,14 @@
       <c r="F140">
         <v>1</v>
       </c>
-      <c r="G140" s="1"/>
+      <c r="G140" s="1">
+        <v>40135</v>
+      </c>
       <c r="H140" s="1">
         <v>40184</v>
       </c>
       <c r="I140">
+        <f t="shared" ref="I140:I203" si="13">H140-G140</f>
         <v>49</v>
       </c>
       <c r="M140">
@@ -14890,11 +14898,14 @@
       <c r="F141">
         <v>1</v>
       </c>
-      <c r="G141" s="1"/>
+      <c r="G141" s="1">
+        <v>40135</v>
+      </c>
       <c r="H141" s="1">
         <v>40193</v>
       </c>
       <c r="I141">
+        <f t="shared" si="13"/>
         <v>58</v>
       </c>
       <c r="M141">
@@ -14930,11 +14941,14 @@
       <c r="F142">
         <v>1</v>
       </c>
-      <c r="G142" s="1"/>
+      <c r="G142" s="1">
+        <v>40135</v>
+      </c>
       <c r="H142" s="1">
         <v>40224</v>
       </c>
       <c r="I142">
+        <f t="shared" si="13"/>
         <v>89</v>
       </c>
       <c r="M142">
@@ -14970,11 +14984,14 @@
       <c r="F143">
         <v>1</v>
       </c>
-      <c r="G143" s="1"/>
+      <c r="G143" s="1">
+        <v>40135</v>
+      </c>
       <c r="H143" s="1">
         <v>40169</v>
       </c>
       <c r="I143">
+        <f t="shared" si="13"/>
         <v>34</v>
       </c>
       <c r="M143">
@@ -15010,11 +15027,14 @@
       <c r="F144">
         <v>1</v>
       </c>
-      <c r="G144" s="1"/>
+      <c r="G144" s="1">
+        <v>40135</v>
+      </c>
       <c r="H144" s="1">
         <v>40203</v>
       </c>
       <c r="I144">
+        <f t="shared" si="13"/>
         <v>68</v>
       </c>
       <c r="M144">
@@ -15050,11 +15070,14 @@
       <c r="F145">
         <v>2</v>
       </c>
-      <c r="G145" s="1"/>
+      <c r="G145" s="1">
+        <v>40135</v>
+      </c>
       <c r="H145" s="1">
         <v>40212</v>
       </c>
       <c r="I145">
+        <f t="shared" si="13"/>
         <v>77</v>
       </c>
       <c r="M145">
@@ -15090,11 +15113,14 @@
       <c r="F146">
         <v>2</v>
       </c>
-      <c r="G146" s="1"/>
+      <c r="G146" s="1">
+        <v>40135</v>
+      </c>
       <c r="H146" s="1">
         <v>40184</v>
       </c>
       <c r="I146">
+        <f t="shared" si="13"/>
         <v>49</v>
       </c>
       <c r="M146">
@@ -15130,11 +15156,14 @@
       <c r="F147">
         <v>2</v>
       </c>
-      <c r="G147" s="1"/>
+      <c r="G147" s="1">
+        <v>40135</v>
+      </c>
       <c r="H147" s="1">
         <v>40193</v>
       </c>
       <c r="I147">
+        <f t="shared" si="13"/>
         <v>58</v>
       </c>
       <c r="M147">
@@ -15170,10 +15199,14 @@
       <c r="F148">
         <v>2</v>
       </c>
+      <c r="G148" s="1">
+        <v>40135</v>
+      </c>
       <c r="H148" s="1">
         <v>40224</v>
       </c>
       <c r="I148">
+        <f t="shared" si="13"/>
         <v>89</v>
       </c>
       <c r="M148">
@@ -15209,10 +15242,14 @@
       <c r="F149">
         <v>2</v>
       </c>
+      <c r="G149" s="1">
+        <v>40135</v>
+      </c>
       <c r="H149" s="1">
         <v>40169</v>
       </c>
       <c r="I149">
+        <f t="shared" si="13"/>
         <v>34</v>
       </c>
       <c r="M149">
@@ -15248,10 +15285,14 @@
       <c r="F150">
         <v>2</v>
       </c>
+      <c r="G150" s="1">
+        <v>40135</v>
+      </c>
       <c r="H150" s="1">
         <v>40203</v>
       </c>
       <c r="I150">
+        <f t="shared" si="13"/>
         <v>68</v>
       </c>
       <c r="M150">
@@ -15287,10 +15328,14 @@
       <c r="F151">
         <v>3</v>
       </c>
+      <c r="G151" s="1">
+        <v>40135</v>
+      </c>
       <c r="H151" s="1">
         <v>40212</v>
       </c>
       <c r="I151">
+        <f t="shared" si="13"/>
         <v>77</v>
       </c>
       <c r="M151">
@@ -15326,10 +15371,14 @@
       <c r="F152">
         <v>3</v>
       </c>
+      <c r="G152" s="1">
+        <v>40135</v>
+      </c>
       <c r="H152" s="1">
         <v>40184</v>
       </c>
       <c r="I152">
+        <f t="shared" si="13"/>
         <v>49</v>
       </c>
       <c r="M152">
@@ -15365,10 +15414,14 @@
       <c r="F153">
         <v>3</v>
       </c>
+      <c r="G153" s="1">
+        <v>40135</v>
+      </c>
       <c r="H153" s="1">
         <v>40193</v>
       </c>
       <c r="I153">
+        <f t="shared" si="13"/>
         <v>58</v>
       </c>
       <c r="M153">
@@ -15404,10 +15457,14 @@
       <c r="F154">
         <v>3</v>
       </c>
+      <c r="G154" s="1">
+        <v>40135</v>
+      </c>
       <c r="H154" s="1">
         <v>40224</v>
       </c>
       <c r="I154">
+        <f t="shared" si="13"/>
         <v>89</v>
       </c>
       <c r="M154">
@@ -15443,10 +15500,14 @@
       <c r="F155">
         <v>3</v>
       </c>
+      <c r="G155" s="1">
+        <v>40135</v>
+      </c>
       <c r="H155" s="1">
         <v>40169</v>
       </c>
       <c r="I155">
+        <f t="shared" si="13"/>
         <v>34</v>
       </c>
       <c r="M155">
@@ -15482,10 +15543,14 @@
       <c r="F156">
         <v>3</v>
       </c>
+      <c r="G156" s="1">
+        <v>40135</v>
+      </c>
       <c r="H156" s="1">
         <v>40203</v>
       </c>
       <c r="I156">
+        <f t="shared" si="13"/>
         <v>68</v>
       </c>
       <c r="M156">
@@ -15521,10 +15586,14 @@
       <c r="F157">
         <v>0</v>
       </c>
+      <c r="G157" s="1">
+        <v>40849</v>
+      </c>
       <c r="H157" s="1">
         <v>40940</v>
       </c>
       <c r="I157">
+        <f t="shared" si="13"/>
         <v>91</v>
       </c>
       <c r="M157">
@@ -15545,7 +15614,7 @@
     </row>
     <row r="158" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A158" t="str">
-        <f t="shared" ref="A158:A161" si="13">B158&amp;C158&amp;"Cv"&amp;E158&amp;"N"&amp;F158</f>
+        <f t="shared" ref="A158:A161" si="14">B158&amp;C158&amp;"Cv"&amp;E158&amp;"N"&amp;F158</f>
         <v>Hastings2011CvTitanN0</v>
       </c>
       <c r="B158" t="s">
@@ -15563,10 +15632,14 @@
       <c r="F158">
         <v>0</v>
       </c>
+      <c r="G158" s="1">
+        <v>40849</v>
+      </c>
       <c r="H158" s="1">
         <v>40912</v>
       </c>
       <c r="I158">
+        <f t="shared" si="13"/>
         <v>63</v>
       </c>
       <c r="M158">
@@ -15587,7 +15660,7 @@
     </row>
     <row r="159" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A159" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Hastings2011CvTitanN0</v>
       </c>
       <c r="B159" t="s">
@@ -15605,10 +15678,14 @@
       <c r="F159">
         <v>0</v>
       </c>
+      <c r="G159" s="1">
+        <v>40849</v>
+      </c>
       <c r="H159" s="1">
         <v>40890</v>
       </c>
       <c r="I159">
+        <f t="shared" si="13"/>
         <v>41</v>
       </c>
       <c r="M159">
@@ -15629,7 +15706,7 @@
     </row>
     <row r="160" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A160" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Hastings2011CvTitanN0</v>
       </c>
       <c r="B160" t="s">
@@ -15647,10 +15724,14 @@
       <c r="F160">
         <v>0</v>
       </c>
+      <c r="G160" s="1">
+        <v>40849</v>
+      </c>
       <c r="H160" s="1">
         <v>40926</v>
       </c>
       <c r="I160">
+        <f t="shared" si="13"/>
         <v>77</v>
       </c>
       <c r="M160">
@@ -15671,7 +15752,7 @@
     </row>
     <row r="161" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A161" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>Hastings2011CvTitanN0</v>
       </c>
       <c r="B161" t="s">
@@ -15689,10 +15770,14 @@
       <c r="F161">
         <v>0</v>
       </c>
+      <c r="G161" s="1">
+        <v>40849</v>
+      </c>
       <c r="H161" s="1">
         <v>40898</v>
       </c>
       <c r="I161">
+        <f t="shared" si="13"/>
         <v>49</v>
       </c>
       <c r="M161">
@@ -15713,7 +15798,7 @@
     </row>
     <row r="162" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A162" t="str">
-        <f t="shared" ref="A162" si="14">B162&amp;C162&amp;"Cv"&amp;E162&amp;"N"&amp;F162</f>
+        <f t="shared" ref="A162" si="15">B162&amp;C162&amp;"Cv"&amp;E162&amp;"N"&amp;F162</f>
         <v>Hastings2011CvTitanN25</v>
       </c>
       <c r="B162" t="s">
@@ -15731,10 +15816,14 @@
       <c r="F162">
         <v>25</v>
       </c>
+      <c r="G162" s="1">
+        <v>40849</v>
+      </c>
       <c r="H162" s="1">
         <v>40940</v>
       </c>
       <c r="I162">
+        <f t="shared" si="13"/>
         <v>91</v>
       </c>
       <c r="M162">
@@ -15755,7 +15844,7 @@
     </row>
     <row r="163" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A163" t="str">
-        <f t="shared" ref="A163:A166" si="15">B163&amp;C163&amp;"Cv"&amp;E163&amp;"N"&amp;F163</f>
+        <f t="shared" ref="A163:A166" si="16">B163&amp;C163&amp;"Cv"&amp;E163&amp;"N"&amp;F163</f>
         <v>Hastings2011CvTitanN25</v>
       </c>
       <c r="B163" t="s">
@@ -15773,10 +15862,14 @@
       <c r="F163">
         <v>25</v>
       </c>
+      <c r="G163" s="1">
+        <v>40849</v>
+      </c>
       <c r="H163" s="1">
         <v>40912</v>
       </c>
       <c r="I163">
+        <f t="shared" si="13"/>
         <v>63</v>
       </c>
       <c r="M163">
@@ -15797,7 +15890,7 @@
     </row>
     <row r="164" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A164" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Hastings2011CvTitanN25</v>
       </c>
       <c r="B164" t="s">
@@ -15815,10 +15908,14 @@
       <c r="F164">
         <v>25</v>
       </c>
+      <c r="G164" s="1">
+        <v>40849</v>
+      </c>
       <c r="H164" s="1">
         <v>40890</v>
       </c>
       <c r="I164">
+        <f t="shared" si="13"/>
         <v>41</v>
       </c>
       <c r="M164">
@@ -15839,7 +15936,7 @@
     </row>
     <row r="165" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A165" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Hastings2011CvTitanN25</v>
       </c>
       <c r="B165" t="s">
@@ -15857,10 +15954,14 @@
       <c r="F165">
         <v>25</v>
       </c>
+      <c r="G165" s="1">
+        <v>40849</v>
+      </c>
       <c r="H165" s="1">
         <v>40926</v>
       </c>
       <c r="I165">
+        <f t="shared" si="13"/>
         <v>77</v>
       </c>
       <c r="M165">
@@ -15881,7 +15982,7 @@
     </row>
     <row r="166" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A166" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Hastings2011CvTitanN25</v>
       </c>
       <c r="B166" t="s">
@@ -15899,10 +16000,14 @@
       <c r="F166">
         <v>25</v>
       </c>
+      <c r="G166" s="1">
+        <v>40849</v>
+      </c>
       <c r="H166" s="1">
         <v>40898</v>
       </c>
       <c r="I166">
+        <f t="shared" si="13"/>
         <v>49</v>
       </c>
       <c r="M166">
@@ -15923,7 +16028,7 @@
     </row>
     <row r="167" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A167" t="str">
-        <f t="shared" ref="A167" si="16">B167&amp;C167&amp;"Cv"&amp;E167&amp;"N"&amp;F167</f>
+        <f t="shared" ref="A167" si="17">B167&amp;C167&amp;"Cv"&amp;E167&amp;"N"&amp;F167</f>
         <v>Hastings2011CvTitanN50</v>
       </c>
       <c r="B167" t="s">
@@ -15941,10 +16046,14 @@
       <c r="F167">
         <v>50</v>
       </c>
+      <c r="G167" s="1">
+        <v>40849</v>
+      </c>
       <c r="H167" s="1">
         <v>40940</v>
       </c>
       <c r="I167">
+        <f t="shared" si="13"/>
         <v>91</v>
       </c>
       <c r="M167">
@@ -15965,7 +16074,7 @@
     </row>
     <row r="168" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A168" t="str">
-        <f t="shared" ref="A168:A171" si="17">B168&amp;C168&amp;"Cv"&amp;E168&amp;"N"&amp;F168</f>
+        <f t="shared" ref="A168:A171" si="18">B168&amp;C168&amp;"Cv"&amp;E168&amp;"N"&amp;F168</f>
         <v>Hastings2011CvTitanN50</v>
       </c>
       <c r="B168" t="s">
@@ -15983,10 +16092,14 @@
       <c r="F168">
         <v>50</v>
       </c>
+      <c r="G168" s="1">
+        <v>40849</v>
+      </c>
       <c r="H168" s="1">
         <v>40912</v>
       </c>
       <c r="I168">
+        <f t="shared" si="13"/>
         <v>63</v>
       </c>
       <c r="M168">
@@ -16007,7 +16120,7 @@
     </row>
     <row r="169" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A169" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Hastings2011CvTitanN50</v>
       </c>
       <c r="B169" t="s">
@@ -16025,10 +16138,14 @@
       <c r="F169">
         <v>50</v>
       </c>
+      <c r="G169" s="1">
+        <v>40849</v>
+      </c>
       <c r="H169" s="1">
         <v>40890</v>
       </c>
       <c r="I169">
+        <f t="shared" si="13"/>
         <v>41</v>
       </c>
       <c r="M169">
@@ -16049,7 +16166,7 @@
     </row>
     <row r="170" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A170" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Hastings2011CvTitanN50</v>
       </c>
       <c r="B170" t="s">
@@ -16067,10 +16184,14 @@
       <c r="F170">
         <v>50</v>
       </c>
+      <c r="G170" s="1">
+        <v>40849</v>
+      </c>
       <c r="H170" s="1">
         <v>40926</v>
       </c>
       <c r="I170">
+        <f t="shared" si="13"/>
         <v>77</v>
       </c>
       <c r="M170">
@@ -16091,7 +16212,7 @@
     </row>
     <row r="171" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A171" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Hastings2011CvTitanN50</v>
       </c>
       <c r="B171" t="s">
@@ -16109,10 +16230,14 @@
       <c r="F171">
         <v>50</v>
       </c>
+      <c r="G171" s="1">
+        <v>40849</v>
+      </c>
       <c r="H171" s="1">
         <v>40898</v>
       </c>
       <c r="I171">
+        <f t="shared" si="13"/>
         <v>49</v>
       </c>
       <c r="M171">
@@ -16133,7 +16258,7 @@
     </row>
     <row r="172" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A172" t="str">
-        <f t="shared" ref="A172" si="18">B172&amp;C172&amp;"Cv"&amp;E172&amp;"N"&amp;F172</f>
+        <f t="shared" ref="A172" si="19">B172&amp;C172&amp;"Cv"&amp;E172&amp;"N"&amp;F172</f>
         <v>Hastings2011CvTitanN100</v>
       </c>
       <c r="B172" t="s">
@@ -16151,10 +16276,14 @@
       <c r="F172">
         <v>100</v>
       </c>
+      <c r="G172" s="1">
+        <v>40849</v>
+      </c>
       <c r="H172" s="1">
         <v>40940</v>
       </c>
       <c r="I172">
+        <f t="shared" si="13"/>
         <v>91</v>
       </c>
       <c r="M172">
@@ -16175,7 +16304,7 @@
     </row>
     <row r="173" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A173" t="str">
-        <f t="shared" ref="A173:A176" si="19">B173&amp;C173&amp;"Cv"&amp;E173&amp;"N"&amp;F173</f>
+        <f t="shared" ref="A173:A176" si="20">B173&amp;C173&amp;"Cv"&amp;E173&amp;"N"&amp;F173</f>
         <v>Hastings2011CvTitanN100</v>
       </c>
       <c r="B173" t="s">
@@ -16193,10 +16322,14 @@
       <c r="F173">
         <v>100</v>
       </c>
+      <c r="G173" s="1">
+        <v>40849</v>
+      </c>
       <c r="H173" s="1">
         <v>40912</v>
       </c>
       <c r="I173">
+        <f t="shared" si="13"/>
         <v>63</v>
       </c>
       <c r="M173">
@@ -16217,7 +16350,7 @@
     </row>
     <row r="174" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A174" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Hastings2011CvTitanN100</v>
       </c>
       <c r="B174" t="s">
@@ -16235,10 +16368,14 @@
       <c r="F174">
         <v>100</v>
       </c>
+      <c r="G174" s="1">
+        <v>40849</v>
+      </c>
       <c r="H174" s="1">
         <v>40890</v>
       </c>
       <c r="I174">
+        <f t="shared" si="13"/>
         <v>41</v>
       </c>
       <c r="M174">
@@ -16259,7 +16396,7 @@
     </row>
     <row r="175" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A175" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Hastings2011CvTitanN100</v>
       </c>
       <c r="B175" t="s">
@@ -16277,10 +16414,14 @@
       <c r="F175">
         <v>100</v>
       </c>
+      <c r="G175" s="1">
+        <v>40849</v>
+      </c>
       <c r="H175" s="1">
         <v>40926</v>
       </c>
       <c r="I175">
+        <f t="shared" si="13"/>
         <v>77</v>
       </c>
       <c r="M175">
@@ -16301,7 +16442,7 @@
     </row>
     <row r="176" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A176" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>Hastings2011CvTitanN100</v>
       </c>
       <c r="B176" t="s">
@@ -16319,10 +16460,14 @@
       <c r="F176">
         <v>100</v>
       </c>
+      <c r="G176" s="1">
+        <v>40849</v>
+      </c>
       <c r="H176" s="1">
         <v>40898</v>
       </c>
       <c r="I176">
+        <f t="shared" si="13"/>
         <v>49</v>
       </c>
       <c r="M176">
@@ -16343,7 +16488,7 @@
     </row>
     <row r="177" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A177" t="str">
-        <f t="shared" ref="A177" si="20">B177&amp;C177&amp;"Cv"&amp;E177&amp;"N"&amp;F177</f>
+        <f t="shared" ref="A177" si="21">B177&amp;C177&amp;"Cv"&amp;E177&amp;"N"&amp;F177</f>
         <v>Hastings2011CvTitanN200</v>
       </c>
       <c r="B177" t="s">
@@ -16361,10 +16506,14 @@
       <c r="F177">
         <v>200</v>
       </c>
+      <c r="G177" s="1">
+        <v>40849</v>
+      </c>
       <c r="H177" s="1">
         <v>40940</v>
       </c>
       <c r="I177">
+        <f t="shared" si="13"/>
         <v>91</v>
       </c>
       <c r="M177">
@@ -16385,7 +16534,7 @@
     </row>
     <row r="178" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A178" t="str">
-        <f t="shared" ref="A178:A182" si="21">B178&amp;C178&amp;"Cv"&amp;E178&amp;"N"&amp;F178</f>
+        <f t="shared" ref="A178:A182" si="22">B178&amp;C178&amp;"Cv"&amp;E178&amp;"N"&amp;F178</f>
         <v>Hastings2011CvTitanN200</v>
       </c>
       <c r="B178" t="s">
@@ -16403,10 +16552,14 @@
       <c r="F178">
         <v>200</v>
       </c>
+      <c r="G178" s="1">
+        <v>40849</v>
+      </c>
       <c r="H178" s="1">
         <v>40912</v>
       </c>
       <c r="I178">
+        <f t="shared" si="13"/>
         <v>63</v>
       </c>
       <c r="M178">
@@ -16427,7 +16580,7 @@
     </row>
     <row r="179" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A179" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Hastings2011CvTitanN200</v>
       </c>
       <c r="B179" t="s">
@@ -16445,10 +16598,14 @@
       <c r="F179">
         <v>200</v>
       </c>
+      <c r="G179" s="1">
+        <v>40849</v>
+      </c>
       <c r="H179" s="1">
         <v>40890</v>
       </c>
       <c r="I179">
+        <f t="shared" si="13"/>
         <v>41</v>
       </c>
       <c r="M179">
@@ -16469,7 +16626,7 @@
     </row>
     <row r="180" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A180" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Hastings2011CvTitanN200</v>
       </c>
       <c r="B180" t="s">
@@ -16487,10 +16644,14 @@
       <c r="F180">
         <v>200</v>
       </c>
+      <c r="G180" s="1">
+        <v>40849</v>
+      </c>
       <c r="H180" s="1">
         <v>40926</v>
       </c>
       <c r="I180">
+        <f t="shared" si="13"/>
         <v>77</v>
       </c>
       <c r="M180">
@@ -16511,7 +16672,7 @@
     </row>
     <row r="181" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A181" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Hastings2011CvTitanN200</v>
       </c>
       <c r="B181" t="s">
@@ -16529,10 +16690,14 @@
       <c r="F181">
         <v>200</v>
       </c>
+      <c r="G181" s="1">
+        <v>40849</v>
+      </c>
       <c r="H181" s="1">
         <v>40898</v>
       </c>
       <c r="I181">
+        <f t="shared" si="13"/>
         <v>49</v>
       </c>
       <c r="M181">
@@ -16553,7 +16718,7 @@
     </row>
     <row r="182" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A182" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>Terang2004CvWinfredN0</v>
       </c>
       <c r="B182" t="s">
@@ -16571,10 +16736,14 @@
       <c r="F182">
         <v>0</v>
       </c>
+      <c r="G182" s="1">
+        <v>38324</v>
+      </c>
       <c r="H182" s="1">
         <v>38394</v>
       </c>
       <c r="I182">
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
       <c r="Q182">
@@ -16589,7 +16758,7 @@
     </row>
     <row r="183" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A183" t="str">
-        <f t="shared" ref="A183:A193" si="22">B183&amp;C183&amp;"Cv"&amp;E183&amp;"N"&amp;F183</f>
+        <f t="shared" ref="A183:A193" si="23">B183&amp;C183&amp;"Cv"&amp;E183&amp;"N"&amp;F183</f>
         <v>Terang2004CvWinfredN40</v>
       </c>
       <c r="B183" t="s">
@@ -16607,10 +16776,14 @@
       <c r="F183">
         <v>40</v>
       </c>
+      <c r="G183" s="1">
+        <v>38324</v>
+      </c>
       <c r="H183" s="1">
         <v>38394</v>
       </c>
       <c r="I183">
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
       <c r="Q183">
@@ -16625,7 +16798,7 @@
     </row>
     <row r="184" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A184" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Terang2004CvWinfredN80</v>
       </c>
       <c r="B184" t="s">
@@ -16643,10 +16816,14 @@
       <c r="F184">
         <v>80</v>
       </c>
+      <c r="G184" s="1">
+        <v>38324</v>
+      </c>
       <c r="H184" s="1">
         <v>38394</v>
       </c>
       <c r="I184">
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
       <c r="Q184">
@@ -16661,7 +16838,7 @@
     </row>
     <row r="185" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A185" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Terang2004CvWinfredN120</v>
       </c>
       <c r="B185" t="s">
@@ -16679,11 +16856,14 @@
       <c r="F185">
         <v>120</v>
       </c>
-      <c r="G185" s="1"/>
+      <c r="G185" s="1">
+        <v>38324</v>
+      </c>
       <c r="H185" s="1">
         <v>38394</v>
       </c>
       <c r="I185">
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
       <c r="Q185">
@@ -16698,7 +16878,7 @@
     </row>
     <row r="186" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A186" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Terang2004CvWinfredN160</v>
       </c>
       <c r="B186" t="s">
@@ -16716,11 +16896,14 @@
       <c r="F186">
         <v>160</v>
       </c>
-      <c r="G186" s="1"/>
+      <c r="G186" s="1">
+        <v>38324</v>
+      </c>
       <c r="H186" s="1">
         <v>38394</v>
       </c>
       <c r="I186">
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
       <c r="Q186">
@@ -16735,7 +16918,7 @@
     </row>
     <row r="187" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A187" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Terang2004CvWinfredN200</v>
       </c>
       <c r="B187" t="s">
@@ -16753,11 +16936,14 @@
       <c r="F187">
         <v>200</v>
       </c>
-      <c r="G187" s="1"/>
+      <c r="G187" s="1">
+        <v>38324</v>
+      </c>
       <c r="H187" s="1">
         <v>38394</v>
       </c>
       <c r="I187">
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
       <c r="Q187">
@@ -16772,7 +16958,7 @@
     </row>
     <row r="188" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A188" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Terang2007CvWinfredN0</v>
       </c>
       <c r="B188" t="s">
@@ -16790,11 +16976,14 @@
       <c r="F188">
         <v>0</v>
       </c>
-      <c r="G188" s="1"/>
+      <c r="G188" s="1">
+        <v>39375</v>
+      </c>
       <c r="H188" s="1">
         <v>39464</v>
       </c>
       <c r="I188">
+        <f t="shared" si="13"/>
         <v>89</v>
       </c>
       <c r="Q188">
@@ -16809,7 +16998,7 @@
     </row>
     <row r="189" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A189" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Terang2007CvWinfredN40</v>
       </c>
       <c r="B189" t="s">
@@ -16827,11 +17016,14 @@
       <c r="F189">
         <v>40</v>
       </c>
-      <c r="G189" s="1"/>
+      <c r="G189" s="1">
+        <v>39375</v>
+      </c>
       <c r="H189" s="1">
         <v>39464</v>
       </c>
       <c r="I189">
+        <f t="shared" si="13"/>
         <v>89</v>
       </c>
       <c r="K189" s="1"/>
@@ -16847,7 +17039,7 @@
     </row>
     <row r="190" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A190" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Terang2007CvWinfredN80</v>
       </c>
       <c r="B190" t="s">
@@ -16865,11 +17057,14 @@
       <c r="F190">
         <v>80</v>
       </c>
-      <c r="G190" s="1"/>
+      <c r="G190" s="1">
+        <v>39375</v>
+      </c>
       <c r="H190" s="1">
         <v>39464</v>
       </c>
       <c r="I190">
+        <f t="shared" si="13"/>
         <v>89</v>
       </c>
       <c r="K190" s="1"/>
@@ -16885,7 +17080,7 @@
     </row>
     <row r="191" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A191" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Terang2007CvWinfredN120</v>
       </c>
       <c r="B191" t="s">
@@ -16903,11 +17098,14 @@
       <c r="F191">
         <v>120</v>
       </c>
-      <c r="G191" s="1"/>
+      <c r="G191" s="1">
+        <v>39375</v>
+      </c>
       <c r="H191" s="1">
         <v>39464</v>
       </c>
       <c r="I191">
+        <f t="shared" si="13"/>
         <v>89</v>
       </c>
       <c r="K191" s="1"/>
@@ -16923,7 +17121,7 @@
     </row>
     <row r="192" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A192" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Terang2007CvWinfredN160</v>
       </c>
       <c r="B192" t="s">
@@ -16941,11 +17139,14 @@
       <c r="F192">
         <v>160</v>
       </c>
-      <c r="G192" s="1"/>
+      <c r="G192" s="1">
+        <v>39375</v>
+      </c>
       <c r="H192" s="1">
         <v>39464</v>
       </c>
       <c r="I192">
+        <f t="shared" si="13"/>
         <v>89</v>
       </c>
       <c r="K192" s="1"/>
@@ -16961,7 +17162,7 @@
     </row>
     <row r="193" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A193" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>Terang2007CvWinfredN200</v>
       </c>
       <c r="B193" t="s">
@@ -16979,11 +17180,14 @@
       <c r="F193">
         <v>200</v>
       </c>
-      <c r="G193" s="1"/>
+      <c r="G193" s="1">
+        <v>39375</v>
+      </c>
       <c r="H193" s="1">
         <v>39464</v>
       </c>
       <c r="I193">
+        <f t="shared" si="13"/>
         <v>89</v>
       </c>
       <c r="K193" s="1"/>
@@ -17017,11 +17221,14 @@
       <c r="F194">
         <v>0</v>
       </c>
-      <c r="G194" s="1"/>
+      <c r="G194" s="1">
+        <v>36477</v>
+      </c>
       <c r="H194" s="1">
         <v>36507</v>
       </c>
       <c r="I194">
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
       <c r="Q194">
@@ -17030,7 +17237,7 @@
     </row>
     <row r="195" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A195" t="str">
-        <f t="shared" ref="A195:A200" si="23">B195&amp;C195&amp;"Cv"&amp;E195&amp;"Irr"&amp;F195</f>
+        <f t="shared" ref="A195:A200" si="24">B195&amp;C195&amp;"Cv"&amp;E195&amp;"Irr"&amp;F195</f>
         <v>Elliott1999CvBonarIrr0</v>
       </c>
       <c r="B195" t="s">
@@ -17048,11 +17255,14 @@
       <c r="F195">
         <v>0</v>
       </c>
-      <c r="G195" s="1"/>
+      <c r="G195" s="1">
+        <v>36477</v>
+      </c>
       <c r="H195" s="1">
         <v>36522</v>
       </c>
       <c r="I195">
+        <f t="shared" si="13"/>
         <v>45</v>
       </c>
       <c r="Q195">
@@ -17061,7 +17271,7 @@
     </row>
     <row r="196" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A196" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Elliott1999CvBonarIrr0</v>
       </c>
       <c r="B196" t="s">
@@ -17079,11 +17289,14 @@
       <c r="F196">
         <v>0</v>
       </c>
-      <c r="G196" s="1"/>
+      <c r="G196" s="1">
+        <v>36477</v>
+      </c>
       <c r="H196" s="1">
         <v>36527</v>
       </c>
       <c r="I196">
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="Q196">
@@ -17092,7 +17305,7 @@
     </row>
     <row r="197" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A197" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Elliott1999CvBonarIrr0</v>
       </c>
       <c r="B197" t="s">
@@ -17110,11 +17323,14 @@
       <c r="F197">
         <v>0</v>
       </c>
-      <c r="G197" s="1"/>
+      <c r="G197" s="1">
+        <v>36477</v>
+      </c>
       <c r="H197" s="1">
         <v>36536</v>
       </c>
       <c r="I197">
+        <f t="shared" si="13"/>
         <v>59</v>
       </c>
       <c r="Q197">
@@ -17123,7 +17339,7 @@
     </row>
     <row r="198" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A198" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Elliott1999CvBonarIrr0</v>
       </c>
       <c r="B198" t="s">
@@ -17141,11 +17357,14 @@
       <c r="F198">
         <v>0</v>
       </c>
-      <c r="G198" s="1"/>
+      <c r="G198" s="1">
+        <v>36477</v>
+      </c>
       <c r="H198" s="1">
         <v>36546</v>
       </c>
       <c r="I198">
+        <f t="shared" si="13"/>
         <v>69</v>
       </c>
       <c r="Q198">
@@ -17154,7 +17373,7 @@
     </row>
     <row r="199" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A199" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Elliott1999CvBonarIrr0</v>
       </c>
       <c r="B199" t="s">
@@ -17172,11 +17391,14 @@
       <c r="F199">
         <v>0</v>
       </c>
-      <c r="G199" s="1"/>
+      <c r="G199" s="1">
+        <v>36477</v>
+      </c>
       <c r="H199" s="1">
         <v>36556</v>
       </c>
       <c r="I199">
+        <f t="shared" si="13"/>
         <v>79</v>
       </c>
       <c r="Q199">
@@ -17185,7 +17407,7 @@
     </row>
     <row r="200" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A200" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>Elliott1999CvBonarIrr0</v>
       </c>
       <c r="B200" t="s">
@@ -17203,11 +17425,14 @@
       <c r="F200">
         <v>0</v>
       </c>
-      <c r="G200" s="1"/>
+      <c r="G200" s="1">
+        <v>36477</v>
+      </c>
       <c r="H200" s="1">
         <v>36567</v>
       </c>
       <c r="I200">
+        <f t="shared" si="13"/>
         <v>90</v>
       </c>
       <c r="Q200">
@@ -17240,11 +17465,14 @@
       <c r="F201">
         <v>20</v>
       </c>
-      <c r="G201" s="1"/>
+      <c r="G201" s="1">
+        <v>36477</v>
+      </c>
       <c r="H201" s="1">
         <v>36507</v>
       </c>
       <c r="I201">
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
       <c r="Q201">
@@ -17253,7 +17481,7 @@
     </row>
     <row r="202" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A202" t="str">
-        <f t="shared" ref="A202:A207" si="24">B202&amp;C202&amp;"Cv"&amp;E202&amp;"Irr"&amp;F202</f>
+        <f t="shared" ref="A202:A207" si="25">B202&amp;C202&amp;"Cv"&amp;E202&amp;"Irr"&amp;F202</f>
         <v>Elliott1999CvBonarIrr20</v>
       </c>
       <c r="B202" t="s">
@@ -17271,11 +17499,14 @@
       <c r="F202">
         <v>20</v>
       </c>
-      <c r="G202" s="1"/>
+      <c r="G202" s="1">
+        <v>36477</v>
+      </c>
       <c r="H202" s="1">
         <v>36522</v>
       </c>
       <c r="I202">
+        <f t="shared" si="13"/>
         <v>45</v>
       </c>
       <c r="Q202">
@@ -17284,7 +17515,7 @@
     </row>
     <row r="203" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A203" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Elliott1999CvBonarIrr20</v>
       </c>
       <c r="B203" t="s">
@@ -17302,11 +17533,14 @@
       <c r="F203">
         <v>20</v>
       </c>
-      <c r="G203" s="1"/>
+      <c r="G203" s="1">
+        <v>36477</v>
+      </c>
       <c r="H203" s="1">
         <v>36527</v>
       </c>
       <c r="I203">
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="Q203">
@@ -17315,7 +17549,7 @@
     </row>
     <row r="204" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A204" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Elliott1999CvBonarIrr20</v>
       </c>
       <c r="B204" t="s">
@@ -17333,11 +17567,14 @@
       <c r="F204">
         <v>20</v>
       </c>
-      <c r="G204" s="1"/>
+      <c r="G204" s="1">
+        <v>36477</v>
+      </c>
       <c r="H204" s="1">
         <v>36536</v>
       </c>
       <c r="I204">
+        <f t="shared" ref="I204:I267" si="26">H204-G204</f>
         <v>59</v>
       </c>
       <c r="Q204">
@@ -17346,7 +17583,7 @@
     </row>
     <row r="205" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A205" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Elliott1999CvBonarIrr20</v>
       </c>
       <c r="B205" t="s">
@@ -17364,11 +17601,14 @@
       <c r="F205">
         <v>20</v>
       </c>
-      <c r="G205" s="1"/>
+      <c r="G205" s="1">
+        <v>36477</v>
+      </c>
       <c r="H205" s="1">
         <v>36546</v>
       </c>
       <c r="I205">
+        <f t="shared" si="26"/>
         <v>69</v>
       </c>
       <c r="Q205">
@@ -17377,7 +17617,7 @@
     </row>
     <row r="206" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A206" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Elliott1999CvBonarIrr20</v>
       </c>
       <c r="B206" t="s">
@@ -17395,11 +17635,14 @@
       <c r="F206">
         <v>20</v>
       </c>
-      <c r="G206" s="1"/>
+      <c r="G206" s="1">
+        <v>36477</v>
+      </c>
       <c r="H206" s="1">
         <v>36556</v>
       </c>
       <c r="I206">
+        <f t="shared" si="26"/>
         <v>79</v>
       </c>
       <c r="Q206">
@@ -17408,7 +17651,7 @@
     </row>
     <row r="207" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A207" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>Elliott1999CvBonarIrr20</v>
       </c>
       <c r="B207" t="s">
@@ -17426,11 +17669,14 @@
       <c r="F207">
         <v>20</v>
       </c>
-      <c r="G207" s="1"/>
+      <c r="G207" s="1">
+        <v>36477</v>
+      </c>
       <c r="H207" s="1">
         <v>36567</v>
       </c>
       <c r="I207">
+        <f t="shared" si="26"/>
         <v>90</v>
       </c>
       <c r="Q207">
@@ -17463,11 +17709,14 @@
       <c r="F208">
         <v>50</v>
       </c>
-      <c r="G208" s="1"/>
+      <c r="G208" s="1">
+        <v>36477</v>
+      </c>
       <c r="H208" s="1">
         <v>36507</v>
       </c>
       <c r="I208">
+        <f t="shared" si="26"/>
         <v>30</v>
       </c>
       <c r="Q208">
@@ -17476,7 +17725,7 @@
     </row>
     <row r="209" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A209" t="str">
-        <f t="shared" ref="A209:A214" si="25">B209&amp;C209&amp;"Cv"&amp;E209&amp;"Irr"&amp;F209</f>
+        <f t="shared" ref="A209:A214" si="27">B209&amp;C209&amp;"Cv"&amp;E209&amp;"Irr"&amp;F209</f>
         <v>Elliott1999CvBonarIrr50</v>
       </c>
       <c r="B209" t="s">
@@ -17494,11 +17743,14 @@
       <c r="F209">
         <v>50</v>
       </c>
-      <c r="G209" s="1"/>
+      <c r="G209" s="1">
+        <v>36477</v>
+      </c>
       <c r="H209" s="1">
         <v>36522</v>
       </c>
       <c r="I209">
+        <f t="shared" si="26"/>
         <v>45</v>
       </c>
       <c r="Q209">
@@ -17507,7 +17759,7 @@
     </row>
     <row r="210" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A210" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>Elliott1999CvBonarIrr50</v>
       </c>
       <c r="B210" t="s">
@@ -17525,11 +17777,14 @@
       <c r="F210">
         <v>50</v>
       </c>
-      <c r="G210" s="1"/>
+      <c r="G210" s="1">
+        <v>36477</v>
+      </c>
       <c r="H210" s="1">
         <v>36527</v>
       </c>
       <c r="I210">
+        <f t="shared" si="26"/>
         <v>50</v>
       </c>
       <c r="Q210">
@@ -17538,7 +17793,7 @@
     </row>
     <row r="211" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A211" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>Elliott1999CvBonarIrr50</v>
       </c>
       <c r="B211" t="s">
@@ -17556,11 +17811,14 @@
       <c r="F211">
         <v>50</v>
       </c>
-      <c r="G211" s="1"/>
+      <c r="G211" s="1">
+        <v>36477</v>
+      </c>
       <c r="H211" s="1">
         <v>36536</v>
       </c>
       <c r="I211">
+        <f t="shared" si="26"/>
         <v>59</v>
       </c>
       <c r="Q211">
@@ -17569,7 +17827,7 @@
     </row>
     <row r="212" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A212" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>Elliott1999CvBonarIrr50</v>
       </c>
       <c r="B212" t="s">
@@ -17587,11 +17845,14 @@
       <c r="F212">
         <v>50</v>
       </c>
-      <c r="G212" s="1"/>
+      <c r="G212" s="1">
+        <v>36477</v>
+      </c>
       <c r="H212" s="1">
         <v>36546</v>
       </c>
       <c r="I212">
+        <f t="shared" si="26"/>
         <v>69</v>
       </c>
       <c r="Q212">
@@ -17600,7 +17861,7 @@
     </row>
     <row r="213" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A213" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>Elliott1999CvBonarIrr50</v>
       </c>
       <c r="B213" t="s">
@@ -17618,11 +17879,14 @@
       <c r="F213">
         <v>50</v>
       </c>
-      <c r="G213" s="1"/>
+      <c r="G213" s="1">
+        <v>36477</v>
+      </c>
       <c r="H213" s="1">
         <v>36556</v>
       </c>
       <c r="I213">
+        <f t="shared" si="26"/>
         <v>79</v>
       </c>
       <c r="Q213">
@@ -17631,7 +17895,7 @@
     </row>
     <row r="214" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A214" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>Elliott1999CvBonarIrr50</v>
       </c>
       <c r="B214" t="s">
@@ -17649,11 +17913,14 @@
       <c r="F214">
         <v>50</v>
       </c>
-      <c r="G214" s="1"/>
+      <c r="G214" s="1">
+        <v>36477</v>
+      </c>
       <c r="H214" s="1">
         <v>36567</v>
       </c>
       <c r="I214">
+        <f t="shared" si="26"/>
         <v>90</v>
       </c>
       <c r="Q214">
@@ -17686,11 +17953,14 @@
       <c r="F215">
         <v>100</v>
       </c>
-      <c r="G215" s="1"/>
+      <c r="G215" s="1">
+        <v>36477</v>
+      </c>
       <c r="H215" s="1">
         <v>36507</v>
       </c>
       <c r="I215">
+        <f t="shared" si="26"/>
         <v>30</v>
       </c>
       <c r="Q215">
@@ -17699,7 +17969,7 @@
     </row>
     <row r="216" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A216" t="str">
-        <f t="shared" ref="A216:A222" si="26">B216&amp;C216&amp;"Cv"&amp;E216&amp;"Irr"&amp;F216</f>
+        <f t="shared" ref="A216:A222" si="28">B216&amp;C216&amp;"Cv"&amp;E216&amp;"Irr"&amp;F216</f>
         <v>Elliott1999CvBonarIrr100</v>
       </c>
       <c r="B216" t="s">
@@ -17717,11 +17987,14 @@
       <c r="F216">
         <v>100</v>
       </c>
-      <c r="G216" s="1"/>
+      <c r="G216" s="1">
+        <v>36477</v>
+      </c>
       <c r="H216" s="1">
         <v>36522</v>
       </c>
       <c r="I216">
+        <f t="shared" si="26"/>
         <v>45</v>
       </c>
       <c r="Q216">
@@ -17730,7 +18003,7 @@
     </row>
     <row r="217" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A217" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>Elliott1999CvBonarIrr100</v>
       </c>
       <c r="B217" t="s">
@@ -17748,11 +18021,14 @@
       <c r="F217">
         <v>100</v>
       </c>
-      <c r="G217" s="1"/>
+      <c r="G217" s="1">
+        <v>36477</v>
+      </c>
       <c r="H217" s="1">
         <v>36527</v>
       </c>
       <c r="I217">
+        <f t="shared" si="26"/>
         <v>50</v>
       </c>
       <c r="Q217">
@@ -17761,7 +18037,7 @@
     </row>
     <row r="218" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A218" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>Elliott1999CvBonarIrr100</v>
       </c>
       <c r="B218" t="s">
@@ -17779,11 +18055,14 @@
       <c r="F218">
         <v>100</v>
       </c>
-      <c r="G218" s="1"/>
+      <c r="G218" s="1">
+        <v>36477</v>
+      </c>
       <c r="H218" s="1">
         <v>36536</v>
       </c>
       <c r="I218">
+        <f t="shared" si="26"/>
         <v>59</v>
       </c>
       <c r="Q218">
@@ -17792,7 +18071,7 @@
     </row>
     <row r="219" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A219" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>Elliott1999CvBonarIrr100</v>
       </c>
       <c r="B219" t="s">
@@ -17810,11 +18089,14 @@
       <c r="F219">
         <v>100</v>
       </c>
-      <c r="G219" s="1"/>
+      <c r="G219" s="1">
+        <v>36477</v>
+      </c>
       <c r="H219" s="1">
         <v>36546</v>
       </c>
       <c r="I219">
+        <f t="shared" si="26"/>
         <v>69</v>
       </c>
       <c r="Q219">
@@ -17823,7 +18105,7 @@
     </row>
     <row r="220" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A220" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>Elliott1999CvBonarIrr100</v>
       </c>
       <c r="B220" t="s">
@@ -17841,11 +18123,14 @@
       <c r="F220">
         <v>100</v>
       </c>
-      <c r="G220" s="1"/>
+      <c r="G220" s="1">
+        <v>36477</v>
+      </c>
       <c r="H220" s="1">
         <v>36556</v>
       </c>
       <c r="I220">
+        <f t="shared" si="26"/>
         <v>79</v>
       </c>
       <c r="Q220">
@@ -17854,7 +18139,7 @@
     </row>
     <row r="221" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A221" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>Elliott1999CvBonarIrr100</v>
       </c>
       <c r="B221" t="s">
@@ -17872,11 +18157,14 @@
       <c r="F221">
         <v>100</v>
       </c>
-      <c r="G221" s="1"/>
+      <c r="G221" s="1">
+        <v>36477</v>
+      </c>
       <c r="H221" s="1">
         <v>36567</v>
       </c>
       <c r="I221">
+        <f t="shared" si="26"/>
         <v>90</v>
       </c>
       <c r="Q221">
@@ -17891,7 +18179,7 @@
     </row>
     <row r="222" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A222" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>Elliott2000CvBonarIrr0</v>
       </c>
       <c r="B222" t="s">
@@ -17906,11 +18194,14 @@
       <c r="F222">
         <v>0</v>
       </c>
-      <c r="G222" s="1"/>
+      <c r="G222" s="1">
+        <v>36830</v>
+      </c>
       <c r="H222" s="1">
         <v>36860</v>
       </c>
       <c r="I222">
+        <f t="shared" si="26"/>
         <v>30</v>
       </c>
       <c r="Q222">
@@ -17919,7 +18210,7 @@
     </row>
     <row r="223" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A223" t="str">
-        <f t="shared" ref="A223:A227" si="27">B223&amp;C223&amp;"Cv"&amp;E223&amp;"Irr"&amp;F223</f>
+        <f t="shared" ref="A223:A227" si="29">B223&amp;C223&amp;"Cv"&amp;E223&amp;"Irr"&amp;F223</f>
         <v>Elliott2000CvBonarIrr0</v>
       </c>
       <c r="B223" t="s">
@@ -17934,11 +18225,14 @@
       <c r="F223">
         <v>0</v>
       </c>
-      <c r="G223" s="1"/>
+      <c r="G223" s="1">
+        <v>36830</v>
+      </c>
       <c r="H223" s="1">
         <v>36878</v>
       </c>
       <c r="I223">
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="Q223">
@@ -17947,7 +18241,7 @@
     </row>
     <row r="224" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A224" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>Elliott2000CvBonarIrr0</v>
       </c>
       <c r="B224" t="s">
@@ -17962,11 +18256,14 @@
       <c r="F224">
         <v>0</v>
       </c>
-      <c r="G224" s="1"/>
+      <c r="G224" s="1">
+        <v>36830</v>
+      </c>
       <c r="H224" s="1">
         <v>36898</v>
       </c>
       <c r="I224">
+        <f t="shared" si="26"/>
         <v>68</v>
       </c>
       <c r="Q224">
@@ -17981,7 +18278,7 @@
     </row>
     <row r="225" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A225" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>Elliott2000CvBonarIrr0</v>
       </c>
       <c r="B225" t="s">
@@ -17996,11 +18293,14 @@
       <c r="F225">
         <v>0</v>
       </c>
-      <c r="G225" s="1"/>
+      <c r="G225" s="1">
+        <v>36830</v>
+      </c>
       <c r="H225" s="1">
         <v>36914</v>
       </c>
       <c r="I225">
+        <f t="shared" si="26"/>
         <v>84</v>
       </c>
       <c r="Q225">
@@ -18015,7 +18315,7 @@
     </row>
     <row r="226" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A226" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>Elliott2000CvBonarIrr0</v>
       </c>
       <c r="B226" t="s">
@@ -18030,11 +18330,14 @@
       <c r="F226">
         <v>0</v>
       </c>
-      <c r="G226" s="1"/>
+      <c r="G226" s="1">
+        <v>36830</v>
+      </c>
       <c r="H226" s="1">
         <v>36929</v>
       </c>
       <c r="I226">
+        <f t="shared" si="26"/>
         <v>99</v>
       </c>
       <c r="Q226">
@@ -18049,7 +18352,7 @@
     </row>
     <row r="227" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A227" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>Elliott2000CvBonarIrr20</v>
       </c>
       <c r="B227" t="s">
@@ -18064,11 +18367,14 @@
       <c r="F227">
         <v>20</v>
       </c>
-      <c r="G227" s="1"/>
+      <c r="G227" s="1">
+        <v>36830</v>
+      </c>
       <c r="H227" s="1">
         <v>36860</v>
       </c>
       <c r="I227">
+        <f t="shared" si="26"/>
         <v>30</v>
       </c>
       <c r="Q227">
@@ -18077,7 +18383,7 @@
     </row>
     <row r="228" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A228" t="str">
-        <f t="shared" ref="A228:A232" si="28">B228&amp;C228&amp;"Cv"&amp;E228&amp;"Irr"&amp;F228</f>
+        <f t="shared" ref="A228:A232" si="30">B228&amp;C228&amp;"Cv"&amp;E228&amp;"Irr"&amp;F228</f>
         <v>Elliott2000CvBonarIrr20</v>
       </c>
       <c r="B228" t="s">
@@ -18092,11 +18398,14 @@
       <c r="F228">
         <v>20</v>
       </c>
-      <c r="G228" s="1"/>
+      <c r="G228" s="1">
+        <v>36830</v>
+      </c>
       <c r="H228" s="1">
         <v>36878</v>
       </c>
       <c r="I228">
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="Q228">
@@ -18105,7 +18414,7 @@
     </row>
     <row r="229" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A229" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>Elliott2000CvBonarIrr20</v>
       </c>
       <c r="B229" t="s">
@@ -18120,11 +18429,14 @@
       <c r="F229">
         <v>20</v>
       </c>
-      <c r="G229" s="1"/>
+      <c r="G229" s="1">
+        <v>36830</v>
+      </c>
       <c r="H229" s="1">
         <v>36898</v>
       </c>
       <c r="I229">
+        <f t="shared" si="26"/>
         <v>68</v>
       </c>
       <c r="Q229">
@@ -18139,7 +18451,7 @@
     </row>
     <row r="230" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A230" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>Elliott2000CvBonarIrr20</v>
       </c>
       <c r="B230" t="s">
@@ -18154,11 +18466,14 @@
       <c r="F230">
         <v>20</v>
       </c>
-      <c r="G230" s="1"/>
+      <c r="G230" s="1">
+        <v>36830</v>
+      </c>
       <c r="H230" s="1">
         <v>36914</v>
       </c>
       <c r="I230">
+        <f t="shared" si="26"/>
         <v>84</v>
       </c>
       <c r="Q230">
@@ -18173,7 +18488,7 @@
     </row>
     <row r="231" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A231" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>Elliott2000CvBonarIrr20</v>
       </c>
       <c r="B231" t="s">
@@ -18188,11 +18503,14 @@
       <c r="F231">
         <v>20</v>
       </c>
-      <c r="G231" s="1"/>
+      <c r="G231" s="1">
+        <v>36830</v>
+      </c>
       <c r="H231" s="1">
         <v>36929</v>
       </c>
       <c r="I231">
+        <f t="shared" si="26"/>
         <v>99</v>
       </c>
       <c r="Q231">
@@ -18207,7 +18525,7 @@
     </row>
     <row r="232" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A232" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>Elliott2000CvBonarIrr40</v>
       </c>
       <c r="B232" t="s">
@@ -18222,11 +18540,14 @@
       <c r="F232">
         <v>40</v>
       </c>
-      <c r="G232" s="1"/>
+      <c r="G232" s="1">
+        <v>36830</v>
+      </c>
       <c r="H232" s="1">
         <v>36860</v>
       </c>
       <c r="I232">
+        <f t="shared" si="26"/>
         <v>30</v>
       </c>
       <c r="Q232">
@@ -18235,7 +18556,7 @@
     </row>
     <row r="233" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A233" t="str">
-        <f t="shared" ref="A233:A237" si="29">B233&amp;C233&amp;"Cv"&amp;E233&amp;"Irr"&amp;F233</f>
+        <f t="shared" ref="A233:A237" si="31">B233&amp;C233&amp;"Cv"&amp;E233&amp;"Irr"&amp;F233</f>
         <v>Elliott2000CvBonarIrr40</v>
       </c>
       <c r="B233" t="s">
@@ -18250,11 +18571,14 @@
       <c r="F233">
         <v>40</v>
       </c>
-      <c r="G233" s="1"/>
+      <c r="G233" s="1">
+        <v>36830</v>
+      </c>
       <c r="H233" s="1">
         <v>36878</v>
       </c>
       <c r="I233">
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="Q233">
@@ -18263,7 +18587,7 @@
     </row>
     <row r="234" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A234" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>Elliott2000CvBonarIrr40</v>
       </c>
       <c r="B234" t="s">
@@ -18278,11 +18602,14 @@
       <c r="F234">
         <v>40</v>
       </c>
-      <c r="G234" s="1"/>
+      <c r="G234" s="1">
+        <v>36830</v>
+      </c>
       <c r="H234" s="1">
         <v>36898</v>
       </c>
       <c r="I234">
+        <f t="shared" si="26"/>
         <v>68</v>
       </c>
       <c r="Q234">
@@ -18297,7 +18624,7 @@
     </row>
     <row r="235" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A235" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>Elliott2000CvBonarIrr40</v>
       </c>
       <c r="B235" t="s">
@@ -18312,11 +18639,14 @@
       <c r="F235">
         <v>40</v>
       </c>
-      <c r="G235" s="1"/>
+      <c r="G235" s="1">
+        <v>36830</v>
+      </c>
       <c r="H235" s="1">
         <v>36914</v>
       </c>
       <c r="I235">
+        <f t="shared" si="26"/>
         <v>84</v>
       </c>
       <c r="Q235">
@@ -18331,7 +18661,7 @@
     </row>
     <row r="236" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A236" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>Elliott2000CvBonarIrr40</v>
       </c>
       <c r="B236" t="s">
@@ -18346,11 +18676,14 @@
       <c r="F236">
         <v>40</v>
       </c>
-      <c r="G236" s="1"/>
+      <c r="G236" s="1">
+        <v>36830</v>
+      </c>
       <c r="H236" s="1">
         <v>36929</v>
       </c>
       <c r="I236">
+        <f t="shared" si="26"/>
         <v>99</v>
       </c>
       <c r="Q236">
@@ -18365,7 +18698,7 @@
     </row>
     <row r="237" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A237" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>Elliott2000CvBonarIrr60</v>
       </c>
       <c r="B237" t="s">
@@ -18380,11 +18713,14 @@
       <c r="F237">
         <v>60</v>
       </c>
-      <c r="G237" s="1"/>
+      <c r="G237" s="1">
+        <v>36830</v>
+      </c>
       <c r="H237" s="1">
         <v>36860</v>
       </c>
       <c r="I237">
+        <f t="shared" si="26"/>
         <v>30</v>
       </c>
       <c r="Q237">
@@ -18393,7 +18729,7 @@
     </row>
     <row r="238" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A238" t="str">
-        <f t="shared" ref="A238:A242" si="30">B238&amp;C238&amp;"Cv"&amp;E238&amp;"Irr"&amp;F238</f>
+        <f t="shared" ref="A238:A242" si="32">B238&amp;C238&amp;"Cv"&amp;E238&amp;"Irr"&amp;F238</f>
         <v>Elliott2000CvBonarIrr60</v>
       </c>
       <c r="B238" t="s">
@@ -18408,11 +18744,14 @@
       <c r="F238">
         <v>60</v>
       </c>
-      <c r="G238" s="1"/>
+      <c r="G238" s="1">
+        <v>36830</v>
+      </c>
       <c r="H238" s="1">
         <v>36878</v>
       </c>
       <c r="I238">
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="Q238">
@@ -18421,7 +18760,7 @@
     </row>
     <row r="239" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A239" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>Elliott2000CvBonarIrr60</v>
       </c>
       <c r="B239" t="s">
@@ -18436,11 +18775,14 @@
       <c r="F239">
         <v>60</v>
       </c>
-      <c r="G239" s="1"/>
+      <c r="G239" s="1">
+        <v>36830</v>
+      </c>
       <c r="H239" s="1">
         <v>36898</v>
       </c>
       <c r="I239">
+        <f t="shared" si="26"/>
         <v>68</v>
       </c>
       <c r="Q239">
@@ -18455,7 +18797,7 @@
     </row>
     <row r="240" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A240" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>Elliott2000CvBonarIrr60</v>
       </c>
       <c r="B240" t="s">
@@ -18470,11 +18812,14 @@
       <c r="F240">
         <v>60</v>
       </c>
-      <c r="G240" s="1"/>
+      <c r="G240" s="1">
+        <v>36830</v>
+      </c>
       <c r="H240" s="1">
         <v>36914</v>
       </c>
       <c r="I240">
+        <f t="shared" si="26"/>
         <v>84</v>
       </c>
       <c r="Q240">
@@ -18489,7 +18834,7 @@
     </row>
     <row r="241" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A241" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>Elliott2000CvBonarIrr60</v>
       </c>
       <c r="B241" t="s">
@@ -18504,11 +18849,14 @@
       <c r="F241">
         <v>60</v>
       </c>
-      <c r="G241" s="1"/>
+      <c r="G241" s="1">
+        <v>36830</v>
+      </c>
       <c r="H241" s="1">
         <v>36929</v>
       </c>
       <c r="I241">
+        <f t="shared" si="26"/>
         <v>99</v>
       </c>
       <c r="Q241">
@@ -18523,7 +18871,7 @@
     </row>
     <row r="242" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A242" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>Elliott2000CvBonarIrr80</v>
       </c>
       <c r="B242" t="s">
@@ -18538,11 +18886,14 @@
       <c r="F242">
         <v>80</v>
       </c>
-      <c r="G242" s="1"/>
+      <c r="G242" s="1">
+        <v>36830</v>
+      </c>
       <c r="H242" s="1">
         <v>36860</v>
       </c>
       <c r="I242">
+        <f t="shared" si="26"/>
         <v>30</v>
       </c>
       <c r="Q242">
@@ -18551,7 +18902,7 @@
     </row>
     <row r="243" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A243" t="str">
-        <f t="shared" ref="A243:A247" si="31">B243&amp;C243&amp;"Cv"&amp;E243&amp;"Irr"&amp;F243</f>
+        <f t="shared" ref="A243:A247" si="33">B243&amp;C243&amp;"Cv"&amp;E243&amp;"Irr"&amp;F243</f>
         <v>Elliott2000CvBonarIrr80</v>
       </c>
       <c r="B243" t="s">
@@ -18566,11 +18917,14 @@
       <c r="F243">
         <v>80</v>
       </c>
-      <c r="G243" s="1"/>
+      <c r="G243" s="1">
+        <v>36830</v>
+      </c>
       <c r="H243" s="1">
         <v>36878</v>
       </c>
       <c r="I243">
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="Q243">
@@ -18579,7 +18933,7 @@
     </row>
     <row r="244" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A244" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>Elliott2000CvBonarIrr80</v>
       </c>
       <c r="B244" t="s">
@@ -18594,11 +18948,14 @@
       <c r="F244">
         <v>80</v>
       </c>
-      <c r="G244" s="1"/>
+      <c r="G244" s="1">
+        <v>36830</v>
+      </c>
       <c r="H244" s="1">
         <v>36898</v>
       </c>
       <c r="I244">
+        <f t="shared" si="26"/>
         <v>68</v>
       </c>
       <c r="Q244">
@@ -18613,7 +18970,7 @@
     </row>
     <row r="245" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A245" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>Elliott2000CvBonarIrr80</v>
       </c>
       <c r="B245" t="s">
@@ -18628,11 +18985,14 @@
       <c r="F245">
         <v>80</v>
       </c>
-      <c r="G245" s="1"/>
+      <c r="G245" s="1">
+        <v>36830</v>
+      </c>
       <c r="H245" s="1">
         <v>36914</v>
       </c>
       <c r="I245">
+        <f t="shared" si="26"/>
         <v>84</v>
       </c>
       <c r="Q245">
@@ -18647,7 +19007,7 @@
     </row>
     <row r="246" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A246" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>Elliott2000CvBonarIrr80</v>
       </c>
       <c r="B246" t="s">
@@ -18662,11 +19022,14 @@
       <c r="F246">
         <v>80</v>
       </c>
-      <c r="G246" s="1"/>
+      <c r="G246" s="1">
+        <v>36830</v>
+      </c>
       <c r="H246" s="1">
         <v>36929</v>
       </c>
       <c r="I246">
+        <f t="shared" si="26"/>
         <v>99</v>
       </c>
       <c r="Q246">
@@ -18681,7 +19044,7 @@
     </row>
     <row r="247" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A247" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>Elliott2000CvBonarIrr100</v>
       </c>
       <c r="B247" t="s">
@@ -18696,11 +19059,14 @@
       <c r="F247">
         <v>100</v>
       </c>
-      <c r="G247" s="1"/>
+      <c r="G247" s="1">
+        <v>36830</v>
+      </c>
       <c r="H247" s="1">
         <v>36860</v>
       </c>
       <c r="I247">
+        <f t="shared" si="26"/>
         <v>30</v>
       </c>
       <c r="Q247">
@@ -18709,7 +19075,7 @@
     </row>
     <row r="248" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A248" t="str">
-        <f t="shared" ref="A248:A251" si="32">B248&amp;C248&amp;"Cv"&amp;E248&amp;"Irr"&amp;F248</f>
+        <f t="shared" ref="A248:A251" si="34">B248&amp;C248&amp;"Cv"&amp;E248&amp;"Irr"&amp;F248</f>
         <v>Elliott2000CvBonarIrr100</v>
       </c>
       <c r="B248" t="s">
@@ -18724,11 +19090,14 @@
       <c r="F248">
         <v>100</v>
       </c>
-      <c r="G248" s="1"/>
+      <c r="G248" s="1">
+        <v>36830</v>
+      </c>
       <c r="H248" s="1">
         <v>36878</v>
       </c>
       <c r="I248">
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="Q248">
@@ -18737,7 +19106,7 @@
     </row>
     <row r="249" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A249" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>Elliott2000CvBonarIrr100</v>
       </c>
       <c r="B249" t="s">
@@ -18752,11 +19121,14 @@
       <c r="F249">
         <v>100</v>
       </c>
-      <c r="G249" s="1"/>
+      <c r="G249" s="1">
+        <v>36830</v>
+      </c>
       <c r="H249" s="1">
         <v>36898</v>
       </c>
       <c r="I249">
+        <f t="shared" si="26"/>
         <v>68</v>
       </c>
       <c r="Q249">
@@ -18771,7 +19143,7 @@
     </row>
     <row r="250" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A250" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>Elliott2000CvBonarIrr100</v>
       </c>
       <c r="B250" t="s">
@@ -18786,11 +19158,14 @@
       <c r="F250">
         <v>100</v>
       </c>
-      <c r="G250" s="1"/>
+      <c r="G250" s="1">
+        <v>36830</v>
+      </c>
       <c r="H250" s="1">
         <v>36914</v>
       </c>
       <c r="I250">
+        <f t="shared" si="26"/>
         <v>84</v>
       </c>
       <c r="Q250">
@@ -18805,7 +19180,7 @@
     </row>
     <row r="251" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A251" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>Elliott2000CvBonarIrr100</v>
       </c>
       <c r="B251" t="s">
@@ -18820,11 +19195,14 @@
       <c r="F251">
         <v>100</v>
       </c>
-      <c r="G251" s="1"/>
+      <c r="G251" s="1">
+        <v>36830</v>
+      </c>
       <c r="H251" s="1">
         <v>36929</v>
       </c>
       <c r="I251">
+        <f t="shared" si="26"/>
         <v>99</v>
       </c>
       <c r="Q251">
@@ -18861,16 +19239,18 @@
         <v>40520</v>
       </c>
       <c r="I252">
-        <v>342</v>
-      </c>
-      <c r="J252" s="1"/>
+        <f t="shared" si="26"/>
+        <v>272</v>
+      </c>
+      <c r="J252" s="10"/>
+      <c r="K252" s="9"/>
       <c r="Q252">
         <v>1025.1059433714699</v>
       </c>
     </row>
     <row r="253" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A253" t="str">
-        <f t="shared" ref="A253:A269" si="33">B253&amp;C253&amp;"Cv"&amp;E253&amp;"TOS"&amp;F253</f>
+        <f t="shared" ref="A253:A269" si="35">B253&amp;C253&amp;"Cv"&amp;E253&amp;"TOS"&amp;F253</f>
         <v>Delegate2010CvTaurusTOS11-mar</v>
       </c>
       <c r="B253" t="s">
@@ -18892,16 +19272,18 @@
         <v>40338</v>
       </c>
       <c r="I253">
-        <v>160</v>
-      </c>
-      <c r="J253" s="1"/>
+        <f t="shared" si="26"/>
+        <v>90</v>
+      </c>
+      <c r="J253" s="10"/>
+      <c r="K253" s="9"/>
       <c r="Q253">
         <v>443</v>
       </c>
     </row>
     <row r="254" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A254" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvTaurusTOS11-mar</v>
       </c>
       <c r="B254" t="s">
@@ -18923,16 +19305,18 @@
         <v>40312</v>
       </c>
       <c r="I254">
-        <v>134</v>
-      </c>
-      <c r="J254" s="1"/>
+        <f t="shared" si="26"/>
+        <v>64</v>
+      </c>
+      <c r="J254" s="10"/>
+      <c r="K254" s="9"/>
       <c r="Q254">
         <v>224.78860335995901</v>
       </c>
     </row>
     <row r="255" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A255" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvTaurusTOS11-mar</v>
       </c>
       <c r="B255" t="s">
@@ -18954,16 +19338,18 @@
         <v>40414</v>
       </c>
       <c r="I255">
-        <v>236</v>
-      </c>
-      <c r="J255" s="1"/>
+        <f t="shared" si="26"/>
+        <v>166</v>
+      </c>
+      <c r="J255" s="10"/>
+      <c r="K255" s="9"/>
       <c r="Q255">
         <v>395.42453702863401</v>
       </c>
     </row>
     <row r="256" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A256" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvTaurusTOS14-apr</v>
       </c>
       <c r="B256" t="s">
@@ -18985,15 +19371,18 @@
         <v>40526</v>
       </c>
       <c r="I256">
-        <v>349</v>
-      </c>
+        <f t="shared" si="26"/>
+        <v>244</v>
+      </c>
+      <c r="J256" s="10"/>
+      <c r="K256" s="9"/>
       <c r="Q256">
         <v>1040.4026412220799</v>
       </c>
     </row>
     <row r="257" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A257" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvTaurusTOS14-apr</v>
       </c>
       <c r="B257" t="s">
@@ -19015,15 +19404,18 @@
         <v>40414</v>
       </c>
       <c r="I257">
-        <v>236</v>
-      </c>
+        <f t="shared" si="26"/>
+        <v>132</v>
+      </c>
+      <c r="J257" s="10"/>
+      <c r="K257" s="9"/>
       <c r="Q257">
         <v>200.93457943925199</v>
       </c>
     </row>
     <row r="258" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A258" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvCBI406TOS11-mar</v>
       </c>
       <c r="B258" t="s">
@@ -19045,15 +19437,18 @@
         <v>40338</v>
       </c>
       <c r="I258">
-        <v>160</v>
-      </c>
+        <f t="shared" si="26"/>
+        <v>90</v>
+      </c>
+      <c r="J258" s="10"/>
+      <c r="K258" s="9"/>
       <c r="Q258">
         <v>375</v>
       </c>
     </row>
     <row r="259" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A259" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvCBI406TOS11-mar</v>
       </c>
       <c r="B259" t="s">
@@ -19075,15 +19470,18 @@
         <v>40522</v>
       </c>
       <c r="I259">
-        <v>344</v>
-      </c>
+        <f t="shared" si="26"/>
+        <v>274</v>
+      </c>
+      <c r="J259" s="10"/>
+      <c r="K259" s="9"/>
       <c r="Q259">
         <v>991.00584998739998</v>
       </c>
     </row>
     <row r="260" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A260" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvCBI406TOS11-mar</v>
       </c>
       <c r="B260" t="s">
@@ -19105,15 +19503,18 @@
         <v>40312</v>
       </c>
       <c r="I260">
-        <v>134</v>
-      </c>
+        <f t="shared" si="26"/>
+        <v>64</v>
+      </c>
+      <c r="J260" s="10"/>
+      <c r="K260" s="9"/>
       <c r="Q260">
         <v>202.17732986460001</v>
       </c>
     </row>
     <row r="261" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A261" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvCBI406TOS11-mar</v>
       </c>
       <c r="B261" t="s">
@@ -19135,15 +19536,18 @@
         <v>40414</v>
       </c>
       <c r="I261">
-        <v>236</v>
-      </c>
+        <f t="shared" si="26"/>
+        <v>166</v>
+      </c>
+      <c r="J261" s="10"/>
+      <c r="K261" s="9"/>
       <c r="Q261">
         <v>444.01170424195999</v>
       </c>
     </row>
     <row r="262" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A262" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvCBI406TOS14-apr</v>
       </c>
       <c r="B262" t="s">
@@ -19165,15 +19569,18 @@
         <v>40522</v>
       </c>
       <c r="I262">
-        <v>341</v>
-      </c>
+        <f t="shared" si="26"/>
+        <v>240</v>
+      </c>
+      <c r="J262" s="10"/>
+      <c r="K262" s="9"/>
       <c r="Q262">
         <v>1054.05995461364</v>
       </c>
     </row>
     <row r="263" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A263" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvCBI406TOS14-apr</v>
       </c>
       <c r="B263" t="s">
@@ -19195,15 +19602,18 @@
         <v>40414</v>
       </c>
       <c r="I263">
-        <v>236</v>
-      </c>
+        <f t="shared" si="26"/>
+        <v>132</v>
+      </c>
+      <c r="J263" s="10"/>
+      <c r="K263" s="9"/>
       <c r="Q263">
         <v>232.50259605399802</v>
       </c>
     </row>
     <row r="264" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A264" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvWinfredTOS11-mar</v>
       </c>
       <c r="B264" t="s">
@@ -19225,15 +19635,18 @@
         <v>40338</v>
       </c>
       <c r="I264">
-        <v>160</v>
-      </c>
+        <f t="shared" si="26"/>
+        <v>90</v>
+      </c>
+      <c r="J264" s="10"/>
+      <c r="K264" s="9"/>
       <c r="Q264">
         <v>496</v>
       </c>
     </row>
     <row r="265" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A265" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvWinfredTOS11-mar</v>
       </c>
       <c r="B265" t="s">
@@ -19255,15 +19668,18 @@
         <v>40522</v>
       </c>
       <c r="I265">
-        <v>344</v>
-      </c>
+        <f t="shared" si="26"/>
+        <v>274</v>
+      </c>
+      <c r="J265" s="10"/>
+      <c r="K265" s="9"/>
       <c r="Q265">
         <v>967.91784984890091</v>
       </c>
     </row>
     <row r="266" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A266" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvWinfredTOS11-mar</v>
       </c>
       <c r="B266" t="s">
@@ -19285,15 +19701,18 @@
         <v>40312</v>
       </c>
       <c r="I266">
-        <v>134</v>
-      </c>
+        <f t="shared" si="26"/>
+        <v>64</v>
+      </c>
+      <c r="J266" s="10"/>
+      <c r="K266" s="9"/>
       <c r="Q266">
         <v>202.630568394829</v>
       </c>
     </row>
     <row r="267" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A267" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvWinfredTOS11-mar</v>
       </c>
       <c r="B267" t="s">
@@ -19315,15 +19734,18 @@
         <v>40414</v>
       </c>
       <c r="I267">
-        <v>236</v>
-      </c>
+        <f t="shared" si="26"/>
+        <v>166</v>
+      </c>
+      <c r="J267" s="10"/>
+      <c r="K267" s="9"/>
       <c r="Q267">
         <v>418.50701520510199</v>
       </c>
     </row>
     <row r="268" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A268" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvWinfredTOS14-apr</v>
       </c>
       <c r="B268" t="s">
@@ -19345,15 +19767,18 @@
         <v>40522</v>
       </c>
       <c r="I268">
-        <v>341</v>
-      </c>
+        <f t="shared" ref="I268:I274" si="36">H268-G268</f>
+        <v>240</v>
+      </c>
+      <c r="J268" s="10"/>
+      <c r="K268" s="9"/>
       <c r="Q268">
         <v>896.72706131591497</v>
       </c>
     </row>
     <row r="269" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A269" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>Delegate2010CvWinfredTOS14-apr</v>
       </c>
       <c r="B269" t="s">
@@ -19375,8 +19800,11 @@
         <v>40414</v>
       </c>
       <c r="I269">
-        <v>236</v>
-      </c>
+        <f t="shared" si="36"/>
+        <v>132</v>
+      </c>
+      <c r="J269" s="10"/>
+      <c r="K269" s="9"/>
       <c r="Q269">
         <v>276.22014537902402</v>
       </c>
@@ -19405,15 +19833,18 @@
         <v>39237</v>
       </c>
       <c r="I270">
-        <v>155</v>
-      </c>
+        <f t="shared" si="36"/>
+        <v>47</v>
+      </c>
+      <c r="J270" s="10"/>
+      <c r="K270" s="9"/>
       <c r="Q270">
         <v>201.73644533332998</v>
       </c>
     </row>
     <row r="271" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A271" t="str">
-        <f t="shared" ref="A271" si="34">B271&amp;C271&amp;"Cv"&amp;E271</f>
+        <f t="shared" ref="A271" si="37">B271&amp;C271&amp;"Cv"&amp;E271</f>
         <v>Wagga2007CvWinfred</v>
       </c>
       <c r="B271" t="s">
@@ -19435,15 +19866,18 @@
         <v>39272</v>
       </c>
       <c r="I271">
-        <v>190</v>
-      </c>
+        <f t="shared" si="36"/>
+        <v>82</v>
+      </c>
+      <c r="J271" s="10"/>
+      <c r="K271" s="9"/>
       <c r="Q271">
         <v>356.63171238215</v>
       </c>
     </row>
     <row r="272" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A272" t="str">
-        <f t="shared" ref="A272:A274" si="35">B272&amp;C272&amp;"Cv"&amp;E272</f>
+        <f t="shared" ref="A272:A274" si="38">B272&amp;C272&amp;"Cv"&amp;E272</f>
         <v>Wagga2007CvCBI406</v>
       </c>
       <c r="B272" t="s">
@@ -19465,15 +19899,18 @@
         <v>39237</v>
       </c>
       <c r="I272">
-        <v>155</v>
-      </c>
+        <f t="shared" si="36"/>
+        <v>47</v>
+      </c>
+      <c r="J272" s="10"/>
+      <c r="K272" s="9"/>
       <c r="Q272">
         <v>217.76852</v>
       </c>
     </row>
     <row r="273" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A273" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>Wagga2007CvCBI406</v>
       </c>
       <c r="B273" t="s">
@@ -19495,15 +19932,18 @@
         <v>39272</v>
       </c>
       <c r="I273">
-        <v>190</v>
-      </c>
+        <f t="shared" si="36"/>
+        <v>82</v>
+      </c>
+      <c r="J273" s="10"/>
+      <c r="K273" s="9"/>
       <c r="Q273">
         <v>487.09084000000001</v>
       </c>
     </row>
     <row r="274" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A274" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>Wagga2007CvCBI406</v>
       </c>
       <c r="B274" t="s">
@@ -19525,8 +19965,11 @@
         <v>39396</v>
       </c>
       <c r="I274">
-        <v>314</v>
-      </c>
+        <f t="shared" si="36"/>
+        <v>206</v>
+      </c>
+      <c r="J274" s="10"/>
+      <c r="K274" s="9"/>
       <c r="Q274">
         <v>890.05769999999995</v>
       </c>

</xml_diff>

<commit_message>
checking Tosari obs data and some parameter exploration
</commit_message>
<xml_diff>
--- a/Prototypes/ForageBrassica/Observed.xlsx
+++ b/Prototypes/ForageBrassica/Observed.xlsx
@@ -2,26 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\APSIMX\Prototypes\ForageBrassica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0B22D4-1985-445E-91FE-E8244F910FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AC73D6-2A1E-41CF-AA82-F17BF66C2921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19215" yWindow="1035" windowWidth="19065" windowHeight="20700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="870" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="Observed" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Observed!$A$1:$R$2243</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Observed!$A$1:$AD$282</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="6" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -831,54 +831,54 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$7:$M$21</c:f>
+              <c:f>Sheet1!$N$7:$N$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>4.3233333333333333</c:v>
+                  <c:v>42.825000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3225</c:v>
+                  <c:v>22.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.76</c:v>
+                  <c:v>42.825000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.7725</c:v>
+                  <c:v>22.05</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.6333333333333337</c:v>
+                  <c:v>47.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4675000000000002</c:v>
+                  <c:v>28.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.9</c:v>
+                  <c:v>28.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5425</c:v>
+                  <c:v>62.625</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.38</c:v>
+                  <c:v>46.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.88</c:v>
+                  <c:v>62.625</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.335</c:v>
+                  <c:v>46.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.6400000000000006</c:v>
+                  <c:v>32.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.5524999999999998</c:v>
+                  <c:v>20.324999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.4275000000000002</c:v>
+                  <c:v>32.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.68</c:v>
+                  <c:v>20.324999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -971,138 +971,138 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$J$34:$J$76</c:f>
+              <c:f>Sheet1!$K$34:$K$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="43"/>
                 <c:pt idx="0">
-                  <c:v>4.2734128856839702</c:v>
+                  <c:v>34.200282249539498</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.38593511386666</c:v>
+                  <c:v>19.877596051968602</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2074015713720101</c:v>
+                  <c:v>25.441745160320302</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.91095004022019</c:v>
+                  <c:v>26.806896168082602</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.20162893622065</c:v>
+                  <c:v>5.8450651428006797</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.44915963655935</c:v>
+                  <c:v>25.3357450797191</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.7784439334703199</c:v>
+                  <c:v>35.365518248583598</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0097414712836899</c:v>
+                  <c:v>20.784739845505399</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.8940096372478501</c:v>
+                  <c:v>23.124367074661201</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.7004576582050701</c:v>
+                  <c:v>27.1812811826737</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.60301068571549</c:v>
+                  <c:v>8.6226157729600104</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.8318485419168304</c:v>
+                  <c:v>30.378181106949899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.6459567578710699</c:v>
+                  <c:v>35.595432902350503</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.1809689235905498</c:v>
+                  <c:v>22.967894172038399</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.9900769428124101</c:v>
+                  <c:v>24.8909660547694</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.7936517312670399</c:v>
+                  <c:v>25.883123228817698</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.39104473691087</c:v>
+                  <c:v>8.0291820344447693</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.1898377099208197</c:v>
+                  <c:v>26.4959718884636</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.1645905694107608</c:v>
+                  <c:v>54.235263824976506</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.0655156887573503</c:v>
+                  <c:v>59.462333005371001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.7301918073282101</c:v>
+                  <c:v>30.111871435414098</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.5986571790632702</c:v>
+                  <c:v>54.7135574613798</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.5882933584288796</c:v>
+                  <c:v>41.494274663762901</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10.7786098294357</c:v>
+                  <c:v>66.724898664496195</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.6040515264749597</c:v>
+                  <c:v>68.630898240402104</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.87838285025913</c:v>
+                  <c:v>32.720131091511703</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6.3985198614214003</c:v>
+                  <c:v>67.091238619369307</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5.0841657364863204</c:v>
+                  <c:v>37.624548377928001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10.2328039729657</c:v>
+                  <c:v>61.822768753192804</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.44165157531648</c:v>
+                  <c:v>60.397863155138495</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.2889581482423198</c:v>
+                  <c:v>35.519334505096701</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6.1086857158512</c:v>
+                  <c:v>61.864072973923896</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.5332892314333497</c:v>
+                  <c:v>44.354304041113394</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>11.410471358379599</c:v>
+                  <c:v>66.356840684830104</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.7910150450980904</c:v>
+                  <c:v>67.7687704079067</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.6301283723671198</c:v>
+                  <c:v>31.641763865877401</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.4603953848704903</c:v>
+                  <c:v>57.596608209016097</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6.1329578285221604</c:v>
+                  <c:v>48.594440612528899</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>12.035353604108399</c:v>
+                  <c:v>69.420234648603611</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.6521133690446499</c:v>
+                  <c:v>67.581100296593291</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.2183130272042701</c:v>
+                  <c:v>33.513764334311205</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>6.7147977953260902</c:v>
+                  <c:v>61.279245342483605</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>6.1139445182990704</c:v>
+                  <c:v>46.895391224573004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3485,11 +3485,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Huth, Neil (A&amp;F, Toowoomba)" refreshedDate="44883.710494560182" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="137" xr:uid="{5D6C32E9-1FB2-4B1F-B708-473EDDD262B3}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Huth, Neil (A&amp;F, Toowoomba)" refreshedDate="44890.327044675927" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="137" xr:uid="{5D6C32E9-1FB2-4B1F-B708-473EDDD262B3}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:Z138" sheet="Observed"/>
   </cacheSource>
-  <cacheFields count="25">
+  <cacheFields count="26">
     <cacheField name="SimulationName" numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -3514,6 +3514,9 @@
         <s v="Winfred"/>
         <s v="Pallaton"/>
       </sharedItems>
+    </cacheField>
+    <cacheField name="Treat" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="SowingDate" numFmtId="14">
       <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2018-06-13T00:00:00" maxDate="2019-04-13T00:00:00"/>
@@ -3570,13 +3573,13 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="0.15000000000000024"/>
     </cacheField>
     <cacheField name="ForageBrassica.AboveGround.Wt" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="44.325000000000003" maxValue="800.4"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="44.325000000000003" maxValue="1505.425"/>
     </cacheField>
     <cacheField name="ForageBrassica.AboveGround.WtError" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="10.946041902593528" maxValue="267.49031602408837"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="10.946041902593528" maxValue="287.76144489258229"/>
     </cacheField>
     <cacheField name="ForageBrassica.AboveGroundLive.Wt" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="44.325000000000003" maxValue="650.85"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="44.325000000000003" maxValue="1123.9749999999999"/>
     </cacheField>
     <cacheField name="ForageBrassica.AboveGroundLive.WtError" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="10.946041902593528" maxValue="243.17717135180814"/>
@@ -3585,19 +3588,19 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="334.875"/>
     </cacheField>
     <cacheField name="ForageBrassica.AboveGroundDead.WtError" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="130.01156358826958"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="3170.0460958793642"/>
     </cacheField>
     <cacheField name="ForageBrassica.Leaf.Wt" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="62.625"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="663.25"/>
     </cacheField>
     <cacheField name="ForageBrassica.Leaf.WtError" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="22.126153453925664"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="221.26153453925664"/>
     </cacheField>
     <cacheField name="ForageBrassica.Stem.Wt" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="11.3"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="460.5"/>
     </cacheField>
     <cacheField name="ForageBrassica.Stem.WtError" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="3.0490435658853197"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="175.03237795714637"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -3616,6 +3619,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-21T00:00:00"/>
     <x v="0"/>
@@ -3630,7 +3634,7 @@
     <n v="13.609555466656508"/>
     <n v="63.7"/>
     <n v="13.609555466656508"/>
-    <n v="0"/>
+    <m/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -3643,6 +3647,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-09-19T00:00:00"/>
     <x v="1"/>
@@ -3657,7 +3662,7 @@
     <n v="57.942126298574848"/>
     <n v="236.65"/>
     <n v="57.942126298574848"/>
-    <n v="0"/>
+    <m/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -3670,6 +3675,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-10-17T00:00:00"/>
     <x v="2"/>
@@ -3684,12 +3690,12 @@
     <n v="130.47721065381495"/>
     <n v="478.15"/>
     <n v="118.64188411630467"/>
+    <m/>
     <n v="0"/>
-    <n v="0"/>
-    <n v="42.825000000000003"/>
-    <n v="9.788556243559789"/>
-    <n v="4.9749999999999996"/>
-    <n v="2.1468969855739859"/>
+    <n v="428.25"/>
+    <n v="97.88556243559789"/>
+    <n v="49.75"/>
+    <n v="21.468969855739857"/>
   </r>
   <r>
     <s v="Tosari2018CvGoliath"/>
@@ -3697,6 +3703,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-11-05T00:00:00"/>
     <x v="3"/>
@@ -3713,10 +3720,10 @@
     <n v="25.090286965278018"/>
     <n v="333.7"/>
     <n v="130.01156358826958"/>
-    <n v="22.05"/>
-    <n v="2.8629821282478636"/>
-    <n v="11.3"/>
-    <n v="2.3565511522844851"/>
+    <n v="220.5"/>
+    <n v="28.629821282478634"/>
+    <n v="113"/>
+    <n v="23.565511522844851"/>
   </r>
   <r>
     <s v="Tosari2018CvHTR24"/>
@@ -3724,6 +3731,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-21T00:00:00"/>
     <x v="0"/>
@@ -3738,7 +3746,7 @@
     <n v="20.109699152399074"/>
     <n v="80.099999999999994"/>
     <n v="20.109699152399074"/>
-    <n v="0"/>
+    <m/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -3751,6 +3759,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-09-19T00:00:00"/>
     <x v="1"/>
@@ -3765,7 +3774,7 @@
     <n v="13.323162787666698"/>
     <n v="257.2"/>
     <n v="13.323162787666698"/>
-    <n v="0"/>
+    <m/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -3778,6 +3787,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-10-09T00:00:00"/>
     <x v="4"/>
@@ -3792,12 +3802,12 @@
     <n v="102.88444569839831"/>
     <n v="494.77499999999998"/>
     <n v="93.520421121093477"/>
+    <m/>
     <n v="0"/>
-    <n v="0"/>
-    <n v="47.2"/>
-    <n v="8.7051708771281451"/>
-    <n v="2.2749999999999999"/>
-    <n v="0.84606934309980364"/>
+    <n v="472"/>
+    <n v="87.051708771281454"/>
+    <n v="22.75"/>
+    <n v="8.4606934309980364"/>
   </r>
   <r>
     <s v="Tosari2018CvHTR24"/>
@@ -3805,6 +3815,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-11-05T00:00:00"/>
     <x v="3"/>
@@ -3821,10 +3832,10 @@
     <n v="83.594153503699047"/>
     <n v="308.375"/>
     <n v="55.32042269060014"/>
-    <n v="28.2"/>
-    <n v="6.4482555780614037"/>
-    <n v="6.875"/>
-    <n v="2.2005681084665385"/>
+    <n v="282"/>
+    <n v="64.482555780614035"/>
+    <n v="68.75"/>
+    <n v="22.005681084665387"/>
   </r>
   <r>
     <s v="Tosari2018CvWinfred"/>
@@ -3832,6 +3843,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-21T00:00:00"/>
     <x v="0"/>
@@ -3846,7 +3858,7 @@
     <n v="17.951137382721278"/>
     <n v="103.75"/>
     <n v="17.951137382721278"/>
-    <n v="0"/>
+    <m/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -3859,6 +3871,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-09-19T00:00:00"/>
     <x v="1"/>
@@ -3873,7 +3886,7 @@
     <n v="81.123650476705421"/>
     <n v="246.7"/>
     <n v="81.123650476705421"/>
-    <n v="0"/>
+    <m/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -3886,6 +3899,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-10-17T00:00:00"/>
     <x v="2"/>
@@ -3900,12 +3914,12 @@
     <n v="267.49031602408837"/>
     <n v="355.35"/>
     <n v="243.17717135180814"/>
+    <m/>
     <n v="0"/>
-    <n v="0"/>
-    <n v="32.700000000000003"/>
-    <n v="22.126153453925664"/>
-    <n v="2.85"/>
-    <n v="2.548855952514121"/>
+    <n v="327"/>
+    <n v="221.26153453925664"/>
+    <n v="28.5"/>
+    <n v="25.488559525141209"/>
   </r>
   <r>
     <s v="Tosari2018CvWinfred"/>
@@ -3913,6 +3927,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-11-05T00:00:00"/>
     <x v="3"/>
@@ -3929,10 +3944,10 @@
     <n v="37.358666999773959"/>
     <n v="334.875"/>
     <n v="72.495994142205305"/>
-    <n v="20.324999999999999"/>
-    <n v="1.1528949070347507"/>
-    <n v="7.95"/>
-    <n v="3.0490435658853197"/>
+    <n v="203.25"/>
+    <n v="11.528949070347508"/>
+    <n v="79.5"/>
+    <n v="30.490435658853198"/>
   </r>
   <r>
     <s v="Tosari2018CvPallaton"/>
@@ -3940,6 +3955,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-21T00:00:00"/>
     <x v="0"/>
@@ -3954,8 +3970,8 @@
     <n v="10.946041902593528"/>
     <n v="44.325000000000003"/>
     <n v="10.946041902593528"/>
-    <n v="0"/>
-    <n v="0"/>
+    <m/>
+    <m/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -3967,6 +3983,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-09-19T00:00:00"/>
     <x v="1"/>
@@ -3981,8 +3998,8 @@
     <n v="43.605685791343006"/>
     <n v="179.625"/>
     <n v="43.605685791343006"/>
-    <n v="0"/>
-    <n v="0"/>
+    <m/>
+    <m/>
     <n v="0"/>
     <n v="0"/>
     <n v="0"/>
@@ -3994,6 +4011,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-10-17T00:00:00"/>
     <x v="2"/>
@@ -4008,12 +4026,12 @@
     <n v="118.24597244726775"/>
     <n v="650.85"/>
     <n v="107.5076586419157"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="62.625"/>
-    <n v="10.56736327882536"/>
-    <n v="2.4500000000000002"/>
-    <n v="0.40414518843273806"/>
+    <m/>
+    <m/>
+    <n v="626.25"/>
+    <n v="105.6736327882536"/>
+    <n v="24.5"/>
+    <n v="4.0414518843273806"/>
   </r>
   <r>
     <s v="Tosari2018CvPallaton"/>
@@ -4021,6 +4039,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-11-05T00:00:00"/>
     <x v="3"/>
@@ -4037,10 +4056,10 @@
     <n v="75.967860528866638"/>
     <n v="240.97499999999999"/>
     <n v="87.477097002586916"/>
-    <n v="46.5"/>
-    <n v="7.2120269919997755"/>
-    <n v="4.3499999999999996"/>
-    <n v="1.8734993995195193"/>
+    <n v="465"/>
+    <n v="72.120269919997753"/>
+    <n v="43.5"/>
+    <n v="18.734993995195193"/>
   </r>
   <r>
     <s v="Tosari2018CvGoliath"/>
@@ -4048,6 +4067,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-12T00:00:00"/>
     <x v="5"/>
@@ -4075,6 +4095,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-18T00:00:00"/>
     <x v="6"/>
@@ -4102,6 +4123,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-24T00:00:00"/>
     <x v="7"/>
@@ -4129,6 +4151,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-31T00:00:00"/>
     <x v="8"/>
@@ -4156,6 +4179,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-07T00:00:00"/>
     <x v="9"/>
@@ -4183,6 +4207,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-21T00:00:00"/>
     <x v="0"/>
@@ -4210,6 +4235,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-29T00:00:00"/>
     <x v="10"/>
@@ -4237,6 +4263,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-09-24T00:00:00"/>
     <x v="11"/>
@@ -4264,6 +4291,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-12T00:00:00"/>
     <x v="5"/>
@@ -4291,6 +4319,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-18T00:00:00"/>
     <x v="6"/>
@@ -4318,6 +4347,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-24T00:00:00"/>
     <x v="7"/>
@@ -4345,6 +4375,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-31T00:00:00"/>
     <x v="8"/>
@@ -4372,6 +4403,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-07T00:00:00"/>
     <x v="9"/>
@@ -4399,6 +4431,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-21T00:00:00"/>
     <x v="0"/>
@@ -4426,6 +4459,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-29T00:00:00"/>
     <x v="10"/>
@@ -4453,6 +4487,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-09-24T00:00:00"/>
     <x v="11"/>
@@ -4480,6 +4515,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-12T00:00:00"/>
     <x v="5"/>
@@ -4507,6 +4543,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-18T00:00:00"/>
     <x v="6"/>
@@ -4534,6 +4571,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-24T00:00:00"/>
     <x v="7"/>
@@ -4561,6 +4599,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-31T00:00:00"/>
     <x v="8"/>
@@ -4588,6 +4627,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-07T00:00:00"/>
     <x v="9"/>
@@ -4615,6 +4655,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-21T00:00:00"/>
     <x v="0"/>
@@ -4642,6 +4683,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-29T00:00:00"/>
     <x v="10"/>
@@ -4669,6 +4711,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-09-24T00:00:00"/>
     <x v="11"/>
@@ -4696,6 +4739,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-12T00:00:00"/>
     <x v="5"/>
@@ -4723,6 +4767,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-18T00:00:00"/>
     <x v="6"/>
@@ -4750,6 +4795,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-24T00:00:00"/>
     <x v="7"/>
@@ -4777,6 +4823,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-07-31T00:00:00"/>
     <x v="8"/>
@@ -4804,6 +4851,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-07T00:00:00"/>
     <x v="9"/>
@@ -4831,6 +4879,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-21T00:00:00"/>
     <x v="0"/>
@@ -4858,6 +4907,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-29T00:00:00"/>
     <x v="10"/>
@@ -4885,6 +4935,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-09-24T00:00:00"/>
     <x v="11"/>
@@ -4912,6 +4963,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-21T00:00:00"/>
     <x v="0"/>
@@ -4939,6 +4991,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-29T00:00:00"/>
     <x v="10"/>
@@ -4966,6 +5019,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-09-19T00:00:00"/>
     <x v="1"/>
@@ -4993,6 +5047,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-10-17T00:00:00"/>
     <x v="2"/>
@@ -5020,6 +5075,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-11-05T00:00:00"/>
     <x v="3"/>
@@ -5047,6 +5103,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-21T00:00:00"/>
     <x v="0"/>
@@ -5074,6 +5131,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-29T00:00:00"/>
     <x v="10"/>
@@ -5101,6 +5159,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-09-19T00:00:00"/>
     <x v="1"/>
@@ -5128,6 +5187,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-10-17T00:00:00"/>
     <x v="2"/>
@@ -5155,6 +5215,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-11-05T00:00:00"/>
     <x v="3"/>
@@ -5182,6 +5243,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-21T00:00:00"/>
     <x v="0"/>
@@ -5209,6 +5271,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-29T00:00:00"/>
     <x v="10"/>
@@ -5236,6 +5299,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-09-19T00:00:00"/>
     <x v="1"/>
@@ -5263,6 +5327,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-10-17T00:00:00"/>
     <x v="2"/>
@@ -5290,6 +5355,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-11-05T00:00:00"/>
     <x v="3"/>
@@ -5317,6 +5383,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-21T00:00:00"/>
     <x v="0"/>
@@ -5344,6 +5411,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-08-29T00:00:00"/>
     <x v="10"/>
@@ -5371,6 +5439,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-09-19T00:00:00"/>
     <x v="1"/>
@@ -5398,6 +5467,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-10-17T00:00:00"/>
     <x v="2"/>
@@ -5425,6 +5495,7 @@
     <x v="0"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2018-06-13T00:00:00"/>
     <d v="2018-11-05T00:00:00"/>
     <x v="3"/>
@@ -5452,6 +5523,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-08T00:00:00"/>
     <x v="12"/>
@@ -5479,6 +5551,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-16T00:00:00"/>
     <x v="13"/>
@@ -5506,6 +5579,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-22T00:00:00"/>
     <x v="14"/>
@@ -5533,6 +5607,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-30T00:00:00"/>
     <x v="8"/>
@@ -5560,6 +5635,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-06-12T00:00:00"/>
     <x v="15"/>
@@ -5587,6 +5663,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-07-03T00:00:00"/>
     <x v="16"/>
@@ -5614,12 +5691,13 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-07-31T00:00:00"/>
     <x v="17"/>
     <m/>
     <n v="17.916666666666668"/>
-    <n v="3.5021638332824323"/>
+    <n v="3.5021638332824301"/>
     <m/>
     <m/>
     <m/>
@@ -5641,6 +5719,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-08T00:00:00"/>
     <x v="12"/>
@@ -5668,6 +5747,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-16T00:00:00"/>
     <x v="13"/>
@@ -5695,6 +5775,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-22T00:00:00"/>
     <x v="14"/>
@@ -5722,6 +5803,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-30T00:00:00"/>
     <x v="8"/>
@@ -5749,6 +5831,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-06-12T00:00:00"/>
     <x v="15"/>
@@ -5776,6 +5859,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-07-03T00:00:00"/>
     <x v="16"/>
@@ -5803,6 +5887,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-07-31T00:00:00"/>
     <x v="17"/>
@@ -5830,6 +5915,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-08T00:00:00"/>
     <x v="12"/>
@@ -5857,6 +5943,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-16T00:00:00"/>
     <x v="13"/>
@@ -5884,6 +5971,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-22T00:00:00"/>
     <x v="14"/>
@@ -5911,6 +5999,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-30T00:00:00"/>
     <x v="8"/>
@@ -5938,6 +6027,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-06-12T00:00:00"/>
     <x v="15"/>
@@ -5965,6 +6055,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-07-03T00:00:00"/>
     <x v="16"/>
@@ -5992,6 +6083,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-07-31T00:00:00"/>
     <x v="17"/>
@@ -6019,6 +6111,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-08T00:00:00"/>
     <x v="12"/>
@@ -6046,6 +6139,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-16T00:00:00"/>
     <x v="13"/>
@@ -6073,6 +6167,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-22T00:00:00"/>
     <x v="14"/>
@@ -6100,6 +6195,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-30T00:00:00"/>
     <x v="8"/>
@@ -6127,6 +6223,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-06-12T00:00:00"/>
     <x v="15"/>
@@ -6154,6 +6251,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-07-03T00:00:00"/>
     <x v="16"/>
@@ -6181,6 +6279,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-07-31T00:00:00"/>
     <x v="17"/>
@@ -6208,6 +6307,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-23T00:00:00"/>
     <x v="7"/>
@@ -6235,6 +6335,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-06-12T00:00:00"/>
     <x v="15"/>
@@ -6262,6 +6363,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-08-22T00:00:00"/>
     <x v="18"/>
@@ -6289,6 +6391,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-09-03T00:00:00"/>
     <x v="19"/>
@@ -6316,6 +6419,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-09-10T00:00:00"/>
     <x v="20"/>
@@ -6343,6 +6447,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-09-24T00:00:00"/>
     <x v="21"/>
@@ -6370,6 +6475,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-23T00:00:00"/>
     <x v="7"/>
@@ -6397,6 +6503,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-06-12T00:00:00"/>
     <x v="15"/>
@@ -6424,6 +6531,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-08-22T00:00:00"/>
     <x v="18"/>
@@ -6451,6 +6559,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-09-03T00:00:00"/>
     <x v="19"/>
@@ -6478,6 +6587,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-09-10T00:00:00"/>
     <x v="20"/>
@@ -6505,6 +6615,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-09-24T00:00:00"/>
     <x v="21"/>
@@ -6532,6 +6643,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-23T00:00:00"/>
     <x v="7"/>
@@ -6559,6 +6671,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-06-12T00:00:00"/>
     <x v="15"/>
@@ -6586,6 +6699,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-08-22T00:00:00"/>
     <x v="18"/>
@@ -6613,6 +6727,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-09-03T00:00:00"/>
     <x v="19"/>
@@ -6640,6 +6755,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-09-10T00:00:00"/>
     <x v="20"/>
@@ -6667,6 +6783,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-09-24T00:00:00"/>
     <x v="21"/>
@@ -6694,6 +6811,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-05-23T00:00:00"/>
     <x v="7"/>
@@ -6721,6 +6839,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-06-12T00:00:00"/>
     <x v="15"/>
@@ -6748,6 +6867,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-06-18T00:00:00"/>
     <x v="22"/>
@@ -6775,6 +6895,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-08-22T00:00:00"/>
     <x v="18"/>
@@ -6802,6 +6923,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-09-03T00:00:00"/>
     <x v="19"/>
@@ -6829,6 +6951,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-09-10T00:00:00"/>
     <x v="20"/>
@@ -6856,6 +6979,7 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="3"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
     <d v="2019-09-24T00:00:00"/>
     <x v="21"/>
@@ -6883,26 +7007,27 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
-    <d v="2019-06-20T00:00:00"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="63.7"/>
-    <n v="13.609555466656508"/>
-    <n v="63.7"/>
-    <n v="13.609555466656508"/>
+    <d v="2019-05-22T00:00:00"/>
+    <x v="14"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="148.44999999999999"/>
+    <n v="16.808033793397726"/>
+    <n v="148.44999999999999"/>
+    <n v="16.808033793397726"/>
     <n v="0"/>
     <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <n v="139.5"/>
+    <n v="14.52583904633395"/>
+    <n v="8.75"/>
+    <n v="2.3629078131263039"/>
   </r>
   <r>
     <s v="Tosari2019CvGoliath"/>
@@ -6910,26 +7035,27 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
-    <d v="2019-07-19T00:00:00"/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="236.65"/>
-    <n v="57.942126298574848"/>
-    <n v="236.65"/>
-    <n v="57.942126298574848"/>
+    <d v="2019-06-12T00:00:00"/>
+    <x v="15"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="375"/>
+    <n v="57.336840977972734"/>
+    <n v="375"/>
+    <n v="57.336840977972734"/>
     <n v="0"/>
     <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <n v="316.25"/>
+    <n v="42.248274126485533"/>
+    <n v="59"/>
+    <n v="18.83259585576738"/>
   </r>
   <r>
     <s v="Tosari2019CvGoliath"/>
@@ -6937,26 +7063,27 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
-    <d v="2019-08-16T00:00:00"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="525.97500000000002"/>
-    <n v="130.47721065381495"/>
-    <n v="478.15"/>
-    <n v="118.64188411630467"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="42.825000000000003"/>
-    <n v="9.788556243559789"/>
-    <n v="4.9749999999999996"/>
-    <n v="2.1468969855739859"/>
+    <d v="2019-07-03T00:00:00"/>
+    <x v="16"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="759.95"/>
+    <n v="66.828611637032637"/>
+    <n v="695.72500000000002"/>
+    <n v="69.154723868535058"/>
+    <n v="64.25"/>
+    <n v="383.3062309259617"/>
+    <n v="503"/>
+    <n v="52.706735812417755"/>
+    <n v="193"/>
+    <n v="20.37972849017703"/>
   </r>
   <r>
     <s v="Tosari2019CvGoliath"/>
@@ -6964,26 +7091,83 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="0"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
-    <d v="2019-09-04T00:00:00"/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="700.52499999999998"/>
-    <n v="118.14232588986332"/>
-    <n v="333.47500000000002"/>
-    <n v="25.090286965278018"/>
-    <n v="333.7"/>
-    <n v="130.01156358826958"/>
-    <n v="22.05"/>
-    <n v="2.8629821282478636"/>
-    <n v="11.3"/>
-    <n v="2.3565511522844851"/>
+    <d v="2019-07-31T00:00:00"/>
+    <x v="17"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="963.92499999999995"/>
+    <n v="156.87397011614132"/>
+    <n v="743.5"/>
+    <n v="159.09299167468063"/>
+    <n v="220.42500000000001"/>
+    <n v="502.6492315720775"/>
+    <n v="467.25"/>
+    <n v="88.80831417534435"/>
+    <n v="276.5"/>
+    <n v="74.853189644797368"/>
+  </r>
+  <r>
+    <s v="Tosari2019CvGoliath"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Nil"/>
+    <x v="0"/>
+    <m/>
+    <d v="2019-04-12T00:00:00"/>
+    <d v="2019-09-03T00:00:00"/>
+    <x v="19"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="1350.95"/>
+    <n v="148.61275180818097"/>
+    <n v="1123.9749999999999"/>
+    <n v="106.48184117491583"/>
+    <n v="226.97499999999999"/>
+    <n v="529.04780817364065"/>
+    <n v="663.25"/>
+    <n v="58.420173456321287"/>
+    <n v="460.5"/>
+    <n v="58.551971216461482"/>
+  </r>
+  <r>
+    <s v="Tosari2019CvGoliath"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Nil"/>
+    <x v="0"/>
+    <m/>
+    <d v="2019-04-12T00:00:00"/>
+    <d v="2019-09-24T00:00:00"/>
+    <x v="21"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="1242.9749999999999"/>
+    <n v="248.78734393051428"/>
+    <n v="698.02499999999998"/>
+    <n v="171.65339835455242"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="442.25"/>
+    <n v="108.29088912123063"/>
+    <n v="255.5"/>
+    <n v="175.03237795714637"/>
   </r>
   <r>
     <s v="Tosari2019CvHTR24"/>
@@ -6991,26 +7175,27 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
-    <d v="2019-06-20T00:00:00"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="80.099999999999994"/>
-    <n v="20.109699152399074"/>
-    <n v="80.099999999999994"/>
-    <n v="20.109699152399074"/>
+    <d v="2019-05-22T00:00:00"/>
+    <x v="14"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="123.72499999999999"/>
+    <n v="34.848373945805086"/>
+    <n v="123.72499999999999"/>
+    <n v="34.848373945805086"/>
     <n v="0"/>
     <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <n v="117.25"/>
+    <n v="31.731950249971504"/>
+    <n v="6.5"/>
+    <n v="3.3166247903553998"/>
   </r>
   <r>
     <s v="Tosari2019CvHTR24"/>
@@ -7018,26 +7203,27 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
-    <d v="2019-07-19T00:00:00"/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="257.2"/>
-    <n v="13.323162787666698"/>
-    <n v="257.2"/>
-    <n v="13.323162787666698"/>
+    <d v="2019-06-12T00:00:00"/>
+    <x v="15"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="372.65"/>
+    <n v="49.790126196532853"/>
+    <n v="372.65"/>
+    <n v="49.790126196532853"/>
     <n v="0"/>
     <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <n v="328.25"/>
+    <n v="38.560558433024106"/>
+    <n v="44"/>
+    <n v="11.69045194450012"/>
   </r>
   <r>
     <s v="Tosari2019CvHTR24"/>
@@ -7045,26 +7231,27 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
-    <d v="2019-08-08T00:00:00"/>
-    <x v="4"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="544.27499999999998"/>
-    <n v="102.88444569839831"/>
-    <n v="494.77499999999998"/>
-    <n v="93.520421121093477"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="47.2"/>
-    <n v="8.7051708771281451"/>
-    <n v="2.2749999999999999"/>
-    <n v="0.84606934309980364"/>
+    <d v="2019-07-03T00:00:00"/>
+    <x v="16"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="849.22500000000002"/>
+    <n v="150.82984618436763"/>
+    <n v="800.6"/>
+    <n v="162.23986357653698"/>
+    <n v="48.625"/>
+    <n v="274.3299412507987"/>
+    <n v="661"/>
+    <n v="126.88052122633586"/>
+    <n v="140.25"/>
+    <n v="38.981833375732002"/>
   </r>
   <r>
     <s v="Tosari2019CvHTR24"/>
@@ -7072,26 +7259,83 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="1"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
-    <d v="2019-09-04T00:00:00"/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="694.35"/>
-    <n v="89.094949351801091"/>
-    <n v="350.875"/>
-    <n v="83.594153503699047"/>
-    <n v="308.375"/>
-    <n v="55.32042269060014"/>
-    <n v="28.2"/>
-    <n v="6.4482555780614037"/>
-    <n v="6.875"/>
-    <n v="2.2005681084665385"/>
+    <d v="2019-07-31T00:00:00"/>
+    <x v="17"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="1128.2249999999999"/>
+    <n v="155.62288552780404"/>
+    <n v="860.82500000000005"/>
+    <n v="123.34097386243282"/>
+    <n v="267.39999999999998"/>
+    <n v="388.37267325770148"/>
+    <n v="586.75"/>
+    <n v="52.73439737653846"/>
+    <n v="274"/>
+    <n v="74.846509604656916"/>
+  </r>
+  <r>
+    <s v="Tosari2019CvHTR24"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Nil"/>
+    <x v="1"/>
+    <m/>
+    <d v="2019-04-12T00:00:00"/>
+    <d v="2019-09-03T00:00:00"/>
+    <x v="19"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="1174.875"/>
+    <n v="144.53461811390838"/>
+    <n v="967.375"/>
+    <n v="144.8291263293863"/>
+    <n v="207.5"/>
+    <n v="250.27584781596485"/>
+    <n v="649.25"/>
+    <n v="89.749187554354307"/>
+    <n v="318.5"/>
+    <n v="74.558701705434757"/>
+  </r>
+  <r>
+    <s v="Tosari2019CvHTR24"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Nil"/>
+    <x v="1"/>
+    <m/>
+    <d v="2019-04-12T00:00:00"/>
+    <d v="2019-09-24T00:00:00"/>
+    <x v="21"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="1505.425"/>
+    <n v="287.76144489258229"/>
+    <n v="922.05"/>
+    <n v="177.68214128981373"/>
+    <n v="274.17500000000001"/>
+    <n v="3170.0460958793642"/>
+    <n v="583.25"/>
+    <n v="110.71096001149419"/>
+    <n v="338.75"/>
+    <n v="68.941400237206281"/>
   </r>
   <r>
     <s v="Tosari2019CvWinfred"/>
@@ -7099,26 +7343,27 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
-    <d v="2019-06-20T00:00:00"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="103.75"/>
-    <n v="17.951137382721278"/>
-    <n v="103.75"/>
-    <n v="17.951137382721278"/>
+    <d v="2019-05-22T00:00:00"/>
+    <x v="14"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="152.57499999999999"/>
+    <n v="37.48211795865685"/>
+    <n v="152.57499999999999"/>
+    <n v="37.48211795865685"/>
     <n v="0"/>
     <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <n v="143"/>
+    <n v="33.025242870668897"/>
+    <n v="10"/>
+    <n v="5.715476066494082"/>
   </r>
   <r>
     <s v="Tosari2019CvWinfred"/>
@@ -7126,26 +7371,27 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
-    <d v="2019-07-19T00:00:00"/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="246.7"/>
-    <n v="81.123650476705421"/>
-    <n v="246.7"/>
-    <n v="81.123650476705421"/>
+    <d v="2019-06-12T00:00:00"/>
+    <x v="15"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="385.52499999999998"/>
+    <n v="97.450786725061036"/>
+    <n v="385.52499999999998"/>
+    <n v="97.450786725061036"/>
     <n v="0"/>
     <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
+    <n v="327"/>
+    <n v="81.580226362356541"/>
+    <n v="58.75"/>
+    <n v="15.903353943953666"/>
   </r>
   <r>
     <s v="Tosari2019CvWinfred"/>
@@ -7153,26 +7399,27 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
-    <d v="2019-08-16T00:00:00"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="390.875"/>
-    <n v="267.49031602408837"/>
-    <n v="355.35"/>
-    <n v="243.17717135180814"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="32.700000000000003"/>
-    <n v="22.126153453925664"/>
-    <n v="2.85"/>
-    <n v="2.548855952514121"/>
+    <d v="2019-07-03T00:00:00"/>
+    <x v="16"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="733.4"/>
+    <n v="91.023330342647142"/>
+    <n v="623.92499999999995"/>
+    <n v="61.772559981489088"/>
+    <n v="109.47499999999999"/>
+    <n v="724.83486625115745"/>
+    <n v="452.75"/>
+    <n v="61.716421369572835"/>
+    <n v="171.25"/>
+    <n v="42.523522902036234"/>
   </r>
   <r>
     <s v="Tosari2019CvWinfred"/>
@@ -7180,142 +7427,35 @@
     <x v="1"/>
     <s v="Nil"/>
     <x v="2"/>
+    <m/>
     <d v="2019-04-12T00:00:00"/>
-    <d v="2019-09-04T00:00:00"/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="645.625"/>
-    <n v="91.004848771919839"/>
-    <n v="282.55"/>
-    <n v="37.358666999773959"/>
-    <n v="334.875"/>
-    <n v="72.495994142205305"/>
-    <n v="20.324999999999999"/>
-    <n v="1.1528949070347507"/>
-    <n v="7.95"/>
-    <n v="3.0490435658853197"/>
-  </r>
-  <r>
-    <s v="Tosari2019CvPallaton"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Nil"/>
-    <x v="3"/>
-    <d v="2019-04-12T00:00:00"/>
-    <d v="2019-06-20T00:00:00"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="44.325000000000003"/>
-    <n v="10.946041902593528"/>
-    <n v="44.325000000000003"/>
-    <n v="10.946041902593528"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <s v="Tosari2019CvPallaton"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Nil"/>
-    <x v="3"/>
-    <d v="2019-04-12T00:00:00"/>
-    <d v="2019-07-19T00:00:00"/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="179.625"/>
-    <n v="43.605685791343006"/>
-    <n v="179.625"/>
-    <n v="43.605685791343006"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <s v="Tosari2019CvPallaton"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Nil"/>
-    <x v="3"/>
-    <d v="2019-04-12T00:00:00"/>
-    <d v="2019-08-16T00:00:00"/>
-    <x v="2"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="715.95"/>
-    <n v="118.24597244726775"/>
-    <n v="650.85"/>
-    <n v="107.5076586419157"/>
-    <n v="0"/>
-    <n v="0"/>
-    <n v="62.625"/>
-    <n v="10.56736327882536"/>
-    <n v="2.4500000000000002"/>
-    <n v="0.40414518843273806"/>
-  </r>
-  <r>
-    <s v="Tosari2019CvPallaton"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Nil"/>
-    <x v="3"/>
-    <d v="2019-04-12T00:00:00"/>
-    <d v="2019-09-04T00:00:00"/>
-    <x v="3"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="800.4"/>
-    <n v="121.35801031109017"/>
-    <n v="508.57499999999999"/>
-    <n v="75.967860528866638"/>
-    <n v="240.97499999999999"/>
-    <n v="87.477097002586916"/>
-    <n v="46.5"/>
-    <n v="7.2120269919997755"/>
-    <n v="4.3499999999999996"/>
-    <n v="1.8734993995195193"/>
+    <d v="2019-07-31T00:00:00"/>
+    <x v="17"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="1028.5"/>
+    <n v="31.073568618146624"/>
+    <n v="794.22500000000002"/>
+    <n v="25.173183482957946"/>
+    <n v="234.22499999999999"/>
+    <n v="471.1088869182297"/>
+    <n v="489.5"/>
+    <n v="66.284739319595033"/>
+    <n v="305"/>
+    <n v="72.869746808946715"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E37CBB69-8253-4EBA-9B3E-56DDB7A5EE18}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A4:E34" firstHeaderRow="1" firstDataRow="2" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="25">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E37CBB69-8253-4EBA-9B3E-56DDB7A5EE18}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A4:E30" firstHeaderRow="1" firstDataRow="2" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="26">
     <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField axis="axisPage" compact="0" outline="0" showAll="0">
       <items count="2">
@@ -7338,6 +7478,7 @@
         <item h="1" x="2"/>
       </items>
     </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
     <pivotField compact="0" numFmtId="14" outline="0" showAll="0"/>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
@@ -7389,9 +7530,9 @@
   <rowFields count="3">
     <field x="4"/>
     <field x="2"/>
-    <field x="7"/>
+    <field x="8"/>
   </rowFields>
-  <rowItems count="29">
+  <rowItems count="25">
     <i>
       <x v="1"/>
       <x/>
@@ -7450,28 +7591,16 @@
       <x v="8"/>
     </i>
     <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="2">
       <x v="12"/>
     </i>
     <i r="2">
-      <x v="13"/>
-    </i>
-    <i r="2">
       <x v="15"/>
-    </i>
-    <i r="2">
-      <x v="16"/>
     </i>
     <i r="2">
       <x v="18"/>
     </i>
     <i r="2">
       <x v="19"/>
-    </i>
-    <i r="2">
-      <x v="20"/>
     </i>
     <i r="2">
       <x v="21"/>
@@ -7498,8 +7627,8 @@
     <pageField fld="1" item="0" hier="-1"/>
   </pageFields>
   <dataFields count="2">
-    <dataField name="Average of ForageBrassica.Leaf.LAI" fld="11" subtotal="average" baseField="2" baseItem="0"/>
-    <dataField name="Average of ForageBrassica.Leaf.Wt" fld="21" subtotal="average" baseField="2" baseItem="0"/>
+    <dataField name="Average of ForageBrassica.Leaf.LAI" fld="12" subtotal="average" baseField="2" baseItem="0"/>
+    <dataField name="Average of ForageBrassica.Leaf.Wt" fld="22" subtotal="average" baseField="2" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -7812,8 +7941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF77B2C-709F-457D-BEEB-E013464C345A}">
   <dimension ref="A2:AB76"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8084,7 +8213,7 @@
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3">
-        <v>47.2</v>
+        <v>472</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -8128,7 +8257,7 @@
         <v>6.1956087824351296E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.45">
       <c r="C17">
         <v>145</v>
       </c>
@@ -8136,7 +8265,7 @@
         <v>1.4675000000000002</v>
       </c>
       <c r="E17" s="3">
-        <v>28.2</v>
+        <v>282</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -8154,7 +8283,7 @@
         <v>7.1720430107526878E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>2019</v>
       </c>
@@ -8183,7 +8312,7 @@
         <v>0.14189602446483182</v>
       </c>
     </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.45">
       <c r="C19">
         <v>34</v>
       </c>
@@ -8205,12 +8334,14 @@
         <v>7.6383763837638369E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.45">
       <c r="C20">
         <v>40</v>
       </c>
       <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3">
+        <v>117.25</v>
+      </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4">
         <v>2019</v>
@@ -8229,7 +8360,7 @@
         <v>0.13539755351681956</v>
       </c>
     </row>
-    <row r="21" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.45">
       <c r="C21">
         <v>41</v>
       </c>
@@ -8253,29 +8384,31 @@
         <v>0.1810578105781058</v>
       </c>
     </row>
-    <row r="22" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.45">
       <c r="C22">
         <v>48</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.45">
       <c r="C23">
         <v>61</v>
       </c>
       <c r="D23" s="3">
         <v>5.2625000000000002</v>
       </c>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="E23" s="3">
+        <v>328.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.45">
       <c r="C24">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3">
-        <v>0</v>
+        <v>661</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="4"/>
@@ -8284,12 +8417,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.45">
       <c r="C25">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="E25" s="3">
+        <v>586.75</v>
+      </c>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
@@ -8303,14 +8438,14 @@
         <v>4.8770575499285984E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.45">
       <c r="C26">
-        <v>98</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3">
-        <v>0</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="D26" s="3">
+        <v>4.5724999999999998</v>
+      </c>
+      <c r="E26" s="3"/>
       <c r="AA26">
         <v>0.5</v>
       </c>
@@ -8319,12 +8454,16 @@
         <v>0.22119921692859512</v>
       </c>
     </row>
-    <row r="27" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.45">
       <c r="C27">
-        <v>110</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+        <v>144</v>
+      </c>
+      <c r="D27" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="E27" s="3">
+        <v>649.25</v>
+      </c>
       <c r="AA27">
         <v>1</v>
       </c>
@@ -8333,14 +8472,14 @@
         <v>0.39346934028736658</v>
       </c>
     </row>
-    <row r="28" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.45">
       <c r="C28">
-        <v>118</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3">
-        <v>47.2</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="D28" s="3">
+        <v>3.07</v>
+      </c>
+      <c r="E28" s="3"/>
       <c r="AA28">
         <v>2</v>
       </c>
@@ -8349,14 +8488,16 @@
         <v>0.63212055882855767</v>
       </c>
     </row>
-    <row r="29" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.45">
       <c r="C29">
-        <v>132</v>
+        <v>165</v>
       </c>
       <c r="D29" s="3">
-        <v>4.5724999999999998</v>
-      </c>
-      <c r="E29" s="3"/>
+        <v>4.0925000000000002</v>
+      </c>
+      <c r="E29" s="3">
+        <v>583.25</v>
+      </c>
       <c r="AA29">
         <v>3</v>
       </c>
@@ -8365,14 +8506,16 @@
         <v>0.77686983985157021</v>
       </c>
     </row>
-    <row r="30" spans="2:28" x14ac:dyDescent="0.45">
-      <c r="C30">
-        <v>144</v>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>24</v>
       </c>
       <c r="D30" s="3">
-        <v>3.9</v>
-      </c>
-      <c r="E30" s="3"/>
+        <v>3.313030303030303</v>
+      </c>
+      <c r="E30" s="3">
+        <v>367.97500000000002</v>
+      </c>
       <c r="AA30">
         <v>4</v>
       </c>
@@ -8381,14 +8524,7 @@
         <v>0.8646647167633873</v>
       </c>
     </row>
-    <row r="31" spans="2:28" x14ac:dyDescent="0.45">
-      <c r="C31">
-        <v>145</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3">
-        <v>28.2</v>
-      </c>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.45">
       <c r="AA31">
         <v>5</v>
       </c>
@@ -8397,14 +8533,7 @@
         <v>0.91791500137610116</v>
       </c>
     </row>
-    <row r="32" spans="2:28" x14ac:dyDescent="0.45">
-      <c r="C32">
-        <v>151</v>
-      </c>
-      <c r="D32" s="3">
-        <v>3.07</v>
-      </c>
-      <c r="E32" s="3"/>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.45">
       <c r="J32" t="s">
         <v>34</v>
       </c>
@@ -8416,14 +8545,7 @@
         <v>0.95021293163213605</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="C33">
-        <v>165</v>
-      </c>
-      <c r="D33" s="3">
-        <v>4.0925000000000002</v>
-      </c>
-      <c r="E33" s="3"/>
+    <row r="33" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J33" t="s">
         <v>28</v>
       </c>
@@ -8441,16 +8563,7 @@
         <v>0.96980261657768152</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="3">
-        <v>3.313030303030303</v>
-      </c>
-      <c r="E34" s="3">
-        <v>18.850000000000001</v>
-      </c>
+    <row r="34" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J34">
         <v>4.2734128856839702</v>
       </c>
@@ -8469,7 +8582,7 @@
         <v>0.98168436111126578</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="35" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J35">
         <v>2.38593511386666</v>
       </c>
@@ -8481,7 +8594,7 @@
         <v>0.12003137138056319</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="36" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J36">
         <v>4.2074015713720101</v>
       </c>
@@ -8493,7 +8606,7 @@
         <v>0.16537393739537953</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="37" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J37">
         <v>3.91095004022019</v>
       </c>
@@ -8505,7 +8618,7 @@
         <v>0.14589343039559829</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="38" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J38">
         <v>1.20162893622065</v>
       </c>
@@ -8517,7 +8630,7 @@
         <v>0.20558007598951858</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="39" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J39">
         <v>4.44915963655935</v>
       </c>
@@ -8529,7 +8642,7 @@
         <v>0.17560800452325512</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="40" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J40">
         <v>4.7784439334703199</v>
       </c>
@@ -8541,7 +8654,7 @@
         <v>0.13511590300706813</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="41" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J41">
         <v>3.0097414712836899</v>
       </c>
@@ -8553,7 +8666,7 @@
         <v>0.1448053472718607</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="42" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J42">
         <v>3.8940096372478501</v>
       </c>
@@ -8565,7 +8678,7 @@
         <v>0.16839421484165754</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="43" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J43">
         <v>3.7004576582050701</v>
       </c>
@@ -8577,7 +8690,7 @@
         <v>0.13613992781782014</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="44" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J44">
         <v>1.60301068571549</v>
       </c>
@@ -8589,7 +8702,7 @@
         <v>0.18590770224766739</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="45" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J45">
         <v>4.8318485419168304</v>
       </c>
@@ -8601,7 +8714,7 @@
         <v>0.15905654538386446</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="46" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J46">
         <v>4.6459567578710699</v>
       </c>
@@ -8613,7 +8726,7 @@
         <v>0.13052114777242335</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="47" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J47">
         <v>3.1809689235905498</v>
       </c>
@@ -8625,7 +8738,7 @@
         <v>0.13849632446770541</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="48" spans="10:28" x14ac:dyDescent="0.45">
       <c r="J48">
         <v>3.9900769428124101</v>
       </c>
@@ -8983,12 +9096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD2243"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="46305" ySplit="1875" topLeftCell="Y117" activePane="bottomLeft"/>
-      <selection activeCell="X1" sqref="X1:X1048576"/>
-      <selection pane="topRight" activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="A146" sqref="A146"/>
-      <selection pane="bottomRight" activeCell="Z139" sqref="Z139:Z181"/>
+    <sheetView topLeftCell="M9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Added York 2018 Experiment
</commit_message>
<xml_diff>
--- a/Prototypes/ForageBrassica/Observed.xlsx
+++ b/Prototypes/ForageBrassica/Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\APSIMX\Prototypes\ForageBrassica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AC73D6-2A1E-41CF-AA82-F17BF66C2921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BBFD3D-17F5-4B93-B4C4-1CAF25B96C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="870" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41250" yWindow="90" windowWidth="25380" windowHeight="20640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="50">
   <si>
     <t>SimulationName</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>CrudeProteinError</t>
+  </si>
+  <si>
+    <t>York</t>
+  </si>
+  <si>
+    <t>ME</t>
   </si>
 </sst>
 </file>
@@ -7453,7 +7459,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E37CBB69-8253-4EBA-9B3E-56DDB7A5EE18}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E37CBB69-8253-4EBA-9B3E-56DDB7A5EE18}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A4:E30" firstHeaderRow="1" firstDataRow="2" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="26">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -7941,7 +7947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF77B2C-709F-457D-BEEB-E013464C345A}">
   <dimension ref="A2:AB76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
@@ -9094,10 +9100,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD2243"/>
+  <dimension ref="A1:AE2243"/>
   <sheetViews>
-    <sheetView topLeftCell="M9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O50" sqref="O50"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="13260" ySplit="750" topLeftCell="Q277" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="AE1" sqref="AE1"/>
+      <selection pane="bottomLeft" activeCell="G283" sqref="G283:G294"/>
+      <selection pane="bottomRight" activeCell="R283" sqref="R283:R294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9126,7 +9135,7 @@
     <col min="27" max="27" width="19.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9224,8 +9233,11 @@
       <c r="AD1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="AE1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f>B2&amp;C2&amp;"Cv"&amp;E2</f>
         <v>Tosari2018CvGoliath</v>
@@ -9292,7 +9304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A17" si="0">B3&amp;C3&amp;"Cv"&amp;E3</f>
         <v>Tosari2018CvGoliath</v>
@@ -9359,7 +9371,7 @@
         <v>3.2691742076555053</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Tosari2018CvGoliath</v>
@@ -9426,7 +9438,7 @@
         <v>0.70710678118654757</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Tosari2018CvGoliath</v>
@@ -9496,7 +9508,7 @@
         <v>1.6583123951776999</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Tosari2018CvHTR24</v>
@@ -9563,7 +9575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Tosari2018CvHTR24</v>
@@ -9630,7 +9642,7 @@
         <v>3.3166247903553998</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>Tosari2018CvHTR24</v>
@@ -9697,7 +9709,7 @@
         <v>1.479019945774904</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Tosari2018CvHTR24</v>
@@ -9767,7 +9779,7 @@
         <v>1.6393596310755001</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Tosari2018CvWinfred</v>
@@ -9834,7 +9846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Tosari2018CvWinfred</v>
@@ -9901,7 +9913,7 @@
         <v>3.082207001484488</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>Tosari2018CvWinfred</v>
@@ -9968,7 +9980,7 @@
         <v>6.1846584384264904</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>Tosari2018CvWinfred</v>
@@ -10038,7 +10050,7 @@
         <v>2.4494897427831779</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>Tosari2018CvPallaton</v>
@@ -10102,7 +10114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>Tosari2018CvPallaton</v>
@@ -10166,7 +10178,7 @@
         <v>3.082207001484488</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>Tosari2018CvPallaton</v>
@@ -20384,7 +20396,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A273" t="str">
         <f t="shared" si="37"/>
         <v>Delegate2010CvWinfredTOS11-mar</v>
@@ -20417,7 +20429,7 @@
         <v>967.91784984890091</v>
       </c>
     </row>
-    <row r="274" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A274" t="str">
         <f t="shared" si="37"/>
         <v>Delegate2010CvWinfredTOS11-mar</v>
@@ -20450,7 +20462,7 @@
         <v>202.630568394829</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A275" t="str">
         <f t="shared" si="37"/>
         <v>Delegate2010CvWinfredTOS11-mar</v>
@@ -20483,7 +20495,7 @@
         <v>418.50701520510199</v>
       </c>
     </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A276" t="str">
         <f t="shared" si="37"/>
         <v>Delegate2010CvWinfredTOS14-apr</v>
@@ -20516,7 +20528,7 @@
         <v>896.72706131591497</v>
       </c>
     </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A277" t="str">
         <f t="shared" si="37"/>
         <v>Delegate2010CvWinfredTOS14-apr</v>
@@ -20549,7 +20561,7 @@
         <v>276.22014537902402</v>
       </c>
     </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A278" t="str">
         <f>B278&amp;C278&amp;"Cv"&amp;E278</f>
         <v>Wagga2007CvWinfred</v>
@@ -20582,7 +20594,7 @@
         <v>201.73644533332998</v>
       </c>
     </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A279" t="str">
         <f t="shared" ref="A279" si="39">B279&amp;C279&amp;"Cv"&amp;E279</f>
         <v>Wagga2007CvWinfred</v>
@@ -20615,9 +20627,9 @@
         <v>356.63171238215</v>
       </c>
     </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A280" t="str">
-        <f t="shared" ref="A280:A282" si="40">B280&amp;C280&amp;"Cv"&amp;E280</f>
+        <f t="shared" ref="A280:A283" si="40">B280&amp;C280&amp;"Cv"&amp;E280</f>
         <v>Wagga2007CvCBI406</v>
       </c>
       <c r="B280" t="s">
@@ -20648,7 +20660,7 @@
         <v>217.76852</v>
       </c>
     </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A281" t="str">
         <f t="shared" si="40"/>
         <v>Wagga2007CvCBI406</v>
@@ -20681,7 +20693,7 @@
         <v>487.09084000000001</v>
       </c>
     </row>
-    <row r="282" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A282" t="str">
         <f t="shared" si="40"/>
         <v>Wagga2007CvCBI406</v>
@@ -20714,91 +20726,511 @@
         <v>890.05769999999995</v>
       </c>
     </row>
-    <row r="283" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="G283" s="1"/>
-      <c r="H283" s="1"/>
-    </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="G284" s="1"/>
-      <c r="H284" s="1"/>
-    </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="G285" s="1"/>
-      <c r="H285" s="1"/>
-    </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="G286" s="1"/>
-      <c r="H286" s="1"/>
-    </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="G287" s="1"/>
-      <c r="H287" s="1"/>
-    </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="G288" s="1"/>
-      <c r="H288" s="1"/>
-    </row>
-    <row r="289" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G289" s="1"/>
-      <c r="H289" s="1"/>
-    </row>
-    <row r="290" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G290" s="1"/>
-      <c r="H290" s="1"/>
-    </row>
-    <row r="291" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G291" s="1"/>
-      <c r="H291" s="1"/>
-    </row>
-    <row r="292" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G292" s="1"/>
-      <c r="H292" s="1"/>
-    </row>
-    <row r="293" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G293" s="1"/>
-      <c r="H293" s="1"/>
-    </row>
-    <row r="294" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G294" s="1"/>
-      <c r="H294" s="1"/>
-    </row>
-    <row r="295" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A283" t="str">
+        <f t="shared" si="40"/>
+        <v>York2018CvGoliath</v>
+      </c>
+      <c r="B283" t="s">
+        <v>48</v>
+      </c>
+      <c r="C283">
+        <v>2018</v>
+      </c>
+      <c r="D283" t="s">
+        <v>9</v>
+      </c>
+      <c r="E283" t="s">
+        <v>10</v>
+      </c>
+      <c r="G283" s="1">
+        <v>43277</v>
+      </c>
+      <c r="H283" s="1">
+        <v>43341</v>
+      </c>
+      <c r="I283">
+        <v>64</v>
+      </c>
+      <c r="Q283">
+        <v>67.507384049999999</v>
+      </c>
+      <c r="S283">
+        <v>67.507384000000002</v>
+      </c>
+    </row>
+    <row r="284" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A284" t="str">
+        <f t="shared" ref="A284:A286" si="41">B284&amp;C284&amp;"Cv"&amp;E284</f>
+        <v>York2018CvGoliath</v>
+      </c>
+      <c r="B284" t="s">
+        <v>48</v>
+      </c>
+      <c r="C284">
+        <v>2018</v>
+      </c>
+      <c r="D284" t="s">
+        <v>9</v>
+      </c>
+      <c r="E284" t="s">
+        <v>10</v>
+      </c>
+      <c r="G284" s="1">
+        <v>43277</v>
+      </c>
+      <c r="H284" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I284">
+        <v>99</v>
+      </c>
+      <c r="Q284">
+        <v>251.27543449999999</v>
+      </c>
+      <c r="S284">
+        <v>251.27543399999999</v>
+      </c>
+      <c r="AA284">
+        <v>78.202500000000001</v>
+      </c>
+      <c r="AC284">
+        <v>12.140625</v>
+      </c>
+      <c r="AE284">
+        <v>11.743830000000001</v>
+      </c>
+    </row>
+    <row r="285" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A285" t="str">
+        <f t="shared" si="41"/>
+        <v>York2018CvGoliath</v>
+      </c>
+      <c r="B285" t="s">
+        <v>48</v>
+      </c>
+      <c r="C285">
+        <v>2018</v>
+      </c>
+      <c r="D285" t="s">
+        <v>9</v>
+      </c>
+      <c r="E285" t="s">
+        <v>10</v>
+      </c>
+      <c r="G285" s="1">
+        <v>43277</v>
+      </c>
+      <c r="H285" s="1">
+        <v>43411</v>
+      </c>
+      <c r="I285">
+        <v>134</v>
+      </c>
+      <c r="Q285">
+        <v>336.6839018</v>
+      </c>
+      <c r="S285">
+        <v>336.68390099999999</v>
+      </c>
+      <c r="AA285">
+        <v>75.422499999999999</v>
+      </c>
+      <c r="AC285">
+        <v>7.7265625</v>
+      </c>
+      <c r="AE285">
+        <v>11.26567</v>
+      </c>
+    </row>
+    <row r="286" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A286" t="str">
+        <f t="shared" si="41"/>
+        <v>York2018CvHTR24</v>
+      </c>
+      <c r="B286" t="s">
+        <v>48</v>
+      </c>
+      <c r="C286">
+        <v>2018</v>
+      </c>
+      <c r="D286" t="s">
+        <v>9</v>
+      </c>
+      <c r="E286" t="s">
+        <v>11</v>
+      </c>
+      <c r="G286" s="1">
+        <v>43277</v>
+      </c>
+      <c r="H286" s="1">
+        <v>43341</v>
+      </c>
+      <c r="I286">
+        <v>64</v>
+      </c>
+      <c r="Q286">
+        <v>78.506400150000005</v>
+      </c>
+      <c r="S286">
+        <v>78.506400150000005</v>
+      </c>
+    </row>
+    <row r="287" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A287" t="str">
+        <f t="shared" ref="A287:A294" si="42">B287&amp;C287&amp;"Cv"&amp;E287</f>
+        <v>York2018CvHTR24</v>
+      </c>
+      <c r="B287" t="s">
+        <v>48</v>
+      </c>
+      <c r="C287">
+        <v>2018</v>
+      </c>
+      <c r="D287" t="s">
+        <v>9</v>
+      </c>
+      <c r="E287" t="s">
+        <v>11</v>
+      </c>
+      <c r="G287" s="1">
+        <v>43277</v>
+      </c>
+      <c r="H287" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I287">
+        <v>99</v>
+      </c>
+      <c r="Q287">
+        <v>233.44817019999999</v>
+      </c>
+      <c r="S287">
+        <v>233.44817019999999</v>
+      </c>
+      <c r="AA287">
+        <v>78.405000000000001</v>
+      </c>
+      <c r="AC287">
+        <v>14.757809999999999</v>
+      </c>
+      <c r="AE287">
+        <v>11.77866</v>
+      </c>
+    </row>
+    <row r="288" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A288" t="str">
+        <f t="shared" si="42"/>
+        <v>York2018CvHTR24</v>
+      </c>
+      <c r="B288" t="s">
+        <v>48</v>
+      </c>
+      <c r="C288">
+        <v>2018</v>
+      </c>
+      <c r="D288" t="s">
+        <v>9</v>
+      </c>
+      <c r="E288" t="s">
+        <v>11</v>
+      </c>
+      <c r="G288" s="1">
+        <v>43277</v>
+      </c>
+      <c r="H288" s="1">
+        <v>43411</v>
+      </c>
+      <c r="I288">
+        <v>134</v>
+      </c>
+      <c r="Q288">
+        <v>382.78380490000001</v>
+      </c>
+      <c r="S288">
+        <v>382.78380490000001</v>
+      </c>
+      <c r="AA288">
+        <v>75.894999999999996</v>
+      </c>
+      <c r="AC288">
+        <v>9.6186710000000009</v>
+      </c>
+      <c r="AE288">
+        <v>11.34699</v>
+      </c>
+    </row>
+    <row r="289" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A289" t="str">
+        <f t="shared" si="42"/>
+        <v>York2018CvWinfred</v>
+      </c>
+      <c r="B289" t="s">
+        <v>48</v>
+      </c>
+      <c r="C289">
+        <v>2018</v>
+      </c>
+      <c r="D289" t="s">
+        <v>9</v>
+      </c>
+      <c r="E289" t="s">
+        <v>12</v>
+      </c>
+      <c r="G289" s="1">
+        <v>43277</v>
+      </c>
+      <c r="H289" s="1">
+        <v>43341</v>
+      </c>
+      <c r="I289">
+        <v>64</v>
+      </c>
+      <c r="Q289">
+        <v>72.059549000000004</v>
+      </c>
+      <c r="S289">
+        <v>72.059549000000004</v>
+      </c>
+    </row>
+    <row r="290" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A290" t="str">
+        <f t="shared" si="42"/>
+        <v>York2018CvWinfred</v>
+      </c>
+      <c r="B290" t="s">
+        <v>48</v>
+      </c>
+      <c r="C290">
+        <v>2018</v>
+      </c>
+      <c r="D290" t="s">
+        <v>9</v>
+      </c>
+      <c r="E290" t="s">
+        <v>12</v>
+      </c>
+      <c r="G290" s="1">
+        <v>43277</v>
+      </c>
+      <c r="H290" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I290">
+        <v>99</v>
+      </c>
+      <c r="Q290">
+        <v>205.31085999999999</v>
+      </c>
+      <c r="S290">
+        <v>205.31085999999999</v>
+      </c>
+      <c r="AA290">
+        <v>76.16</v>
+      </c>
+      <c r="AC290">
+        <v>13.935930000000001</v>
+      </c>
+      <c r="AE290">
+        <v>11.392519999999999</v>
+      </c>
+    </row>
+    <row r="291" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A291" t="str">
+        <f t="shared" si="42"/>
+        <v>York2018CvWinfred</v>
+      </c>
+      <c r="B291" t="s">
+        <v>48</v>
+      </c>
+      <c r="C291">
+        <v>2018</v>
+      </c>
+      <c r="D291" t="s">
+        <v>9</v>
+      </c>
+      <c r="E291" t="s">
+        <v>12</v>
+      </c>
+      <c r="G291" s="1">
+        <v>43277</v>
+      </c>
+      <c r="H291" s="1">
+        <v>43411</v>
+      </c>
+      <c r="I291">
+        <v>134</v>
+      </c>
+      <c r="Q291">
+        <v>289.57514000000003</v>
+      </c>
+      <c r="S291">
+        <v>289.57514000000003</v>
+      </c>
+      <c r="AA291">
+        <v>75.260000000000005</v>
+      </c>
+      <c r="AC291">
+        <v>7.7234369999999997</v>
+      </c>
+      <c r="AE291">
+        <v>11.237719999999999</v>
+      </c>
+    </row>
+    <row r="292" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A292" t="str">
+        <f t="shared" si="42"/>
+        <v>York2018CvPallaton</v>
+      </c>
+      <c r="B292" t="s">
+        <v>48</v>
+      </c>
+      <c r="C292">
+        <v>2018</v>
+      </c>
+      <c r="D292" t="s">
+        <v>9</v>
+      </c>
+      <c r="E292" t="s">
+        <v>13</v>
+      </c>
+      <c r="G292" s="1">
+        <v>43277</v>
+      </c>
+      <c r="H292" s="1">
+        <v>43341</v>
+      </c>
+      <c r="I292">
+        <v>64</v>
+      </c>
+      <c r="Q292">
+        <v>60.629922999999998</v>
+      </c>
+      <c r="S292">
+        <v>60.629923199999993</v>
+      </c>
+    </row>
+    <row r="293" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A293" t="str">
+        <f t="shared" si="42"/>
+        <v>York2018CvPallaton</v>
+      </c>
+      <c r="B293" t="s">
+        <v>48</v>
+      </c>
+      <c r="C293">
+        <v>2018</v>
+      </c>
+      <c r="D293" t="s">
+        <v>9</v>
+      </c>
+      <c r="E293" t="s">
+        <v>13</v>
+      </c>
+      <c r="G293" s="1">
+        <v>43277</v>
+      </c>
+      <c r="H293" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I293">
+        <v>99</v>
+      </c>
+      <c r="Q293">
+        <v>231.40583999999998</v>
+      </c>
+      <c r="S293">
+        <v>231.40584699999999</v>
+      </c>
+      <c r="AA293">
+        <v>77.725499999999997</v>
+      </c>
+      <c r="AC293">
+        <v>14.677187</v>
+      </c>
+      <c r="AE293">
+        <v>11.66178</v>
+      </c>
+    </row>
+    <row r="294" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A294" t="str">
+        <f t="shared" si="42"/>
+        <v>York2018CvPallaton</v>
+      </c>
+      <c r="B294" t="s">
+        <v>48</v>
+      </c>
+      <c r="C294">
+        <v>2018</v>
+      </c>
+      <c r="D294" t="s">
+        <v>9</v>
+      </c>
+      <c r="E294" t="s">
+        <v>13</v>
+      </c>
+      <c r="G294" s="1">
+        <v>43277</v>
+      </c>
+      <c r="H294" s="1">
+        <v>43411</v>
+      </c>
+      <c r="I294">
+        <v>134</v>
+      </c>
+      <c r="Q294">
+        <v>454.44965000000002</v>
+      </c>
+      <c r="S294">
+        <v>454.44965300000001</v>
+      </c>
+      <c r="AA294">
+        <v>78.802499999999995</v>
+      </c>
+      <c r="AC294">
+        <v>9.7109375</v>
+      </c>
+      <c r="AE294">
+        <v>11.84703</v>
+      </c>
+    </row>
+    <row r="295" spans="1:31" x14ac:dyDescent="0.45">
       <c r="G295" s="1"/>
       <c r="H295" s="1"/>
     </row>
-    <row r="296" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:31" x14ac:dyDescent="0.45">
       <c r="G296" s="1"/>
       <c r="H296" s="1"/>
     </row>
-    <row r="297" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:31" x14ac:dyDescent="0.45">
       <c r="G297" s="1"/>
       <c r="H297" s="1"/>
     </row>
-    <row r="298" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:31" x14ac:dyDescent="0.45">
       <c r="G298" s="1"/>
       <c r="H298" s="1"/>
     </row>
-    <row r="299" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:31" x14ac:dyDescent="0.45">
       <c r="G299" s="1"/>
       <c r="H299" s="1"/>
     </row>
-    <row r="300" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:31" x14ac:dyDescent="0.45">
       <c r="G300" s="1"/>
       <c r="H300" s="1"/>
     </row>
-    <row r="301" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:31" x14ac:dyDescent="0.45">
       <c r="G301" s="1"/>
       <c r="H301" s="1"/>
     </row>
-    <row r="302" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:31" x14ac:dyDescent="0.45">
       <c r="G302" s="1"/>
       <c r="H302" s="1"/>
     </row>
-    <row r="303" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:31" x14ac:dyDescent="0.45">
       <c r="G303" s="1"/>
       <c r="H303" s="1"/>
     </row>
-    <row r="304" spans="7:8" x14ac:dyDescent="0.45">
+    <row r="304" spans="1:31" x14ac:dyDescent="0.45">
       <c r="G304" s="1"/>
       <c r="H304" s="1"/>
     </row>

</xml_diff>